<commit_message>
add weight for reason
</commit_message>
<xml_diff>
--- a/excel/fupan_analysis.xlsx
+++ b/excel/fupan_analysis.xlsx
@@ -114,39 +114,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -157,13 +160,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -172,7 +175,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7569,7 +7575,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>互联网</t>
+          <t>业绩增长</t>
         </is>
       </c>
       <c r="B2" s="4" t="inlineStr">
@@ -7641,574 +7647,574 @@
     <row r="3">
       <c r="A3" s="10" t="inlineStr">
         <is>
+          <t>国企改革</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>中旗新材4</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>泰慕士4</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>连云港3</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>泰慕士4</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>国光连锁6</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>中旗新材4</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>中旗新材4</t>
+        </is>
+      </c>
+      <c r="I3" s="7" t="inlineStr">
+        <is>
+          <t>天元股份6</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="inlineStr">
+        <is>
+          <t>安记食品7</t>
+        </is>
+      </c>
+      <c r="K3" s="4" t="inlineStr">
+        <is>
+          <t>步步高6</t>
+        </is>
+      </c>
+      <c r="L3" s="9" t="inlineStr">
+        <is>
+          <t>东贝集团4</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="inlineStr">
+        <is>
+          <t>永安药业5</t>
+        </is>
+      </c>
+      <c r="N3" s="6" t="inlineStr">
+        <is>
+          <t>渝三峡A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>机器人</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>中源家居</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>新金路5</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>曙光股份3</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>双成药业5</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>立方制药5</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>国光连锁6</t>
+        </is>
+      </c>
+      <c r="H4" s="6" t="inlineStr">
+        <is>
+          <t>连云港3</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="inlineStr">
+        <is>
+          <t>步步高6</t>
+        </is>
+      </c>
+      <c r="J4" s="12" t="inlineStr">
+        <is>
+          <t>乐山电力7</t>
+        </is>
+      </c>
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>东贝集团4</t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>永安药业5</t>
+        </is>
+      </c>
+      <c r="M4" s="13" t="inlineStr">
+        <is>
+          <t>先达股份5</t>
+        </is>
+      </c>
+      <c r="N4" s="14" t="inlineStr">
+        <is>
+          <t>东珠生态6</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="15" t="inlineStr">
+        <is>
           <t>大消费</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
-        <is>
-          <t>中旗新材4</t>
-        </is>
-      </c>
-      <c r="C3" s="12" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>曙光股份3</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="inlineStr">
+        <is>
+          <t>锦江航运</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>泰慕士4</t>
         </is>
       </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>连云港3</t>
-        </is>
-      </c>
-      <c r="E3" s="12" t="inlineStr">
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>国光连锁6</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>安记食品7</t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>新金路5</t>
+        </is>
+      </c>
+      <c r="H5" s="12" t="inlineStr">
+        <is>
+          <t>乐山电力7</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="inlineStr">
+        <is>
+          <t>尤夫股份5</t>
+        </is>
+      </c>
+      <c r="J5" s="8" t="inlineStr">
+        <is>
+          <t>新金路5</t>
+        </is>
+      </c>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>生意宝4</t>
+        </is>
+      </c>
+      <c r="L5" s="13" t="inlineStr">
+        <is>
+          <t>威尔药业4</t>
+        </is>
+      </c>
+      <c r="M5" s="9" t="inlineStr">
+        <is>
+          <t>中欣氟材5</t>
+        </is>
+      </c>
+      <c r="N5" s="14" t="inlineStr">
+        <is>
+          <t>鸿博股份4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="16" t="inlineStr">
+        <is>
+          <t>互联网</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
         <is>
           <t>泰慕士4</t>
         </is>
       </c>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>两面针3</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>贝因美</t>
+        </is>
+      </c>
+      <c r="E6" s="12" t="inlineStr">
+        <is>
+          <t>乐山电力7</t>
+        </is>
+      </c>
+      <c r="F6" s="13" t="inlineStr">
+        <is>
+          <t>亚联机械5</t>
+        </is>
+      </c>
+      <c r="G6" s="12" t="inlineStr">
+        <is>
+          <t>乐山电力7</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>安记食品7</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>海联金汇4</t>
+        </is>
+      </c>
+      <c r="J6" s="6" t="inlineStr">
+        <is>
+          <t>天保基建6</t>
+        </is>
+      </c>
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>茂业商业5</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="inlineStr">
+        <is>
+          <t>茂业商业5</t>
+        </is>
+      </c>
+      <c r="M6" s="4" t="inlineStr">
+        <is>
+          <t>茂业商业5</t>
+        </is>
+      </c>
+      <c r="N6" s="5" t="inlineStr">
+        <is>
+          <t>汉商集团2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17" t="inlineStr">
+        <is>
+          <t>AI</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>远大控股2</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>双成药业5</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>双成药业5</t>
+        </is>
+      </c>
+      <c r="E7" s="8" t="inlineStr">
+        <is>
+          <t>新金路5</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>天沃科技6</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="inlineStr">
+        <is>
+          <t>立方制药5</t>
+        </is>
+      </c>
+      <c r="H7" s="6" t="inlineStr">
+        <is>
+          <t>天保基建6</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>青岛金王3</t>
+        </is>
+      </c>
+      <c r="J7" s="6" t="inlineStr">
+        <is>
+          <t>天沃科技6</t>
+        </is>
+      </c>
+      <c r="K7" s="12" t="inlineStr">
+        <is>
+          <t>宁波联合2</t>
+        </is>
+      </c>
+      <c r="L7" s="6" t="inlineStr">
+        <is>
+          <t>华银电力3</t>
+        </is>
+      </c>
+      <c r="M7" s="6" t="inlineStr">
+        <is>
+          <t>渝三峡A4</t>
+        </is>
+      </c>
+      <c r="N7" s="4" t="inlineStr">
+        <is>
+          <t>瀛通通讯3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="inlineStr">
+        <is>
+          <t>电力</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>跨境通3</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>中毅达3</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>欧亚集团</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>浔兴股份5</t>
+        </is>
+      </c>
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>红宝丽5</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>安记食品7</t>
+        </is>
+      </c>
+      <c r="H8" s="13" t="inlineStr">
+        <is>
+          <t>亚联机械5</t>
+        </is>
+      </c>
+      <c r="I8" s="13" t="inlineStr">
+        <is>
+          <t>先达股份5</t>
+        </is>
+      </c>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>双成药业5</t>
+        </is>
+      </c>
+      <c r="K8" s="6" t="inlineStr">
+        <is>
+          <t>华银电力3</t>
+        </is>
+      </c>
+      <c r="L8" s="14" t="inlineStr">
+        <is>
+          <t>鸿博股份4</t>
+        </is>
+      </c>
+      <c r="M8" s="14" t="inlineStr">
+        <is>
+          <t>鸿博股份4</t>
+        </is>
+      </c>
+      <c r="N8" s="9" t="inlineStr">
+        <is>
+          <t>全筑股份2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="inlineStr">
+        <is>
+          <t>化工</t>
+        </is>
+      </c>
+      <c r="B9" s="20" t="inlineStr">
+        <is>
+          <t>建艺集团</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
         <is>
           <t>国光连锁6</t>
         </is>
       </c>
-      <c r="G3" s="11" t="inlineStr">
-        <is>
-          <t>中旗新材4</t>
-        </is>
-      </c>
-      <c r="H3" s="11" t="inlineStr">
-        <is>
-          <t>中旗新材4</t>
-        </is>
-      </c>
-      <c r="I3" s="7" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>两面针3</t>
+        </is>
+      </c>
+      <c r="E9" s="8" t="inlineStr">
+        <is>
+          <t>立方制药5</t>
+        </is>
+      </c>
+      <c r="F9" s="13" t="inlineStr">
+        <is>
+          <t>特力A3</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="inlineStr">
+        <is>
+          <t>天保基建6</t>
+        </is>
+      </c>
+      <c r="H9" s="6" t="inlineStr">
+        <is>
+          <t>天沃科技6</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>新晨科技2</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr">
         <is>
           <t>天元股份6</t>
         </is>
       </c>
-      <c r="J3" s="4" t="inlineStr">
+      <c r="K9" s="14" t="inlineStr">
+        <is>
+          <t>东珠生态6</t>
+        </is>
+      </c>
+      <c r="L9" s="12" t="inlineStr">
+        <is>
+          <t>华电辽能2</t>
+        </is>
+      </c>
+      <c r="M9" s="14" t="inlineStr">
+        <is>
+          <t>东珠生态6</t>
+        </is>
+      </c>
+      <c r="N9" s="12" t="inlineStr">
+        <is>
+          <t>金鸿顺2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="21" t="inlineStr">
+        <is>
+          <t>多次上榜</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>南宁百货</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>天沃科技6</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>天沃科技6</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>安记食品7</t>
         </is>
       </c>
-      <c r="K3" s="4" t="inlineStr">
-        <is>
-          <t>步步高6</t>
-        </is>
-      </c>
-      <c r="L3" s="7" t="inlineStr">
-        <is>
-          <t>东贝集团4</t>
-        </is>
-      </c>
-      <c r="M3" s="12" t="inlineStr">
-        <is>
-          <t>永安药业5</t>
-        </is>
-      </c>
-      <c r="N3" s="6" t="inlineStr">
-        <is>
-          <t>渝三峡A4</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="inlineStr">
-        <is>
-          <t>国企改革</t>
-        </is>
-      </c>
-      <c r="B4" s="7" t="inlineStr">
-        <is>
-          <t>中源家居</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="inlineStr">
-        <is>
-          <t>新金路5</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>曙光股份3</t>
-        </is>
-      </c>
-      <c r="E4" s="11" t="inlineStr">
-        <is>
-          <t>双成药业5</t>
-        </is>
-      </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>立方制药5</t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="inlineStr">
-        <is>
-          <t>国光连锁6</t>
-        </is>
-      </c>
-      <c r="H4" s="6" t="inlineStr">
-        <is>
-          <t>连云港3</t>
-        </is>
-      </c>
-      <c r="I4" s="4" t="inlineStr">
-        <is>
-          <t>步步高6</t>
-        </is>
-      </c>
-      <c r="J4" s="12" t="inlineStr">
-        <is>
-          <t>乐山电力7</t>
-        </is>
-      </c>
-      <c r="K4" s="7" t="inlineStr">
-        <is>
-          <t>东贝集团4</t>
-        </is>
-      </c>
-      <c r="L4" s="12" t="inlineStr">
-        <is>
-          <t>永安药业5</t>
-        </is>
-      </c>
-      <c r="M4" s="9" t="inlineStr">
-        <is>
-          <t>先达股份5</t>
-        </is>
-      </c>
-      <c r="N4" s="12" t="inlineStr">
-        <is>
-          <t>东珠生态6</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="14" t="inlineStr">
-        <is>
-          <t>军工</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>曙光股份3</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>锦江航运</t>
-        </is>
-      </c>
-      <c r="D5" s="12" t="inlineStr">
-        <is>
-          <t>泰慕士4</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>国光连锁6</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t>安记食品7</t>
-        </is>
-      </c>
-      <c r="G5" s="8" t="inlineStr">
-        <is>
-          <t>新金路5</t>
-        </is>
-      </c>
-      <c r="H5" s="12" t="inlineStr">
-        <is>
-          <t>乐山电力7</t>
-        </is>
-      </c>
-      <c r="I5" s="6" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
+        <is>
+          <t>天保基建6</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr">
+        <is>
+          <t>保税科技4</t>
+        </is>
+      </c>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>红宝丽5</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="inlineStr">
+        <is>
+          <t>三木集团3</t>
+        </is>
+      </c>
+      <c r="J10" s="6" t="inlineStr">
         <is>
           <t>尤夫股份5</t>
         </is>
       </c>
-      <c r="J5" s="8" t="inlineStr">
-        <is>
-          <t>新金路5</t>
-        </is>
-      </c>
-      <c r="K5" s="7" t="inlineStr">
-        <is>
-          <t>生意宝4</t>
-        </is>
-      </c>
-      <c r="L5" s="9" t="inlineStr">
-        <is>
-          <t>威尔药业4</t>
-        </is>
-      </c>
-      <c r="M5" s="9" t="inlineStr">
-        <is>
-          <t>中欣氟材5</t>
-        </is>
-      </c>
-      <c r="N5" s="12" t="inlineStr">
-        <is>
-          <t>鸿博股份4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="15" t="inlineStr">
-        <is>
-          <t>半导体</t>
-        </is>
-      </c>
-      <c r="B6" s="12" t="inlineStr">
-        <is>
-          <t>泰慕士4</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr">
-        <is>
-          <t>两面针3</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
-          <t>贝因美</t>
-        </is>
-      </c>
-      <c r="E6" s="12" t="inlineStr">
-        <is>
-          <t>乐山电力7</t>
-        </is>
-      </c>
-      <c r="F6" s="9" t="inlineStr">
-        <is>
-          <t>亚联机械5</t>
-        </is>
-      </c>
-      <c r="G6" s="12" t="inlineStr">
-        <is>
-          <t>乐山电力7</t>
-        </is>
-      </c>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t>安记食品7</t>
-        </is>
-      </c>
-      <c r="I6" s="12" t="inlineStr">
-        <is>
-          <t>海联金汇4</t>
-        </is>
-      </c>
-      <c r="J6" s="6" t="inlineStr">
-        <is>
-          <t>天保基建6</t>
-        </is>
-      </c>
-      <c r="K6" s="4" t="inlineStr">
-        <is>
-          <t>茂业商业5</t>
-        </is>
-      </c>
-      <c r="L6" s="4" t="inlineStr">
-        <is>
-          <t>茂业商业5</t>
-        </is>
-      </c>
-      <c r="M6" s="4" t="inlineStr">
-        <is>
-          <t>茂业商业5</t>
-        </is>
-      </c>
-      <c r="N6" s="12" t="inlineStr">
-        <is>
-          <t>汉商集团2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="16" t="inlineStr">
-        <is>
-          <t>业绩增长</t>
-        </is>
-      </c>
-      <c r="B7" s="7" t="inlineStr">
-        <is>
-          <t>远大控股2</t>
-        </is>
-      </c>
-      <c r="C7" s="11" t="inlineStr">
-        <is>
-          <t>双成药业5</t>
-        </is>
-      </c>
-      <c r="D7" s="11" t="inlineStr">
-        <is>
-          <t>双成药业5</t>
-        </is>
-      </c>
-      <c r="E7" s="8" t="inlineStr">
-        <is>
-          <t>新金路5</t>
-        </is>
-      </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>天沃科技6</t>
-        </is>
-      </c>
-      <c r="G7" s="8" t="inlineStr">
-        <is>
-          <t>立方制药5</t>
-        </is>
-      </c>
-      <c r="H7" s="6" t="inlineStr">
-        <is>
-          <t>天保基建6</t>
-        </is>
-      </c>
-      <c r="I7" s="12" t="inlineStr">
-        <is>
-          <t>青岛金王3</t>
-        </is>
-      </c>
-      <c r="J7" s="6" t="inlineStr">
-        <is>
-          <t>天沃科技6</t>
-        </is>
-      </c>
-      <c r="K7" s="12" t="inlineStr">
-        <is>
-          <t>宁波联合2</t>
-        </is>
-      </c>
-      <c r="L7" s="6" t="inlineStr">
-        <is>
-          <t>华银电力3</t>
-        </is>
-      </c>
-      <c r="M7" s="6" t="inlineStr">
-        <is>
-          <t>渝三峡A4</t>
-        </is>
-      </c>
-      <c r="N7" s="4" t="inlineStr">
-        <is>
-          <t>瀛通通讯3</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="17" t="inlineStr">
-        <is>
-          <t>券商</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>跨境通3</t>
-        </is>
-      </c>
-      <c r="C8" s="6" t="inlineStr">
-        <is>
-          <t>中毅达3</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>欧亚集团</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr">
-        <is>
-          <t>浔兴股份5</t>
-        </is>
-      </c>
-      <c r="F8" s="8" t="inlineStr">
-        <is>
-          <t>红宝丽5</t>
-        </is>
-      </c>
-      <c r="G8" s="4" t="inlineStr">
-        <is>
-          <t>安记食品7</t>
-        </is>
-      </c>
-      <c r="H8" s="9" t="inlineStr">
-        <is>
-          <t>亚联机械5</t>
-        </is>
-      </c>
-      <c r="I8" s="9" t="inlineStr">
-        <is>
-          <t>先达股份5</t>
-        </is>
-      </c>
-      <c r="J8" s="11" t="inlineStr">
-        <is>
-          <t>双成药业5</t>
-        </is>
-      </c>
-      <c r="K8" s="6" t="inlineStr">
-        <is>
-          <t>华银电力3</t>
-        </is>
-      </c>
-      <c r="L8" s="12" t="inlineStr">
-        <is>
-          <t>鸿博股份4</t>
-        </is>
-      </c>
-      <c r="M8" s="12" t="inlineStr">
-        <is>
-          <t>鸿博股份4</t>
-        </is>
-      </c>
-      <c r="N8" s="7" t="inlineStr">
-        <is>
-          <t>全筑股份2</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="18" t="inlineStr">
-        <is>
-          <t>化工</t>
-        </is>
-      </c>
-      <c r="B9" s="19" t="inlineStr">
-        <is>
-          <t>建艺集团</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>国光连锁6</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>两面针3</t>
-        </is>
-      </c>
-      <c r="E9" s="8" t="inlineStr">
-        <is>
-          <t>立方制药5</t>
-        </is>
-      </c>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>特力A3</t>
-        </is>
-      </c>
-      <c r="G9" s="6" t="inlineStr">
-        <is>
-          <t>天保基建6</t>
-        </is>
-      </c>
-      <c r="H9" s="6" t="inlineStr">
-        <is>
-          <t>天沃科技6</t>
-        </is>
-      </c>
-      <c r="I9" s="12" t="inlineStr">
-        <is>
-          <t>新晨科技2</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr">
-        <is>
-          <t>天元股份6</t>
-        </is>
-      </c>
-      <c r="K9" s="12" t="inlineStr">
-        <is>
-          <t>东珠生态6</t>
-        </is>
-      </c>
-      <c r="L9" s="9" t="inlineStr">
-        <is>
-          <t>华电辽能2</t>
-        </is>
-      </c>
-      <c r="M9" s="12" t="inlineStr">
-        <is>
-          <t>东珠生态6</t>
-        </is>
-      </c>
-      <c r="N9" s="12" t="inlineStr">
-        <is>
-          <t>金鸿顺2</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="20" t="inlineStr">
-        <is>
-          <t>多次上榜</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>南宁百货</t>
-        </is>
-      </c>
-      <c r="C10" s="6" t="inlineStr">
-        <is>
-          <t>天沃科技6</t>
-        </is>
-      </c>
-      <c r="D10" s="6" t="inlineStr">
-        <is>
-          <t>天沃科技6</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
-        <is>
-          <t>安记食品7</t>
-        </is>
-      </c>
-      <c r="F10" s="6" t="inlineStr">
-        <is>
-          <t>天保基建6</t>
-        </is>
-      </c>
-      <c r="G10" s="6" t="inlineStr">
-        <is>
-          <t>保税科技4</t>
-        </is>
-      </c>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>红宝丽5</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr">
-        <is>
-          <t>三木集团3</t>
-        </is>
-      </c>
-      <c r="J10" s="6" t="inlineStr">
-        <is>
-          <t>尤夫股份5</t>
-        </is>
-      </c>
-      <c r="K10" s="9" t="inlineStr">
+      <c r="K10" s="13" t="inlineStr">
         <is>
           <t>金富科技2</t>
         </is>
       </c>
-      <c r="L10" s="9" t="inlineStr">
+      <c r="L10" s="14" t="inlineStr">
         <is>
           <t>中电鑫龙2</t>
         </is>
       </c>
-      <c r="M10" s="6" t="inlineStr">
+      <c r="M10" s="9" t="inlineStr">
         <is>
           <t>方正电机3</t>
         </is>
       </c>
-      <c r="N10" s="9" t="inlineStr">
+      <c r="N10" s="13" t="inlineStr">
         <is>
           <t>新坐标2</t>
         </is>
@@ -8255,7 +8261,7 @@
           <t>保税科技4</t>
         </is>
       </c>
-      <c r="I11" s="7" t="inlineStr">
+      <c r="I11" s="6" t="inlineStr">
         <is>
           <t>轻纺城2</t>
         </is>
@@ -8270,25 +8276,25 @@
           <t>西昌电力4</t>
         </is>
       </c>
-      <c r="L11" s="9" t="inlineStr">
+      <c r="L11" s="12" t="inlineStr">
         <is>
           <t>华电能源2</t>
         </is>
       </c>
-      <c r="M11" s="12" t="inlineStr">
+      <c r="M11" s="5" t="inlineStr">
         <is>
           <t>宿迁联盛2</t>
         </is>
       </c>
-      <c r="N11" s="12" t="inlineStr">
+      <c r="N11" s="5" t="inlineStr">
         <is>
           <t>大千生态5</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="21" t="n"/>
-      <c r="B12" s="11" t="inlineStr">
+      <c r="A12" s="22" t="n"/>
+      <c r="B12" s="5" t="inlineStr">
         <is>
           <t>盈方微2</t>
         </is>
@@ -8303,12 +8309,12 @@
           <t>国光连锁6</t>
         </is>
       </c>
-      <c r="E12" s="12" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>亚邦股份2</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="13" t="inlineStr">
         <is>
           <t>新宏泽2</t>
         </is>
@@ -8318,12 +8324,12 @@
           <t>尤夫股份5</t>
         </is>
       </c>
-      <c r="H12" s="7" t="inlineStr">
+      <c r="H12" s="6" t="inlineStr">
         <is>
           <t>华贸物流4</t>
         </is>
       </c>
-      <c r="I12" s="12" t="inlineStr">
+      <c r="I12" s="5" t="inlineStr">
         <is>
           <t>永安药业5</t>
         </is>
@@ -8348,19 +8354,19 @@
           <t>华阳新材2</t>
         </is>
       </c>
-      <c r="N12" s="9" t="inlineStr">
+      <c r="N12" s="13" t="inlineStr">
         <is>
           <t>金麒麟2</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="12" t="inlineStr">
+      <c r="B13" s="5" t="inlineStr">
         <is>
           <t>通达创智2</t>
         </is>
       </c>
-      <c r="C13" s="22" t="inlineStr">
+      <c r="C13" s="23" t="inlineStr">
         <is>
           <t>韶能股份4</t>
         </is>
@@ -8370,7 +8376,7 @@
           <t>立方制药5</t>
         </is>
       </c>
-      <c r="E13" s="12" t="inlineStr">
+      <c r="E13" s="5" t="inlineStr">
         <is>
           <t>荣丰控股3</t>
         </is>
@@ -8380,7 +8386,7 @@
           <t>保税科技4</t>
         </is>
       </c>
-      <c r="G13" s="12" t="inlineStr">
+      <c r="G13" s="5" t="inlineStr">
         <is>
           <t>东方材料3</t>
         </is>
@@ -8390,32 +8396,32 @@
           <t>红墙股份6</t>
         </is>
       </c>
-      <c r="I13" s="12" t="inlineStr">
+      <c r="I13" s="9" t="inlineStr">
         <is>
           <t>京城股份2</t>
         </is>
       </c>
-      <c r="J13" s="12" t="inlineStr">
+      <c r="J13" s="5" t="inlineStr">
         <is>
           <t>海联金汇4</t>
         </is>
       </c>
-      <c r="K13" s="9" t="inlineStr">
+      <c r="K13" s="8" t="inlineStr">
         <is>
           <t>海森药业2</t>
         </is>
       </c>
-      <c r="L13" s="12" t="inlineStr">
+      <c r="L13" s="9" t="inlineStr">
         <is>
           <t>天娱数科2</t>
         </is>
       </c>
-      <c r="M13" s="12" t="inlineStr">
+      <c r="M13" s="5" t="inlineStr">
         <is>
           <t>塞力医疗2</t>
         </is>
       </c>
-      <c r="N13" s="23" t="inlineStr">
+      <c r="N13" s="24" t="inlineStr">
         <is>
           <t>宁波东力3</t>
         </is>
@@ -8432,12 +8438,12 @@
           <t>迪生力3</t>
         </is>
       </c>
-      <c r="D14" s="7" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>华贸物流4</t>
         </is>
       </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="E14" s="13" t="inlineStr">
         <is>
           <t>亚联机械5</t>
         </is>
@@ -8447,7 +8453,7 @@
           <t>红墙股份6</t>
         </is>
       </c>
-      <c r="G14" s="12" t="inlineStr">
+      <c r="G14" s="5" t="inlineStr">
         <is>
           <t>武汉凡谷2</t>
         </is>
@@ -8457,39 +8463,39 @@
           <t>步步高6</t>
         </is>
       </c>
-      <c r="I14" s="12" t="inlineStr">
+      <c r="I14" s="5" t="inlineStr">
         <is>
           <t>圣龙股份2</t>
         </is>
       </c>
-      <c r="J14" s="9" t="inlineStr">
+      <c r="J14" s="13" t="inlineStr">
         <is>
           <t>先达股份5</t>
         </is>
       </c>
-      <c r="K14" s="23" t="inlineStr">
+      <c r="K14" s="25" t="inlineStr">
         <is>
           <t>卫星化学2</t>
         </is>
       </c>
-      <c r="L14" s="12" t="inlineStr">
+      <c r="L14" s="5" t="inlineStr">
         <is>
           <t>上海物贸2</t>
         </is>
       </c>
-      <c r="M14" s="23" t="inlineStr">
+      <c r="M14" s="26" t="inlineStr">
         <is>
           <t>会稽山2</t>
         </is>
       </c>
-      <c r="N14" s="9" t="inlineStr">
+      <c r="N14" s="14" t="inlineStr">
         <is>
           <t>兴民智通</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="12" t="inlineStr">
+      <c r="B15" s="5" t="inlineStr">
         <is>
           <t>亚邦股份2</t>
         </is>
@@ -8504,12 +8510,12 @@
           <t>浔兴股份5</t>
         </is>
       </c>
-      <c r="E15" s="12" t="inlineStr">
+      <c r="E15" s="5" t="inlineStr">
         <is>
           <t>通达创智2</t>
         </is>
       </c>
-      <c r="F15" s="12" t="inlineStr">
+      <c r="F15" s="5" t="inlineStr">
         <is>
           <t>中铝国际2</t>
         </is>
@@ -8524,22 +8530,22 @@
           <t>天元股份6</t>
         </is>
       </c>
-      <c r="I15" s="12" t="inlineStr">
+      <c r="I15" s="9" t="inlineStr">
         <is>
           <t>浙江荣泰3</t>
         </is>
       </c>
-      <c r="J15" s="5" t="inlineStr">
+      <c r="J15" s="14" t="inlineStr">
         <is>
           <t>润贝航科5</t>
         </is>
       </c>
-      <c r="K15" s="19" t="inlineStr">
+      <c r="K15" s="20" t="inlineStr">
         <is>
           <t>南国置业</t>
         </is>
       </c>
-      <c r="L15" s="9" t="inlineStr">
+      <c r="L15" s="13" t="inlineStr">
         <is>
           <t>珀莱雅2</t>
         </is>
@@ -8549,19 +8555,19 @@
           <t>柳钢股份</t>
         </is>
       </c>
-      <c r="N15" s="19" t="inlineStr">
+      <c r="N15" s="9" t="inlineStr">
         <is>
           <t>电光科技</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="6" t="inlineStr">
+      <c r="B16" s="8" t="inlineStr">
         <is>
           <t>中毅达3</t>
         </is>
       </c>
-      <c r="C16" s="9" t="inlineStr">
+      <c r="C16" s="13" t="inlineStr">
         <is>
           <t>有研新材</t>
         </is>
@@ -8576,7 +8582,7 @@
           <t>麦趣尔3</t>
         </is>
       </c>
-      <c r="F16" s="12" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>渝开发3</t>
         </is>
@@ -8591,17 +8597,17 @@
           <t>百大集团3</t>
         </is>
       </c>
-      <c r="I16" s="23" t="inlineStr">
+      <c r="I16" s="24" t="inlineStr">
         <is>
           <t>中欣氟材5</t>
         </is>
       </c>
-      <c r="J16" s="7" t="inlineStr">
+      <c r="J16" s="6" t="inlineStr">
         <is>
           <t>三木集团3</t>
         </is>
       </c>
-      <c r="K16" s="9" t="inlineStr">
+      <c r="K16" s="13" t="inlineStr">
         <is>
           <t>惠而浦</t>
         </is>
@@ -8611,34 +8617,34 @@
           <t>亚太实业3</t>
         </is>
       </c>
-      <c r="M16" s="9" t="inlineStr">
+      <c r="M16" s="13" t="inlineStr">
         <is>
           <t>得润电子</t>
         </is>
       </c>
-      <c r="N16" s="19" t="inlineStr">
+      <c r="N16" s="14" t="inlineStr">
         <is>
           <t>美克家居</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="19" t="inlineStr">
+      <c r="B17" s="14" t="inlineStr">
         <is>
           <t>英派斯</t>
         </is>
       </c>
-      <c r="C17" s="19" t="inlineStr">
+      <c r="C17" s="9" t="inlineStr">
         <is>
           <t>北自科技</t>
         </is>
       </c>
-      <c r="D17" s="12" t="inlineStr">
+      <c r="D17" s="5" t="inlineStr">
         <is>
           <t>东方材料3</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="E17" s="6" t="inlineStr">
         <is>
           <t>华贸物流4</t>
         </is>
@@ -8653,12 +8659,12 @@
           <t>百大集团3</t>
         </is>
       </c>
-      <c r="H17" s="5" t="inlineStr">
+      <c r="H17" s="14" t="inlineStr">
         <is>
           <t>润贝航科5</t>
         </is>
       </c>
-      <c r="I17" s="9" t="inlineStr">
+      <c r="I17" s="13" t="inlineStr">
         <is>
           <t>浙江世宝</t>
         </is>
@@ -8668,29 +8674,29 @@
           <t>中欣氟材5</t>
         </is>
       </c>
-      <c r="K17" s="9" t="inlineStr">
+      <c r="K17" s="14" t="inlineStr">
         <is>
           <t>中电鑫龙2</t>
         </is>
       </c>
-      <c r="L17" s="24" t="inlineStr">
+      <c r="L17" s="27" t="inlineStr">
         <is>
           <t>渝三峡A4</t>
         </is>
       </c>
-      <c r="M17" s="9" t="inlineStr">
+      <c r="M17" s="13" t="inlineStr">
         <is>
           <t>今创集团</t>
         </is>
       </c>
-      <c r="N17" s="5" t="inlineStr">
+      <c r="N17" s="9" t="inlineStr">
         <is>
           <t>中超控股2</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="11" t="inlineStr">
+      <c r="B18" s="5" t="inlineStr">
         <is>
           <t>双成药业5</t>
         </is>
@@ -8705,42 +8711,42 @@
           <t>麦趣尔3</t>
         </is>
       </c>
-      <c r="E18" s="12" t="inlineStr">
+      <c r="E18" s="5" t="inlineStr">
         <is>
           <t>盛泰集团2</t>
         </is>
       </c>
-      <c r="F18" s="12" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>宏昌电子2</t>
         </is>
       </c>
-      <c r="G18" s="5" t="inlineStr">
+      <c r="G18" s="14" t="inlineStr">
         <is>
           <t>润贝航科5</t>
         </is>
       </c>
-      <c r="H18" s="9" t="inlineStr">
+      <c r="H18" s="13" t="inlineStr">
         <is>
           <t>威尔药业4</t>
         </is>
       </c>
-      <c r="I18" s="9" t="inlineStr">
+      <c r="I18" s="8" t="inlineStr">
         <is>
           <t>海森药业2</t>
         </is>
       </c>
-      <c r="J18" s="12" t="inlineStr">
+      <c r="J18" s="5" t="inlineStr">
         <is>
           <t>永安药业5</t>
         </is>
       </c>
-      <c r="K18" s="12" t="inlineStr">
+      <c r="K18" s="14" t="inlineStr">
         <is>
           <t>鸿博股份4</t>
         </is>
       </c>
-      <c r="L18" s="12" t="inlineStr">
+      <c r="L18" s="5" t="inlineStr">
         <is>
           <t>绿康生化2</t>
         </is>
@@ -8750,7 +8756,7 @@
           <t>天奇股份</t>
         </is>
       </c>
-      <c r="N18" s="9" t="inlineStr">
+      <c r="N18" s="13" t="inlineStr">
         <is>
           <t>通鼎互联</t>
         </is>
@@ -8762,12 +8768,12 @@
           <t>燕塘乳业</t>
         </is>
       </c>
-      <c r="C19" s="19" t="inlineStr">
+      <c r="C19" s="20" t="inlineStr">
         <is>
           <t>京华激光</t>
         </is>
       </c>
-      <c r="D19" s="12" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>荣丰控股3</t>
         </is>
@@ -8777,7 +8783,7 @@
           <t>南京港2</t>
         </is>
       </c>
-      <c r="F19" s="25" t="inlineStr">
+      <c r="F19" s="28" t="inlineStr">
         <is>
           <t>红蜻蜓2</t>
         </is>
@@ -8787,59 +8793,59 @@
           <t>航发科技2</t>
         </is>
       </c>
-      <c r="H19" s="12" t="inlineStr">
+      <c r="H19" s="5" t="inlineStr">
         <is>
           <t>海联金汇4</t>
         </is>
       </c>
-      <c r="I19" s="12" t="inlineStr">
+      <c r="I19" s="14" t="inlineStr">
         <is>
           <t>朝阳科技2</t>
         </is>
       </c>
-      <c r="J19" s="12" t="inlineStr">
+      <c r="J19" s="9" t="inlineStr">
         <is>
           <t>浙江荣泰3</t>
         </is>
       </c>
-      <c r="K19" s="9" t="inlineStr">
+      <c r="K19" s="13" t="inlineStr">
         <is>
           <t>康盛股份</t>
         </is>
       </c>
-      <c r="L19" s="9" t="inlineStr">
+      <c r="L19" s="13" t="inlineStr">
         <is>
           <t>金麒麟2</t>
         </is>
       </c>
-      <c r="M19" s="19" t="inlineStr">
+      <c r="M19" s="20" t="inlineStr">
         <is>
           <t>菜百股份</t>
         </is>
       </c>
-      <c r="N19" s="9" t="inlineStr">
+      <c r="N19" s="12" t="inlineStr">
         <is>
           <t>九鼎新材2</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="19" t="inlineStr">
+      <c r="B20" s="20" t="inlineStr">
         <is>
           <t>华达新材</t>
         </is>
       </c>
-      <c r="C20" s="19" t="inlineStr">
+      <c r="C20" s="9" t="inlineStr">
         <is>
           <t>大胜达</t>
         </is>
       </c>
-      <c r="D20" s="9" t="inlineStr">
+      <c r="D20" s="13" t="inlineStr">
         <is>
           <t>亚联机械5</t>
         </is>
       </c>
-      <c r="E20" s="9" t="inlineStr">
+      <c r="E20" s="13" t="inlineStr">
         <is>
           <t>特力A3</t>
         </is>
@@ -8849,7 +8855,7 @@
           <t>山东华鹏</t>
         </is>
       </c>
-      <c r="G20" s="9" t="inlineStr">
+      <c r="G20" s="13" t="inlineStr">
         <is>
           <t>威尔药业4</t>
         </is>
@@ -8864,22 +8870,22 @@
           <t>春秋电子</t>
         </is>
       </c>
-      <c r="J20" s="6" t="inlineStr">
+      <c r="J20" s="9" t="inlineStr">
         <is>
           <t>方正电机3</t>
         </is>
       </c>
-      <c r="K20" s="9" t="inlineStr">
+      <c r="K20" s="13" t="inlineStr">
         <is>
           <t>珀莱雅2</t>
         </is>
       </c>
-      <c r="L20" s="19" t="inlineStr">
+      <c r="L20" s="20" t="inlineStr">
         <is>
           <t>普路通</t>
         </is>
       </c>
-      <c r="M20" s="9" t="inlineStr">
+      <c r="M20" s="13" t="inlineStr">
         <is>
           <t>三和管桩</t>
         </is>
@@ -8906,7 +8912,7 @@
           <t>安记食品7</t>
         </is>
       </c>
-      <c r="E21" s="11" t="inlineStr">
+      <c r="E21" s="8" t="inlineStr">
         <is>
           <t>渤海化学3</t>
         </is>
@@ -8916,7 +8922,7 @@
           <t>三夫户外2</t>
         </is>
       </c>
-      <c r="G21" s="12" t="inlineStr">
+      <c r="G21" s="5" t="inlineStr">
         <is>
           <t>华脉科技2</t>
         </is>
@@ -8926,17 +8932,17 @@
           <t>安正时尚3</t>
         </is>
       </c>
-      <c r="I21" s="9" t="inlineStr">
+      <c r="I21" s="8" t="inlineStr">
         <is>
           <t>卫星化学2</t>
         </is>
       </c>
-      <c r="J21" s="7" t="inlineStr">
+      <c r="J21" s="9" t="inlineStr">
         <is>
           <t>东贝集团4</t>
         </is>
       </c>
-      <c r="K21" s="12" t="inlineStr">
+      <c r="K21" s="5" t="inlineStr">
         <is>
           <t>塞力医疗2</t>
         </is>
@@ -8951,19 +8957,19 @@
           <t>迪生力3</t>
         </is>
       </c>
-      <c r="N21" s="4" t="inlineStr">
+      <c r="N21" s="6" t="inlineStr">
         <is>
           <t>深康佳A</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="23" t="inlineStr">
+      <c r="B22" s="26" t="inlineStr">
         <is>
           <t>和科达2</t>
         </is>
       </c>
-      <c r="C22" s="9" t="inlineStr">
+      <c r="C22" s="13" t="inlineStr">
         <is>
           <t>九洲药业</t>
         </is>
@@ -8978,12 +8984,12 @@
           <t>天保基建6</t>
         </is>
       </c>
-      <c r="F22" s="19" t="inlineStr">
+      <c r="F22" s="20" t="inlineStr">
         <is>
           <t>三湘印象</t>
         </is>
       </c>
-      <c r="G22" s="7" t="inlineStr">
+      <c r="G22" s="4" t="inlineStr">
         <is>
           <t>五芳斋2</t>
         </is>
@@ -8993,17 +8999,17 @@
           <t>华泰股份2</t>
         </is>
       </c>
-      <c r="I22" s="19" t="inlineStr">
+      <c r="I22" s="20" t="inlineStr">
         <is>
           <t>浙江自然</t>
         </is>
       </c>
-      <c r="J22" s="12" t="inlineStr">
+      <c r="J22" s="9" t="inlineStr">
         <is>
           <t>丰华股份2</t>
         </is>
       </c>
-      <c r="K22" s="9" t="inlineStr">
+      <c r="K22" s="13" t="inlineStr">
         <is>
           <t>九牧王</t>
         </is>
@@ -9013,7 +9019,7 @@
           <t>三夫户外2</t>
         </is>
       </c>
-      <c r="M22" s="11" t="inlineStr">
+      <c r="M22" s="8" t="inlineStr">
         <is>
           <t>三孚股份2</t>
         </is>
@@ -9025,27 +9031,27 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="19" t="inlineStr">
+      <c r="B23" s="20" t="inlineStr">
         <is>
           <t>宁水集团</t>
         </is>
       </c>
-      <c r="C23" s="19" t="inlineStr">
+      <c r="C23" s="12" t="inlineStr">
         <is>
           <t>华嵘控股</t>
         </is>
       </c>
-      <c r="D23" s="25" t="inlineStr">
+      <c r="D23" s="28" t="inlineStr">
         <is>
           <t>利仁科技2</t>
         </is>
       </c>
-      <c r="E23" s="12" t="inlineStr">
+      <c r="E23" s="5" t="inlineStr">
         <is>
           <t>金陵饭店2</t>
         </is>
       </c>
-      <c r="F23" s="12" t="inlineStr">
+      <c r="F23" s="5" t="inlineStr">
         <is>
           <t>海能达2</t>
         </is>
@@ -9055,104 +9061,104 @@
           <t>石基信息2</t>
         </is>
       </c>
-      <c r="H23" s="9" t="inlineStr">
+      <c r="H23" s="13" t="inlineStr">
         <is>
           <t>先达股份5</t>
         </is>
       </c>
-      <c r="I23" s="9" t="inlineStr">
+      <c r="I23" s="13" t="inlineStr">
         <is>
           <t>永茂泰</t>
         </is>
       </c>
-      <c r="J23" s="12" t="inlineStr">
+      <c r="J23" s="5" t="inlineStr">
         <is>
           <t>棒杰股份2</t>
         </is>
       </c>
-      <c r="K23" s="9" t="inlineStr">
+      <c r="K23" s="13" t="inlineStr">
         <is>
           <t>顺博合金</t>
         </is>
       </c>
-      <c r="L23" s="9" t="inlineStr">
+      <c r="L23" s="8" t="inlineStr">
         <is>
           <t>金能科技</t>
         </is>
       </c>
-      <c r="M23" s="9" t="inlineStr">
+      <c r="M23" s="13" t="inlineStr">
         <is>
           <t>道道全</t>
         </is>
       </c>
-      <c r="N23" s="12" t="inlineStr">
+      <c r="N23" s="5" t="inlineStr">
         <is>
           <t>莱绅通灵3</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="19" t="inlineStr">
+      <c r="B24" s="20" t="inlineStr">
         <is>
           <t>实益达</t>
         </is>
       </c>
-      <c r="C24" s="12" t="inlineStr">
+      <c r="C24" s="5" t="inlineStr">
         <is>
           <t>罗欣药业2</t>
         </is>
       </c>
-      <c r="D24" s="19" t="inlineStr">
+      <c r="D24" s="20" t="inlineStr">
         <is>
           <t>华资实业</t>
         </is>
       </c>
-      <c r="E24" s="12" t="inlineStr">
+      <c r="E24" s="14" t="inlineStr">
         <is>
           <t>东珠生态6</t>
         </is>
       </c>
-      <c r="F24" s="19" t="inlineStr">
+      <c r="F24" s="20" t="inlineStr">
         <is>
           <t>御银股份</t>
         </is>
       </c>
-      <c r="G24" s="12" t="inlineStr">
+      <c r="G24" s="5" t="inlineStr">
         <is>
           <t>海能达2</t>
         </is>
       </c>
-      <c r="H24" s="12" t="inlineStr">
+      <c r="H24" s="5" t="inlineStr">
         <is>
           <t>青岛金王3</t>
         </is>
       </c>
-      <c r="I24" s="5" t="inlineStr">
+      <c r="I24" s="20" t="inlineStr">
         <is>
           <t>襄阳轴承</t>
         </is>
       </c>
-      <c r="J24" s="12" t="inlineStr">
+      <c r="J24" s="5" t="inlineStr">
         <is>
           <t>西陇科学3</t>
         </is>
       </c>
-      <c r="K24" s="19" t="inlineStr">
+      <c r="K24" s="20" t="inlineStr">
         <is>
           <t>恒宝股份</t>
         </is>
       </c>
-      <c r="L24" s="7" t="inlineStr">
+      <c r="L24" s="14" t="inlineStr">
         <is>
           <t>金财互联</t>
         </is>
       </c>
-      <c r="M24" s="19" t="inlineStr">
+      <c r="M24" s="12" t="inlineStr">
         <is>
           <t>申科股份</t>
         </is>
       </c>
-      <c r="N24" s="12" t="inlineStr">
+      <c r="N24" s="5" t="inlineStr">
         <is>
           <t>翠微股份3</t>
         </is>
@@ -9164,7 +9170,7 @@
           <t>超声电子</t>
         </is>
       </c>
-      <c r="C25" s="19" t="inlineStr">
+      <c r="C25" s="20" t="inlineStr">
         <is>
           <t>思美传媒</t>
         </is>
@@ -9174,32 +9180,32 @@
           <t>集泰股份</t>
         </is>
       </c>
-      <c r="E25" s="12" t="inlineStr">
+      <c r="E25" s="5" t="inlineStr">
         <is>
           <t>兄弟科技2</t>
         </is>
       </c>
-      <c r="F25" s="12" t="inlineStr">
+      <c r="F25" s="5" t="inlineStr">
         <is>
           <t>九鼎投资2</t>
         </is>
       </c>
-      <c r="G25" s="12" t="inlineStr">
+      <c r="G25" s="5" t="inlineStr">
         <is>
           <t>大千生态5</t>
         </is>
       </c>
-      <c r="H25" s="12" t="inlineStr">
+      <c r="H25" s="14" t="inlineStr">
         <is>
           <t>信雅达2</t>
         </is>
       </c>
-      <c r="I25" s="12" t="inlineStr">
+      <c r="I25" s="9" t="inlineStr">
         <is>
           <t>丰华股份2</t>
         </is>
       </c>
-      <c r="J25" s="12" t="inlineStr">
+      <c r="J25" s="5" t="inlineStr">
         <is>
           <t>三维化学2</t>
         </is>
@@ -9209,29 +9215,29 @@
           <t>广誉远</t>
         </is>
       </c>
-      <c r="L25" s="9" t="inlineStr">
+      <c r="L25" s="14" t="inlineStr">
         <is>
           <t>大位科技2</t>
         </is>
       </c>
-      <c r="M25" s="19" t="inlineStr">
+      <c r="M25" s="20" t="inlineStr">
         <is>
           <t>蓝帆医疗</t>
         </is>
       </c>
-      <c r="N25" s="11" t="inlineStr">
+      <c r="N25" s="9" t="inlineStr">
         <is>
           <t>探路者</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="9" t="inlineStr">
+      <c r="B26" s="14" t="inlineStr">
         <is>
           <t>美格智能</t>
         </is>
       </c>
-      <c r="C26" s="19" t="inlineStr">
+      <c r="C26" s="20" t="inlineStr">
         <is>
           <t>英利汽车</t>
         </is>
@@ -9241,22 +9247,22 @@
           <t>上海雅仕</t>
         </is>
       </c>
-      <c r="E26" s="26" t="inlineStr">
+      <c r="E26" s="27" t="inlineStr">
         <is>
           <t>桂发祥2</t>
         </is>
       </c>
-      <c r="F26" s="12" t="inlineStr">
+      <c r="F26" s="5" t="inlineStr">
         <is>
           <t>新能泰山2</t>
         </is>
       </c>
-      <c r="G26" s="12" t="inlineStr">
+      <c r="G26" s="5" t="inlineStr">
         <is>
           <t>莱绅通灵3</t>
         </is>
       </c>
-      <c r="H26" s="12" t="inlineStr">
+      <c r="H26" s="5" t="inlineStr">
         <is>
           <t>顺灏股份2</t>
         </is>
@@ -9266,7 +9272,7 @@
           <t>卓翼科技</t>
         </is>
       </c>
-      <c r="J26" s="23" t="inlineStr">
+      <c r="J26" s="26" t="inlineStr">
         <is>
           <t>健尔康3</t>
         </is>
@@ -9276,49 +9282,49 @@
           <t>亚太实业3</t>
         </is>
       </c>
-      <c r="L26" s="19" t="inlineStr">
+      <c r="L26" s="20" t="inlineStr">
         <is>
           <t>新锦动力</t>
         </is>
       </c>
-      <c r="M26" s="9" t="inlineStr">
+      <c r="M26" s="13" t="inlineStr">
         <is>
           <t>博创科技</t>
         </is>
       </c>
-      <c r="N26" s="19" t="inlineStr">
+      <c r="N26" s="9" t="inlineStr">
         <is>
           <t>振江股份</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="7" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>南极电商2</t>
         </is>
       </c>
-      <c r="C27" s="9" t="inlineStr">
+      <c r="C27" s="13" t="inlineStr">
         <is>
           <t>亚联机械5</t>
         </is>
       </c>
-      <c r="D27" s="19" t="inlineStr">
+      <c r="D27" s="20" t="inlineStr">
         <is>
           <t>中创物流</t>
         </is>
       </c>
-      <c r="E27" s="9" t="inlineStr">
+      <c r="E27" s="13" t="inlineStr">
         <is>
           <t>新宏泽2</t>
         </is>
       </c>
-      <c r="F27" s="11" t="inlineStr">
+      <c r="F27" s="13" t="inlineStr">
         <is>
           <t>达利凯普</t>
         </is>
       </c>
-      <c r="G27" s="12" t="inlineStr">
+      <c r="G27" s="5" t="inlineStr">
         <is>
           <t>仁智股份2</t>
         </is>
@@ -9328,7 +9334,7 @@
           <t>生意宝4</t>
         </is>
       </c>
-      <c r="I27" s="9" t="inlineStr">
+      <c r="I27" s="13" t="inlineStr">
         <is>
           <t>健尔康3</t>
         </is>
@@ -9338,29 +9344,29 @@
           <t>迪生力3</t>
         </is>
       </c>
-      <c r="K27" s="12" t="inlineStr">
+      <c r="K27" s="9" t="inlineStr">
         <is>
           <t>天娱数科2</t>
         </is>
       </c>
-      <c r="L27" s="19" t="inlineStr">
+      <c r="L27" s="20" t="inlineStr">
         <is>
           <t>狮头股份</t>
         </is>
       </c>
-      <c r="M27" s="9" t="inlineStr">
+      <c r="M27" s="14" t="inlineStr">
         <is>
           <t>奥拓电子</t>
         </is>
       </c>
-      <c r="N27" s="5" t="inlineStr">
+      <c r="N27" s="14" t="inlineStr">
         <is>
           <t>润贝航科5</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="19" t="inlineStr">
+      <c r="B28" s="12" t="inlineStr">
         <is>
           <t>大金重工</t>
         </is>
@@ -9370,7 +9376,7 @@
           <t>创源股份</t>
         </is>
       </c>
-      <c r="D28" s="5" t="inlineStr">
+      <c r="D28" s="12" t="inlineStr">
         <is>
           <t>飞沃科技</t>
         </is>
@@ -9380,17 +9386,17 @@
           <t>蓝科高新2</t>
         </is>
       </c>
-      <c r="F28" s="19" t="inlineStr">
+      <c r="F28" s="20" t="inlineStr">
         <is>
           <t>巨力索具</t>
         </is>
       </c>
-      <c r="G28" s="12" t="inlineStr">
+      <c r="G28" s="5" t="inlineStr">
         <is>
           <t>新华联2</t>
         </is>
       </c>
-      <c r="H28" s="12" t="inlineStr">
+      <c r="H28" s="5" t="inlineStr">
         <is>
           <t>三房巷2</t>
         </is>
@@ -9400,17 +9406,17 @@
           <t>华纬科技</t>
         </is>
       </c>
-      <c r="J28" s="12" t="inlineStr">
+      <c r="J28" s="5" t="inlineStr">
         <is>
           <t>好想你2</t>
         </is>
       </c>
-      <c r="K28" s="19" t="inlineStr">
+      <c r="K28" s="20" t="inlineStr">
         <is>
           <t>天元智能</t>
         </is>
       </c>
-      <c r="L28" s="19" t="inlineStr">
+      <c r="L28" s="14" t="inlineStr">
         <is>
           <t>德生科技</t>
         </is>
@@ -9420,7 +9426,7 @@
           <t>聚赛龙</t>
         </is>
       </c>
-      <c r="N28" s="9" t="inlineStr">
+      <c r="N28" s="14" t="inlineStr">
         <is>
           <t>正和生态2</t>
         </is>
@@ -9432,7 +9438,7 @@
           <t>瀛通通讯3</t>
         </is>
       </c>
-      <c r="C29" s="19" t="inlineStr">
+      <c r="C29" s="20" t="inlineStr">
         <is>
           <t>国华网安</t>
         </is>
@@ -9442,7 +9448,7 @@
           <t>天保基建6</t>
         </is>
       </c>
-      <c r="E29" s="19" t="inlineStr">
+      <c r="E29" s="20" t="inlineStr">
         <is>
           <t>德尔未来</t>
         </is>
@@ -9452,17 +9458,17 @@
           <t>百大集团3</t>
         </is>
       </c>
-      <c r="G29" s="24" t="inlineStr">
+      <c r="G29" s="27" t="inlineStr">
         <is>
           <t>国风新材2</t>
         </is>
       </c>
-      <c r="H29" s="26" t="inlineStr">
+      <c r="H29" s="29" t="inlineStr">
         <is>
           <t>有友食品2</t>
         </is>
       </c>
-      <c r="I29" s="6" t="inlineStr">
+      <c r="I29" s="9" t="inlineStr">
         <is>
           <t>方正电机3</t>
         </is>
@@ -9472,17 +9478,17 @@
           <t>茂业商业5</t>
         </is>
       </c>
-      <c r="K29" s="9" t="inlineStr">
+      <c r="K29" s="12" t="inlineStr">
         <is>
           <t>华电辽能2</t>
         </is>
       </c>
-      <c r="L29" s="19" t="inlineStr">
+      <c r="L29" s="9" t="inlineStr">
         <is>
           <t>四川金顶</t>
         </is>
       </c>
-      <c r="M29" s="19" t="inlineStr">
+      <c r="M29" s="14" t="inlineStr">
         <is>
           <t>利通电子</t>
         </is>
@@ -9519,7 +9525,7 @@
           <t>神马股份</t>
         </is>
       </c>
-      <c r="G30" s="12" t="inlineStr">
+      <c r="G30" s="9" t="inlineStr">
         <is>
           <t>京城股份2</t>
         </is>
@@ -9529,17 +9535,17 @@
           <t>致尚科技2</t>
         </is>
       </c>
-      <c r="I30" s="9" t="inlineStr">
+      <c r="I30" s="13" t="inlineStr">
         <is>
           <t>金富科技2</t>
         </is>
       </c>
-      <c r="J30" s="9" t="inlineStr">
+      <c r="J30" s="13" t="inlineStr">
         <is>
           <t>金凯生科</t>
         </is>
       </c>
-      <c r="K30" s="19" t="inlineStr">
+      <c r="K30" s="12" t="inlineStr">
         <is>
           <t>吉鑫科技</t>
         </is>
@@ -9549,19 +9555,19 @@
           <t>京能电力</t>
         </is>
       </c>
-      <c r="M30" s="19" t="inlineStr">
+      <c r="M30" s="9" t="inlineStr">
         <is>
           <t>银宝山新</t>
         </is>
       </c>
-      <c r="N30" s="9" t="inlineStr">
+      <c r="N30" s="14" t="inlineStr">
         <is>
           <t>超讯通信</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="19" t="inlineStr">
+      <c r="B31" s="9" t="inlineStr">
         <is>
           <t>合锻智能</t>
         </is>
@@ -9571,32 +9577,32 @@
           <t>岭南股份</t>
         </is>
       </c>
-      <c r="D31" s="19" t="inlineStr">
+      <c r="D31" s="20" t="inlineStr">
         <is>
           <t>重庆港</t>
         </is>
       </c>
-      <c r="E31" s="12" t="inlineStr">
+      <c r="E31" s="5" t="inlineStr">
         <is>
           <t>渝开发3</t>
         </is>
       </c>
-      <c r="F31" s="12" t="inlineStr">
+      <c r="F31" s="5" t="inlineStr">
         <is>
           <t>武汉凡谷2</t>
         </is>
       </c>
-      <c r="G31" s="19" t="inlineStr">
+      <c r="G31" s="20" t="inlineStr">
         <is>
           <t>琏升科技</t>
         </is>
       </c>
-      <c r="H31" s="12" t="inlineStr">
+      <c r="H31" s="5" t="inlineStr">
         <is>
           <t>新晨科技2</t>
         </is>
       </c>
-      <c r="I31" s="19" t="inlineStr">
+      <c r="I31" s="14" t="inlineStr">
         <is>
           <t>中科金财</t>
         </is>
@@ -9606,12 +9612,12 @@
           <t>浔兴股份5</t>
         </is>
       </c>
-      <c r="K31" s="12" t="inlineStr">
+      <c r="K31" s="5" t="inlineStr">
         <is>
           <t>天府文旅2</t>
         </is>
       </c>
-      <c r="L31" s="12" t="inlineStr">
+      <c r="L31" s="5" t="inlineStr">
         <is>
           <t>新能泰山2</t>
         </is>
@@ -9621,7 +9627,7 @@
           <t>沈阳化工</t>
         </is>
       </c>
-      <c r="N31" s="6" t="inlineStr">
+      <c r="N31" s="14" t="inlineStr">
         <is>
           <t>浙文互联</t>
         </is>
@@ -9633,7 +9639,7 @@
           <t>生意宝4</t>
         </is>
       </c>
-      <c r="C32" s="19" t="inlineStr">
+      <c r="C32" s="20" t="inlineStr">
         <is>
           <t>金龙羽</t>
         </is>
@@ -9643,27 +9649,27 @@
           <t>维维股份2</t>
         </is>
       </c>
-      <c r="E32" s="12" t="inlineStr">
+      <c r="E32" s="5" t="inlineStr">
         <is>
           <t>西陇科学3</t>
         </is>
       </c>
-      <c r="F32" s="12" t="inlineStr">
+      <c r="F32" s="5" t="inlineStr">
         <is>
           <t>新华联2</t>
         </is>
       </c>
-      <c r="G32" s="12" t="inlineStr">
+      <c r="G32" s="5" t="inlineStr">
         <is>
           <t>绿康生化2</t>
         </is>
       </c>
-      <c r="H32" s="9" t="inlineStr">
+      <c r="H32" s="13" t="inlineStr">
         <is>
           <t>福斯达</t>
         </is>
       </c>
-      <c r="I32" s="6" t="inlineStr">
+      <c r="I32" s="9" t="inlineStr">
         <is>
           <t>日海智能</t>
         </is>
@@ -9673,7 +9679,7 @@
           <t>华银电力3</t>
         </is>
       </c>
-      <c r="K32" s="19" t="inlineStr">
+      <c r="K32" s="20" t="inlineStr">
         <is>
           <t>方大集团</t>
         </is>
@@ -9683,29 +9689,29 @@
           <t>恒润股份</t>
         </is>
       </c>
-      <c r="M32" s="9" t="inlineStr">
+      <c r="M32" s="13" t="inlineStr">
         <is>
           <t>新坐标2</t>
         </is>
       </c>
-      <c r="N32" s="12" t="inlineStr">
+      <c r="N32" s="5" t="inlineStr">
         <is>
           <t>重庆建工3</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="19" t="inlineStr">
+      <c r="B33" s="20" t="inlineStr">
         <is>
           <t>舒华体育</t>
         </is>
       </c>
-      <c r="C33" s="9" t="inlineStr">
+      <c r="C33" s="13" t="inlineStr">
         <is>
           <t>建投能源</t>
         </is>
       </c>
-      <c r="D33" s="12" t="inlineStr">
+      <c r="D33" s="14" t="inlineStr">
         <is>
           <t>恒锋信息2</t>
         </is>
@@ -9715,7 +9721,7 @@
           <t>国风新材2</t>
         </is>
       </c>
-      <c r="F33" s="7" t="inlineStr">
+      <c r="F33" s="4" t="inlineStr">
         <is>
           <t>文峰股份</t>
         </is>
@@ -9725,27 +9731,27 @@
           <t>久其软件2</t>
         </is>
       </c>
-      <c r="H33" s="7" t="inlineStr">
+      <c r="H33" s="6" t="inlineStr">
         <is>
           <t>三木集团3</t>
         </is>
       </c>
-      <c r="I33" s="19" t="inlineStr">
+      <c r="I33" s="9" t="inlineStr">
         <is>
           <t>秦川机床</t>
         </is>
       </c>
-      <c r="J33" s="12" t="inlineStr">
+      <c r="J33" s="5" t="inlineStr">
         <is>
           <t>渝开发3</t>
         </is>
       </c>
-      <c r="K33" s="9" t="inlineStr">
+      <c r="K33" s="12" t="inlineStr">
         <is>
           <t>华电能源2</t>
         </is>
       </c>
-      <c r="L33" s="12" t="inlineStr">
+      <c r="L33" s="5" t="inlineStr">
         <is>
           <t>大千生态5</t>
         </is>
@@ -9755,24 +9761,24 @@
           <t>新瀚新材2</t>
         </is>
       </c>
-      <c r="N33" s="9" t="inlineStr">
+      <c r="N33" s="13" t="inlineStr">
         <is>
           <t>保龄宝</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="5" t="inlineStr">
+      <c r="B34" s="9" t="inlineStr">
         <is>
           <t>中超控股2</t>
         </is>
       </c>
-      <c r="C34" s="19" t="inlineStr">
+      <c r="C34" s="20" t="inlineStr">
         <is>
           <t>领湃科技</t>
         </is>
       </c>
-      <c r="D34" s="19" t="inlineStr">
+      <c r="D34" s="20" t="inlineStr">
         <is>
           <t>华建集团</t>
         </is>
@@ -9782,7 +9788,7 @@
           <t>善水科技</t>
         </is>
       </c>
-      <c r="F34" s="9" t="inlineStr">
+      <c r="F34" s="13" t="inlineStr">
         <is>
           <t>威尔药业4</t>
         </is>
@@ -9797,7 +9803,7 @@
           <t>长江投资</t>
         </is>
       </c>
-      <c r="I34" s="12" t="inlineStr">
+      <c r="I34" s="9" t="inlineStr">
         <is>
           <t>南方精工3</t>
         </is>
@@ -9807,17 +9813,17 @@
           <t>郴电国际</t>
         </is>
       </c>
-      <c r="K34" s="7" t="inlineStr">
+      <c r="K34" s="4" t="inlineStr">
         <is>
           <t>中央商场</t>
         </is>
       </c>
-      <c r="L34" s="6" t="inlineStr">
+      <c r="L34" s="8" t="inlineStr">
         <is>
           <t>中毅达3</t>
         </is>
       </c>
-      <c r="M34" s="9" t="inlineStr">
+      <c r="M34" s="8" t="inlineStr">
         <is>
           <t>大洋生物</t>
         </is>
@@ -9829,7 +9835,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="19" t="inlineStr">
+      <c r="B35" s="14" t="inlineStr">
         <is>
           <t>京北方</t>
         </is>
@@ -9839,17 +9845,17 @@
           <t>红宝丽5</t>
         </is>
       </c>
-      <c r="D35" s="9" t="inlineStr">
+      <c r="D35" s="13" t="inlineStr">
         <is>
           <t>特力A3</t>
         </is>
       </c>
-      <c r="E35" s="11" t="inlineStr">
+      <c r="E35" s="12" t="inlineStr">
         <is>
           <t>睿能科技</t>
         </is>
       </c>
-      <c r="F35" s="12" t="inlineStr">
+      <c r="F35" s="5" t="inlineStr">
         <is>
           <t>神开股份2</t>
         </is>
@@ -9859,7 +9865,7 @@
           <t>跨境通3</t>
         </is>
       </c>
-      <c r="H35" s="19" t="inlineStr">
+      <c r="H35" s="20" t="inlineStr">
         <is>
           <t>万林物流</t>
         </is>
@@ -9869,7 +9875,7 @@
           <t>宁波东力3</t>
         </is>
       </c>
-      <c r="J35" s="19" t="inlineStr">
+      <c r="J35" s="20" t="inlineStr">
         <is>
           <t>河化股份</t>
         </is>
@@ -9879,49 +9885,49 @@
           <t>北鼎股份</t>
         </is>
       </c>
-      <c r="L35" s="9" t="inlineStr">
+      <c r="L35" s="13" t="inlineStr">
         <is>
           <t>廊坊发展</t>
         </is>
       </c>
-      <c r="M35" s="12" t="inlineStr">
+      <c r="M35" s="14" t="inlineStr">
         <is>
           <t>利欧股份2</t>
         </is>
       </c>
-      <c r="N35" s="11" t="inlineStr">
+      <c r="N35" s="20" t="inlineStr">
         <is>
           <t>冠石科技</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="27" t="inlineStr">
+      <c r="B36" s="20" t="inlineStr">
         <is>
           <t>兰生股份</t>
         </is>
       </c>
-      <c r="C36" s="12" t="inlineStr">
+      <c r="C36" s="5" t="inlineStr">
         <is>
           <t>兄弟科技2</t>
         </is>
       </c>
-      <c r="D36" s="9" t="inlineStr">
+      <c r="D36" s="13" t="inlineStr">
         <is>
           <t>健尔康3</t>
         </is>
       </c>
-      <c r="E36" s="19" t="inlineStr">
+      <c r="E36" s="20" t="inlineStr">
         <is>
           <t>神雾节能</t>
         </is>
       </c>
-      <c r="F36" s="12" t="inlineStr">
+      <c r="F36" s="5" t="inlineStr">
         <is>
           <t>华脉科技2</t>
         </is>
       </c>
-      <c r="G36" s="5" t="inlineStr">
+      <c r="G36" s="9" t="inlineStr">
         <is>
           <t>利君股份</t>
         </is>
@@ -9946,17 +9952,17 @@
           <t>宇晶股份</t>
         </is>
       </c>
-      <c r="L36" s="9" t="inlineStr">
+      <c r="L36" s="13" t="inlineStr">
         <is>
           <t>弘景光电</t>
         </is>
       </c>
-      <c r="M36" s="11" t="inlineStr">
+      <c r="M36" s="9" t="inlineStr">
         <is>
           <t>日盈电子</t>
         </is>
       </c>
-      <c r="N36" s="19" t="inlineStr">
+      <c r="N36" s="20" t="inlineStr">
         <is>
           <t>未名医药</t>
         </is>
@@ -9968,12 +9974,12 @@
           <t>国光连锁6</t>
         </is>
       </c>
-      <c r="C37" s="7" t="inlineStr">
+      <c r="C37" s="6" t="inlineStr">
         <is>
           <t>华贸物流4</t>
         </is>
       </c>
-      <c r="D37" s="19" t="inlineStr">
+      <c r="D37" s="20" t="inlineStr">
         <is>
           <t>中关村</t>
         </is>
@@ -9998,12 +10004,12 @@
           <t>嘉诚国际</t>
         </is>
       </c>
-      <c r="I37" s="9" t="inlineStr">
+      <c r="I37" s="13" t="inlineStr">
         <is>
           <t>芯瑞达</t>
         </is>
       </c>
-      <c r="J37" s="19" t="inlineStr">
+      <c r="J37" s="20" t="inlineStr">
         <is>
           <t>永杉锂业</t>
         </is>
@@ -10018,44 +10024,44 @@
           <t>瀛通通讯3</t>
         </is>
       </c>
-      <c r="M37" s="12" t="inlineStr">
+      <c r="M37" s="5" t="inlineStr">
         <is>
           <t>东方创业2</t>
         </is>
       </c>
-      <c r="N37" s="9" t="inlineStr">
+      <c r="N37" s="13" t="inlineStr">
         <is>
           <t>大博医疗</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="19" t="inlineStr">
+      <c r="B38" s="20" t="inlineStr">
         <is>
           <t>康普顿</t>
         </is>
       </c>
-      <c r="C38" s="12" t="inlineStr">
+      <c r="C38" s="5" t="inlineStr">
         <is>
           <t>大千生态5</t>
         </is>
       </c>
-      <c r="D38" s="12" t="inlineStr">
+      <c r="D38" s="5" t="inlineStr">
         <is>
           <t>金陵饭店2</t>
         </is>
       </c>
-      <c r="E38" s="19" t="inlineStr">
+      <c r="E38" s="12" t="inlineStr">
         <is>
           <t>神力股份</t>
         </is>
       </c>
-      <c r="F38" s="19" t="inlineStr">
+      <c r="F38" s="9" t="inlineStr">
         <is>
           <t>奇精机械</t>
         </is>
       </c>
-      <c r="G38" s="9" t="inlineStr">
+      <c r="G38" s="13" t="inlineStr">
         <is>
           <t>鹏欣资源</t>
         </is>
@@ -10065,27 +10071,27 @@
           <t>中通客车</t>
         </is>
       </c>
-      <c r="I38" s="19" t="inlineStr">
+      <c r="I38" s="9" t="inlineStr">
         <is>
           <t>光洋股份</t>
         </is>
       </c>
-      <c r="J38" s="19" t="inlineStr">
+      <c r="J38" s="20" t="inlineStr">
         <is>
           <t>菲林格尔</t>
         </is>
       </c>
-      <c r="K38" s="12" t="inlineStr">
+      <c r="K38" s="5" t="inlineStr">
         <is>
           <t>深中华A2</t>
         </is>
       </c>
-      <c r="L38" s="9" t="inlineStr">
+      <c r="L38" s="13" t="inlineStr">
         <is>
           <t>新北洋</t>
         </is>
       </c>
-      <c r="M38" s="9" t="inlineStr">
+      <c r="M38" s="13" t="inlineStr">
         <is>
           <t>蓝丰生化</t>
         </is>
@@ -10097,7 +10103,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="19" t="inlineStr">
+      <c r="B39" s="20" t="inlineStr">
         <is>
           <t>曲美家居</t>
         </is>
@@ -10112,12 +10118,12 @@
           <t>华茂股份</t>
         </is>
       </c>
-      <c r="E39" s="19" t="inlineStr">
+      <c r="E39" s="14" t="inlineStr">
         <is>
           <t>福鞍股份</t>
         </is>
       </c>
-      <c r="F39" s="7" t="inlineStr">
+      <c r="F39" s="4" t="inlineStr">
         <is>
           <t>友阿股份</t>
         </is>
@@ -10132,17 +10138,17 @@
           <t>庄园牧场</t>
         </is>
       </c>
-      <c r="I39" s="12" t="inlineStr">
+      <c r="I39" s="14" t="inlineStr">
         <is>
           <t>东珠生态6</t>
         </is>
       </c>
-      <c r="J39" s="9" t="inlineStr">
+      <c r="J39" s="13" t="inlineStr">
         <is>
           <t>尔康制药</t>
         </is>
       </c>
-      <c r="K39" s="9" t="inlineStr">
+      <c r="K39" s="8" t="inlineStr">
         <is>
           <t>天原股份</t>
         </is>
@@ -10152,7 +10158,7 @@
           <t>雅博股份</t>
         </is>
       </c>
-      <c r="M39" s="9" t="inlineStr">
+      <c r="M39" s="13" t="inlineStr">
         <is>
           <t>哈森股份</t>
         </is>
@@ -10164,17 +10170,17 @@
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="12" t="inlineStr">
+      <c r="B40" s="5" t="inlineStr">
         <is>
           <t>威领股份2</t>
         </is>
       </c>
-      <c r="C40" s="19" t="inlineStr">
+      <c r="C40" s="20" t="inlineStr">
         <is>
           <t>洁雅股份</t>
         </is>
       </c>
-      <c r="D40" s="19" t="inlineStr">
+      <c r="D40" s="20" t="inlineStr">
         <is>
           <t>强邦新材</t>
         </is>
@@ -10184,7 +10190,7 @@
           <t>怡达股份</t>
         </is>
       </c>
-      <c r="F40" s="12" t="inlineStr">
+      <c r="F40" s="5" t="inlineStr">
         <is>
           <t>大千生态5</t>
         </is>
@@ -10194,17 +10200,17 @@
           <t>西王食品2</t>
         </is>
       </c>
-      <c r="H40" s="19" t="inlineStr">
+      <c r="H40" s="20" t="inlineStr">
         <is>
           <t>优博讯</t>
         </is>
       </c>
-      <c r="I40" s="19" t="inlineStr">
+      <c r="I40" s="9" t="inlineStr">
         <is>
           <t>利安科技</t>
         </is>
       </c>
-      <c r="J40" s="9" t="inlineStr">
+      <c r="J40" s="13" t="inlineStr">
         <is>
           <t>凯莱英</t>
         </is>
@@ -10214,59 +10220,59 @@
           <t>中坚科技</t>
         </is>
       </c>
-      <c r="L40" s="12" t="inlineStr">
+      <c r="L40" s="5" t="inlineStr">
         <is>
           <t>宿迁联盛2</t>
         </is>
       </c>
-      <c r="M40" s="19" t="inlineStr">
+      <c r="M40" s="9" t="inlineStr">
         <is>
           <t>鼎际得</t>
         </is>
       </c>
-      <c r="N40" s="11" t="inlineStr">
+      <c r="N40" s="20" t="inlineStr">
         <is>
           <t>弘元绿能</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="19" t="inlineStr">
+      <c r="B41" s="20" t="inlineStr">
         <is>
           <t>合力科技</t>
         </is>
       </c>
-      <c r="C41" s="19" t="inlineStr">
+      <c r="C41" s="20" t="inlineStr">
         <is>
           <t>宏盛股份</t>
         </is>
       </c>
-      <c r="D41" s="19" t="inlineStr">
+      <c r="D41" s="20" t="inlineStr">
         <is>
           <t>长联科技</t>
         </is>
       </c>
-      <c r="E41" s="9" t="inlineStr">
+      <c r="E41" s="12" t="inlineStr">
         <is>
           <t>九鼎新材2</t>
         </is>
       </c>
-      <c r="F41" s="5" t="inlineStr">
+      <c r="F41" s="20" t="inlineStr">
         <is>
           <t>盛路通信</t>
         </is>
       </c>
-      <c r="G41" s="9" t="inlineStr">
+      <c r="G41" s="13" t="inlineStr">
         <is>
           <t>横店影视</t>
         </is>
       </c>
-      <c r="H41" s="12" t="inlineStr">
+      <c r="H41" s="5" t="inlineStr">
         <is>
           <t>翠微股份3</t>
         </is>
       </c>
-      <c r="I41" s="6" t="inlineStr">
+      <c r="I41" s="9" t="inlineStr">
         <is>
           <t>龙溪股份2</t>
         </is>
@@ -10281,7 +10287,7 @@
           <t>渝三峡A4</t>
         </is>
       </c>
-      <c r="L41" s="9" t="inlineStr">
+      <c r="L41" s="13" t="inlineStr">
         <is>
           <t>联合化学2</t>
         </is>
@@ -10291,7 +10297,7 @@
           <t>顾家家居</t>
         </is>
       </c>
-      <c r="N41" s="19" t="inlineStr">
+      <c r="N41" s="20" t="inlineStr">
         <is>
           <t>空港股份</t>
         </is>
@@ -10308,17 +10314,17 @@
           <t>浔兴股份5</t>
         </is>
       </c>
-      <c r="D42" s="19" t="inlineStr">
+      <c r="D42" s="14" t="inlineStr">
         <is>
           <t>慈文传媒</t>
         </is>
       </c>
-      <c r="E42" s="5" t="inlineStr">
+      <c r="E42" s="20" t="inlineStr">
         <is>
           <t>兴业股份</t>
         </is>
       </c>
-      <c r="F42" s="19" t="inlineStr">
+      <c r="F42" s="20" t="inlineStr">
         <is>
           <t>世嘉科技</t>
         </is>
@@ -10328,12 +10334,12 @@
           <t>灵康药业2</t>
         </is>
       </c>
-      <c r="H42" s="11" t="inlineStr">
+      <c r="H42" s="5" t="inlineStr">
         <is>
           <t>盈方微2</t>
         </is>
       </c>
-      <c r="I42" s="9" t="inlineStr">
+      <c r="I42" s="13" t="inlineStr">
         <is>
           <t>和科达2</t>
         </is>
@@ -10348,12 +10354,12 @@
           <t>三峡旅游2</t>
         </is>
       </c>
-      <c r="M42" s="19" t="inlineStr">
+      <c r="M42" s="20" t="inlineStr">
         <is>
           <t>宁波华翔</t>
         </is>
       </c>
-      <c r="N42" s="19" t="inlineStr">
+      <c r="N42" s="20" t="inlineStr">
         <is>
           <t>西上海</t>
         </is>
@@ -10370,17 +10376,17 @@
           <t>苏豪弘业</t>
         </is>
       </c>
-      <c r="D43" s="4" t="inlineStr">
+      <c r="D43" s="6" t="inlineStr">
         <is>
           <t>桂发祥2</t>
         </is>
       </c>
-      <c r="E43" s="11" t="inlineStr">
+      <c r="E43" s="8" t="inlineStr">
         <is>
           <t>三孚股份2</t>
         </is>
       </c>
-      <c r="F43" s="19" t="inlineStr">
+      <c r="F43" s="20" t="inlineStr">
         <is>
           <t>通宇通讯</t>
         </is>
@@ -10390,39 +10396,39 @@
           <t>安正时尚3</t>
         </is>
       </c>
-      <c r="H43" s="9" t="inlineStr">
+      <c r="H43" s="13" t="inlineStr">
         <is>
           <t>永鼎股份</t>
         </is>
       </c>
-      <c r="I43" s="19" t="inlineStr">
+      <c r="I43" s="9" t="inlineStr">
         <is>
           <t>兆威机电</t>
         </is>
       </c>
-      <c r="J43" s="19" t="inlineStr">
+      <c r="J43" s="20" t="inlineStr">
         <is>
           <t>上海凤凰</t>
         </is>
       </c>
-      <c r="K43" s="12" t="inlineStr">
+      <c r="K43" s="5" t="inlineStr">
         <is>
           <t>上海物贸2</t>
         </is>
       </c>
-      <c r="M43" s="7" t="inlineStr">
+      <c r="M43" s="9" t="inlineStr">
         <is>
           <t>全筑股份2</t>
         </is>
       </c>
-      <c r="N43" s="9" t="inlineStr">
+      <c r="N43" s="12" t="inlineStr">
         <is>
           <t>旺能环境</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="12" t="inlineStr">
+      <c r="B44" s="5" t="inlineStr">
         <is>
           <t>海陆重工3</t>
         </is>
@@ -10432,7 +10438,7 @@
           <t>瑞贝卡</t>
         </is>
       </c>
-      <c r="D44" s="11" t="inlineStr">
+      <c r="D44" s="8" t="inlineStr">
         <is>
           <t>渤海化学3</t>
         </is>
@@ -10447,44 +10453,44 @@
           <t>传艺科技</t>
         </is>
       </c>
-      <c r="G44" s="9" t="inlineStr">
+      <c r="G44" s="13" t="inlineStr">
         <is>
           <t>富春环保</t>
         </is>
       </c>
-      <c r="H44" s="19" t="inlineStr">
+      <c r="H44" s="20" t="inlineStr">
         <is>
           <t>海欣食品</t>
         </is>
       </c>
-      <c r="I44" s="7" t="inlineStr">
+      <c r="I44" s="9" t="inlineStr">
         <is>
           <t>东贝集团4</t>
         </is>
       </c>
-      <c r="J44" s="19" t="inlineStr">
+      <c r="J44" s="9" t="inlineStr">
         <is>
           <t>中广核技</t>
         </is>
       </c>
-      <c r="K44" s="19" t="inlineStr">
+      <c r="K44" s="12" t="inlineStr">
         <is>
           <t>长源电力</t>
         </is>
       </c>
-      <c r="M44" s="9" t="inlineStr">
+      <c r="M44" s="14" t="inlineStr">
         <is>
           <t>平治信息</t>
         </is>
       </c>
-      <c r="N44" s="19" t="inlineStr">
+      <c r="N44" s="20" t="inlineStr">
         <is>
           <t>韩建河山</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="19" t="inlineStr">
+      <c r="B45" s="20" t="inlineStr">
         <is>
           <t>康力源</t>
         </is>
@@ -10494,7 +10500,7 @@
           <t>久其软件2</t>
         </is>
       </c>
-      <c r="D45" s="12" t="inlineStr">
+      <c r="D45" s="5" t="inlineStr">
         <is>
           <t>盛泰集团2</t>
         </is>
@@ -10504,12 +10510,12 @@
           <t>宁波中百</t>
         </is>
       </c>
-      <c r="F45" s="19" t="inlineStr">
+      <c r="F45" s="20" t="inlineStr">
         <is>
           <t>同兴科技</t>
         </is>
       </c>
-      <c r="G45" s="9" t="inlineStr">
+      <c r="G45" s="14" t="inlineStr">
         <is>
           <t>大位科技2</t>
         </is>
@@ -10519,34 +10525,34 @@
           <t>珠江钢琴</t>
         </is>
       </c>
-      <c r="I45" s="19" t="inlineStr">
+      <c r="I45" s="20" t="inlineStr">
         <is>
           <t>中马传动</t>
         </is>
       </c>
-      <c r="J45" s="12" t="inlineStr">
+      <c r="J45" s="5" t="inlineStr">
         <is>
           <t>罗欣药业2</t>
         </is>
       </c>
-      <c r="K45" s="19" t="inlineStr">
+      <c r="K45" s="12" t="inlineStr">
         <is>
           <t>九洲集团</t>
         </is>
       </c>
-      <c r="M45" s="9" t="inlineStr">
+      <c r="M45" s="13" t="inlineStr">
         <is>
           <t>雅运股份</t>
         </is>
       </c>
-      <c r="N45" s="19" t="inlineStr">
+      <c r="N45" s="9" t="inlineStr">
         <is>
           <t>瑞芯微</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="9" t="inlineStr">
+      <c r="B46" s="13" t="inlineStr">
         <is>
           <t>思维列控</t>
         </is>
@@ -10556,17 +10562,17 @@
           <t>新华锦2</t>
         </is>
       </c>
-      <c r="D46" s="12" t="inlineStr">
+      <c r="D46" s="5" t="inlineStr">
         <is>
           <t>翠微股份3</t>
         </is>
       </c>
-      <c r="E46" s="12" t="inlineStr">
+      <c r="E46" s="5" t="inlineStr">
         <is>
           <t>莱绅通灵3</t>
         </is>
       </c>
-      <c r="F46" s="19" t="inlineStr">
+      <c r="F46" s="20" t="inlineStr">
         <is>
           <t>东方通信</t>
         </is>
@@ -10576,12 +10582,12 @@
           <t>生意宝4</t>
         </is>
       </c>
-      <c r="H46" s="19" t="inlineStr">
+      <c r="H46" s="20" t="inlineStr">
         <is>
           <t>吉大正元</t>
         </is>
       </c>
-      <c r="I46" s="4" t="inlineStr">
+      <c r="I46" s="9" t="inlineStr">
         <is>
           <t>红旗连锁</t>
         </is>
@@ -10591,7 +10597,7 @@
           <t>广西能源</t>
         </is>
       </c>
-      <c r="K46" s="5" t="inlineStr">
+      <c r="K46" s="20" t="inlineStr">
         <is>
           <t>天津普林</t>
         </is>
@@ -10601,7 +10607,7 @@
           <t>宁波东力3</t>
         </is>
       </c>
-      <c r="N46" s="19" t="inlineStr">
+      <c r="N46" s="9" t="inlineStr">
         <is>
           <t>精工科技</t>
         </is>
@@ -10618,12 +10624,12 @@
           <t>三态股份</t>
         </is>
       </c>
-      <c r="D47" s="19" t="inlineStr">
+      <c r="D47" s="14" t="inlineStr">
         <is>
           <t>创识科技</t>
         </is>
       </c>
-      <c r="E47" s="19" t="inlineStr">
+      <c r="E47" s="20" t="inlineStr">
         <is>
           <t>登云股份</t>
         </is>
@@ -10633,7 +10639,7 @@
           <t>永杰新材</t>
         </is>
       </c>
-      <c r="G47" s="12" t="inlineStr">
+      <c r="G47" s="5" t="inlineStr">
         <is>
           <t>海联金汇4</t>
         </is>
@@ -10643,7 +10649,7 @@
           <t>尖峰集团</t>
         </is>
       </c>
-      <c r="I47" s="12" t="inlineStr">
+      <c r="I47" s="5" t="inlineStr">
         <is>
           <t>神开股份2</t>
         </is>
@@ -10653,24 +10659,24 @@
           <t>久祺股份2</t>
         </is>
       </c>
-      <c r="K47" s="11" t="inlineStr">
+      <c r="K47" s="9" t="inlineStr">
         <is>
           <t>好上好</t>
         </is>
       </c>
-      <c r="M47" s="9" t="inlineStr">
+      <c r="M47" s="14" t="inlineStr">
         <is>
           <t>丸美生物</t>
         </is>
       </c>
-      <c r="N47" s="6" t="inlineStr">
+      <c r="N47" s="9" t="inlineStr">
         <is>
           <t>南京化纤</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="19" t="inlineStr">
+      <c r="B48" s="20" t="inlineStr">
         <is>
           <t>怡球资源</t>
         </is>
@@ -10685,64 +10691,64 @@
           <t>华软科技</t>
         </is>
       </c>
-      <c r="F48" s="12" t="inlineStr">
+      <c r="F48" s="14" t="inlineStr">
         <is>
           <t>朝阳科技2</t>
         </is>
       </c>
-      <c r="G48" s="11" t="inlineStr">
+      <c r="G48" s="20" t="inlineStr">
         <is>
           <t>立昂微</t>
         </is>
       </c>
-      <c r="H48" s="12" t="inlineStr">
+      <c r="H48" s="5" t="inlineStr">
         <is>
           <t>东方创业2</t>
         </is>
       </c>
-      <c r="I48" s="12" t="inlineStr">
+      <c r="I48" s="5" t="inlineStr">
         <is>
           <t>三维化学2</t>
         </is>
       </c>
-      <c r="J48" s="19" t="inlineStr">
+      <c r="J48" s="20" t="inlineStr">
         <is>
           <t>天元宠物</t>
         </is>
       </c>
-      <c r="K48" s="19" t="inlineStr">
+      <c r="K48" s="20" t="inlineStr">
         <is>
           <t>畅联股份</t>
         </is>
       </c>
-      <c r="M48" s="12" t="inlineStr">
+      <c r="M48" s="5" t="inlineStr">
         <is>
           <t>汉商集团2</t>
         </is>
       </c>
-      <c r="N48" s="19" t="inlineStr">
+      <c r="N48" s="14" t="inlineStr">
         <is>
           <t>中光学</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="B49" s="6" t="inlineStr">
+      <c r="B49" s="9" t="inlineStr">
         <is>
           <t>云内动力</t>
         </is>
       </c>
-      <c r="C49" s="12" t="inlineStr">
+      <c r="C49" s="5" t="inlineStr">
         <is>
           <t>东方材料3</t>
         </is>
       </c>
-      <c r="E49" s="9" t="inlineStr">
+      <c r="E49" s="13" t="inlineStr">
         <is>
           <t>拓维信息2</t>
         </is>
       </c>
-      <c r="F49" s="19" t="inlineStr">
+      <c r="F49" s="20" t="inlineStr">
         <is>
           <t>华锋股份</t>
         </is>
@@ -10752,39 +10758,39 @@
           <t>拉芳家化</t>
         </is>
       </c>
-      <c r="H49" s="19" t="inlineStr">
+      <c r="H49" s="20" t="inlineStr">
         <is>
           <t>中油资本</t>
         </is>
       </c>
-      <c r="I49" s="19" t="inlineStr">
+      <c r="I49" s="9" t="inlineStr">
         <is>
           <t>美湖股份</t>
         </is>
       </c>
-      <c r="J49" s="9" t="inlineStr">
+      <c r="J49" s="13" t="inlineStr">
         <is>
           <t>依依股份</t>
         </is>
       </c>
-      <c r="K49" s="19" t="inlineStr">
+      <c r="K49" s="9" t="inlineStr">
         <is>
           <t>南方路机</t>
         </is>
       </c>
-      <c r="M49" s="9" t="inlineStr">
+      <c r="M49" s="13" t="inlineStr">
         <is>
           <t>百润股份</t>
         </is>
       </c>
-      <c r="N49" s="9" t="inlineStr">
+      <c r="N49" s="12" t="inlineStr">
         <is>
           <t>新联电子</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="19" t="inlineStr">
+      <c r="B50" s="14" t="inlineStr">
         <is>
           <t>比依股份</t>
         </is>
@@ -10794,12 +10800,12 @@
           <t>永泰运2</t>
         </is>
       </c>
-      <c r="E50" s="19" t="inlineStr">
+      <c r="E50" s="20" t="inlineStr">
         <is>
           <t>惠发食品</t>
         </is>
       </c>
-      <c r="F50" s="12" t="inlineStr">
+      <c r="F50" s="5" t="inlineStr">
         <is>
           <t>仁智股份2</t>
         </is>
@@ -10809,12 +10815,12 @@
           <t>有友食品2</t>
         </is>
       </c>
-      <c r="H50" s="7" t="inlineStr">
+      <c r="H50" s="6" t="inlineStr">
         <is>
           <t>轻纺城2</t>
         </is>
       </c>
-      <c r="I50" s="9" t="inlineStr">
+      <c r="I50" s="13" t="inlineStr">
         <is>
           <t>龙江交通</t>
         </is>
@@ -10824,17 +10830,17 @@
           <t>韶能股份4</t>
         </is>
       </c>
-      <c r="K50" s="9" t="inlineStr">
+      <c r="K50" s="13" t="inlineStr">
         <is>
           <t>拓维信息2</t>
         </is>
       </c>
-      <c r="M50" s="9" t="inlineStr">
+      <c r="M50" s="13" t="inlineStr">
         <is>
           <t>梦百合</t>
         </is>
       </c>
-      <c r="N50" s="4" t="inlineStr">
+      <c r="N50" s="9" t="inlineStr">
         <is>
           <t>光大同创</t>
         </is>
@@ -10846,7 +10852,7 @@
           <t>乐山电力7</t>
         </is>
       </c>
-      <c r="C51" s="12" t="inlineStr">
+      <c r="C51" s="9" t="inlineStr">
         <is>
           <t>南方精工3</t>
         </is>
@@ -10856,7 +10862,7 @@
           <t>泰嘉股份2</t>
         </is>
       </c>
-      <c r="F51" s="19" t="inlineStr">
+      <c r="F51" s="20" t="inlineStr">
         <is>
           <t>金融街</t>
         </is>
@@ -10871,17 +10877,17 @@
           <t>星湖科技</t>
         </is>
       </c>
-      <c r="I51" s="19" t="inlineStr">
+      <c r="I51" s="9" t="inlineStr">
         <is>
           <t>长华集团</t>
         </is>
       </c>
-      <c r="J51" s="11" t="inlineStr">
+      <c r="J51" s="8" t="inlineStr">
         <is>
           <t>渤海化学3</t>
         </is>
       </c>
-      <c r="K51" s="9" t="inlineStr">
+      <c r="K51" s="13" t="inlineStr">
         <is>
           <t>甘李药业</t>
         </is>
@@ -10891,34 +10897,34 @@
           <t>吉华集团</t>
         </is>
       </c>
-      <c r="N51" s="19" t="inlineStr">
+      <c r="N51" s="20" t="inlineStr">
         <is>
           <t>天普股份</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="B52" s="12" t="inlineStr">
+      <c r="B52" s="5" t="inlineStr">
         <is>
           <t>荣丰控股3</t>
         </is>
       </c>
-      <c r="C52" s="12" t="inlineStr">
+      <c r="C52" s="14" t="inlineStr">
         <is>
           <t>东珠生态6</t>
         </is>
       </c>
-      <c r="E52" s="19" t="inlineStr">
+      <c r="E52" s="20" t="inlineStr">
         <is>
           <t>益佰制药</t>
         </is>
       </c>
-      <c r="F52" s="19" t="inlineStr">
+      <c r="F52" s="20" t="inlineStr">
         <is>
           <t>国中水务</t>
         </is>
       </c>
-      <c r="G52" s="12" t="inlineStr">
+      <c r="G52" s="14" t="inlineStr">
         <is>
           <t>信雅达2</t>
         </is>
@@ -10928,7 +10934,7 @@
           <t>洪兴股份2</t>
         </is>
       </c>
-      <c r="I52" s="19" t="inlineStr">
+      <c r="I52" s="9" t="inlineStr">
         <is>
           <t>肇民科技</t>
         </is>
@@ -10938,7 +10944,7 @@
           <t>宁波联合2</t>
         </is>
       </c>
-      <c r="K52" s="5" t="inlineStr">
+      <c r="K52" s="12" t="inlineStr">
         <is>
           <t>泰豪科技2</t>
         </is>
@@ -10955,12 +10961,12 @@
       </c>
     </row>
     <row r="53">
-      <c r="B53" s="19" t="inlineStr">
+      <c r="B53" s="20" t="inlineStr">
         <is>
           <t>雪人股份</t>
         </is>
       </c>
-      <c r="C53" s="19" t="inlineStr">
+      <c r="C53" s="20" t="inlineStr">
         <is>
           <t>长鸿高科</t>
         </is>
@@ -10970,12 +10976,12 @@
           <t>红蜻蜓2</t>
         </is>
       </c>
-      <c r="F53" s="11" t="inlineStr">
+      <c r="F53" s="20" t="inlineStr">
         <is>
           <t>高新发展</t>
         </is>
       </c>
-      <c r="G53" s="12" t="inlineStr">
+      <c r="G53" s="5" t="inlineStr">
         <is>
           <t>青岛金王3</t>
         </is>
@@ -10985,7 +10991,7 @@
           <t>赤天化</t>
         </is>
       </c>
-      <c r="I53" s="9" t="inlineStr">
+      <c r="I53" s="13" t="inlineStr">
         <is>
           <t>恒勃股份</t>
         </is>
@@ -10995,24 +11001,24 @@
           <t>新瀚新材2</t>
         </is>
       </c>
-      <c r="K53" s="9" t="inlineStr">
+      <c r="K53" s="13" t="inlineStr">
         <is>
           <t>百龙创园</t>
         </is>
       </c>
-      <c r="M53" s="9" t="inlineStr">
+      <c r="M53" s="14" t="inlineStr">
         <is>
           <t>美利云</t>
         </is>
       </c>
-      <c r="N53" s="19" t="inlineStr">
+      <c r="N53" s="9" t="inlineStr">
         <is>
           <t>福达股份</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="19" t="inlineStr">
+      <c r="B54" s="20" t="inlineStr">
         <is>
           <t>动力新科</t>
         </is>
@@ -11022,7 +11028,7 @@
           <t>西王食品2</t>
         </is>
       </c>
-      <c r="E54" s="19" t="inlineStr">
+      <c r="E54" s="14" t="inlineStr">
         <is>
           <t>泛微网络</t>
         </is>
@@ -11037,34 +11043,34 @@
           <t>阳光乳业</t>
         </is>
       </c>
-      <c r="H54" s="12" t="inlineStr">
+      <c r="H54" s="5" t="inlineStr">
         <is>
           <t>圣龙股份2</t>
         </is>
       </c>
-      <c r="I54" s="19" t="inlineStr">
+      <c r="I54" s="20" t="inlineStr">
         <is>
           <t>吉林化纤</t>
         </is>
       </c>
-      <c r="K54" s="9" t="inlineStr">
+      <c r="K54" s="13" t="inlineStr">
         <is>
           <t>会稽山2</t>
         </is>
       </c>
-      <c r="M54" s="11" t="inlineStr">
+      <c r="M54" s="5" t="inlineStr">
         <is>
           <t>中旗新材4</t>
         </is>
       </c>
-      <c r="N54" s="19" t="inlineStr">
+      <c r="N54" s="20" t="inlineStr">
         <is>
           <t>华夏幸福</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="B55" s="19" t="inlineStr">
+      <c r="B55" s="20" t="inlineStr">
         <is>
           <t>安源煤业</t>
         </is>
@@ -11079,27 +11085,27 @@
           <t>沃顿科技</t>
         </is>
       </c>
-      <c r="F55" s="19" t="inlineStr">
+      <c r="F55" s="20" t="inlineStr">
         <is>
           <t>我爱我家</t>
         </is>
       </c>
-      <c r="G55" s="11" t="inlineStr">
+      <c r="G55" s="20" t="inlineStr">
         <is>
           <t>至正股份</t>
         </is>
       </c>
-      <c r="H55" s="19" t="inlineStr">
+      <c r="H55" s="9" t="inlineStr">
         <is>
           <t>奇德新材</t>
         </is>
       </c>
-      <c r="I55" s="12" t="inlineStr">
+      <c r="I55" s="5" t="inlineStr">
         <is>
           <t>棒杰股份2</t>
         </is>
       </c>
-      <c r="K55" s="6" t="inlineStr">
+      <c r="K55" s="9" t="inlineStr">
         <is>
           <t>赛福天</t>
         </is>
@@ -11109,14 +11115,14 @@
           <t>大叶股份</t>
         </is>
       </c>
-      <c r="N55" s="19" t="inlineStr">
+      <c r="N55" s="20" t="inlineStr">
         <is>
           <t>湖北广电</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="B56" s="19" t="inlineStr">
+      <c r="B56" s="20" t="inlineStr">
         <is>
           <t>金陵体育</t>
         </is>
@@ -11126,12 +11132,12 @@
           <t>西昌电力4</t>
         </is>
       </c>
-      <c r="E56" s="12" t="inlineStr">
+      <c r="E56" s="5" t="inlineStr">
         <is>
           <t>宏昌电子2</t>
         </is>
       </c>
-      <c r="F56" s="19" t="inlineStr">
+      <c r="F56" s="20" t="inlineStr">
         <is>
           <t>新城市</t>
         </is>
@@ -11141,17 +11147,17 @@
           <t>祖名股份</t>
         </is>
       </c>
-      <c r="H56" s="19" t="inlineStr">
+      <c r="H56" s="20" t="inlineStr">
         <is>
           <t>中农联合</t>
         </is>
       </c>
-      <c r="I56" s="9" t="inlineStr">
+      <c r="I56" s="12" t="inlineStr">
         <is>
           <t>长城科技</t>
         </is>
       </c>
-      <c r="K56" s="19" t="inlineStr">
+      <c r="K56" s="20" t="inlineStr">
         <is>
           <t>我乐家居</t>
         </is>
@@ -11161,24 +11167,24 @@
           <t>兆丰股份</t>
         </is>
       </c>
-      <c r="N56" s="6" t="inlineStr">
+      <c r="N56" s="9" t="inlineStr">
         <is>
           <t>龙溪股份2</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="B57" s="12" t="inlineStr">
+      <c r="B57" s="5" t="inlineStr">
         <is>
           <t>天府文旅2</t>
         </is>
       </c>
-      <c r="C57" s="19" t="inlineStr">
+      <c r="C57" s="20" t="inlineStr">
         <is>
           <t>新亚电缆</t>
         </is>
       </c>
-      <c r="E57" s="19" t="inlineStr">
+      <c r="E57" s="20" t="inlineStr">
         <is>
           <t>德才股份</t>
         </is>
@@ -11188,17 +11194,17 @@
           <t>黑牡丹</t>
         </is>
       </c>
-      <c r="G57" s="5" t="inlineStr">
+      <c r="G57" s="20" t="inlineStr">
         <is>
           <t>国睿科技</t>
         </is>
       </c>
-      <c r="H57" s="19" t="inlineStr">
+      <c r="H57" s="20" t="inlineStr">
         <is>
           <t>天鹅股份</t>
         </is>
       </c>
-      <c r="I57" s="12" t="inlineStr">
+      <c r="I57" s="5" t="inlineStr">
         <is>
           <t>海陆重工3</t>
         </is>
@@ -11213,14 +11219,14 @@
           <t>金鸿顺2</t>
         </is>
       </c>
-      <c r="N57" s="19" t="inlineStr">
+      <c r="N57" s="9" t="inlineStr">
         <is>
           <t>宏昌科技</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="B58" s="19" t="inlineStr">
+      <c r="B58" s="20" t="inlineStr">
         <is>
           <t>君禾股份</t>
         </is>
@@ -11230,7 +11236,7 @@
           <t>赣能股份</t>
         </is>
       </c>
-      <c r="E58" s="12" t="inlineStr">
+      <c r="E58" s="5" t="inlineStr">
         <is>
           <t>海陆重工3</t>
         </is>
@@ -11240,49 +11246,49 @@
           <t>源飞宠物</t>
         </is>
       </c>
-      <c r="H58" s="19" t="inlineStr">
+      <c r="H58" s="20" t="inlineStr">
         <is>
           <t>美邦股份</t>
         </is>
       </c>
-      <c r="I58" s="19" t="inlineStr">
+      <c r="I58" s="20" t="inlineStr">
         <is>
           <t>合众思壮</t>
         </is>
       </c>
-      <c r="K58" s="19" t="inlineStr">
+      <c r="K58" s="9" t="inlineStr">
         <is>
           <t>夏厦精密</t>
         </is>
       </c>
-      <c r="M58" s="9" t="inlineStr">
+      <c r="M58" s="13" t="inlineStr">
         <is>
           <t>闰土股份</t>
         </is>
       </c>
-      <c r="N58" s="9" t="inlineStr">
+      <c r="N58" s="13" t="inlineStr">
         <is>
           <t>炜冈科技</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="B59" s="19" t="inlineStr">
+      <c r="B59" s="20" t="inlineStr">
         <is>
           <t>大悦城</t>
         </is>
       </c>
-      <c r="C59" s="9" t="inlineStr">
+      <c r="C59" s="14" t="inlineStr">
         <is>
           <t>正和生态2</t>
         </is>
       </c>
-      <c r="E59" s="19" t="inlineStr">
+      <c r="E59" s="14" t="inlineStr">
         <is>
           <t>广联达</t>
         </is>
       </c>
-      <c r="G59" s="19" t="inlineStr">
+      <c r="G59" s="20" t="inlineStr">
         <is>
           <t>潮宏基</t>
         </is>
@@ -11292,44 +11298,44 @@
           <t>宝鼎科技</t>
         </is>
       </c>
-      <c r="I59" s="19" t="inlineStr">
+      <c r="I59" s="20" t="inlineStr">
         <is>
           <t>万丰奥威</t>
         </is>
       </c>
-      <c r="K59" s="19" t="inlineStr">
+      <c r="K59" s="20" t="inlineStr">
         <is>
           <t>博菲电气</t>
         </is>
       </c>
-      <c r="M59" s="19" t="inlineStr">
+      <c r="M59" s="14" t="inlineStr">
         <is>
           <t>兆易创新</t>
         </is>
       </c>
-      <c r="N59" s="19" t="inlineStr">
+      <c r="N59" s="9" t="inlineStr">
         <is>
           <t>祥鑫科技</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="B60" s="19" t="inlineStr">
+      <c r="B60" s="20" t="inlineStr">
         <is>
           <t>东诚药业</t>
         </is>
       </c>
-      <c r="E60" s="19" t="inlineStr">
+      <c r="E60" s="14" t="inlineStr">
         <is>
           <t>尚品宅配</t>
         </is>
       </c>
-      <c r="G60" s="19" t="inlineStr">
+      <c r="G60" s="20" t="inlineStr">
         <is>
           <t>舒泰神</t>
         </is>
       </c>
-      <c r="H60" s="12" t="inlineStr">
+      <c r="H60" s="5" t="inlineStr">
         <is>
           <t>深中华A2</t>
         </is>
@@ -11339,7 +11345,7 @@
           <t>德美化工</t>
         </is>
       </c>
-      <c r="K60" s="9" t="inlineStr">
+      <c r="K60" s="13" t="inlineStr">
         <is>
           <t>全新好</t>
         </is>
@@ -11351,7 +11357,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="B61" s="19" t="inlineStr">
+      <c r="B61" s="20" t="inlineStr">
         <is>
           <t>中洲特材</t>
         </is>
@@ -11366,7 +11372,7 @@
           <t>贝仕达克</t>
         </is>
       </c>
-      <c r="H61" s="19" t="inlineStr">
+      <c r="H61" s="20" t="inlineStr">
         <is>
           <t>东江环保</t>
         </is>
@@ -11376,12 +11382,12 @@
           <t>嵘泰股份2</t>
         </is>
       </c>
-      <c r="K61" s="19" t="inlineStr">
+      <c r="K61" s="20" t="inlineStr">
         <is>
           <t>黑猫股份</t>
         </is>
       </c>
-      <c r="N61" s="12" t="inlineStr">
+      <c r="N61" s="9" t="inlineStr">
         <is>
           <t>南方精工3</t>
         </is>
@@ -11398,17 +11404,17 @@
           <t>志邦家居</t>
         </is>
       </c>
-      <c r="G62" s="9" t="inlineStr">
+      <c r="G62" s="13" t="inlineStr">
         <is>
           <t>长青股份</t>
         </is>
       </c>
-      <c r="H62" s="19" t="inlineStr">
+      <c r="H62" s="20" t="inlineStr">
         <is>
           <t>振华股份</t>
         </is>
       </c>
-      <c r="K62" s="11" t="inlineStr">
+      <c r="K62" s="12" t="inlineStr">
         <is>
           <t>智光电气</t>
         </is>
@@ -11420,22 +11426,22 @@
       </c>
     </row>
     <row r="63">
-      <c r="B63" s="6" t="inlineStr">
+      <c r="B63" s="9" t="inlineStr">
         <is>
           <t>赛摩智能</t>
         </is>
       </c>
-      <c r="E63" s="7" t="inlineStr">
+      <c r="E63" s="4" t="inlineStr">
         <is>
           <t>五芳斋2</t>
         </is>
       </c>
-      <c r="G63" s="19" t="inlineStr">
+      <c r="G63" s="20" t="inlineStr">
         <is>
           <t>宏和科技</t>
         </is>
       </c>
-      <c r="H63" s="19" t="inlineStr">
+      <c r="H63" s="20" t="inlineStr">
         <is>
           <t>凯美特气</t>
         </is>
@@ -11445,34 +11451,34 @@
           <t>明星电力</t>
         </is>
       </c>
-      <c r="N63" s="11" t="inlineStr">
+      <c r="N63" s="20" t="inlineStr">
         <is>
           <t>兴森科技</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="B64" s="19" t="inlineStr">
+      <c r="B64" s="20" t="inlineStr">
         <is>
           <t>威尔泰</t>
         </is>
       </c>
-      <c r="E64" s="12" t="inlineStr">
+      <c r="E64" s="5" t="inlineStr">
         <is>
           <t>重庆建工3</t>
         </is>
       </c>
-      <c r="G64" s="19" t="inlineStr">
+      <c r="G64" s="20" t="inlineStr">
         <is>
           <t>哈药股份</t>
         </is>
       </c>
-      <c r="H64" s="19" t="inlineStr">
+      <c r="H64" s="20" t="inlineStr">
         <is>
           <t>东峰集团</t>
         </is>
       </c>
-      <c r="K64" s="9" t="inlineStr">
+      <c r="K64" s="12" t="inlineStr">
         <is>
           <t>湖南发展</t>
         </is>
@@ -11489,27 +11495,27 @@
           <t>齐心集团</t>
         </is>
       </c>
-      <c r="E65" s="5" t="inlineStr">
+      <c r="E65" s="14" t="inlineStr">
         <is>
           <t>润贝航科5</t>
         </is>
       </c>
-      <c r="G65" s="11" t="inlineStr">
+      <c r="G65" s="13" t="inlineStr">
         <is>
           <t>晓程科技</t>
         </is>
       </c>
-      <c r="H65" s="19" t="inlineStr">
+      <c r="H65" s="20" t="inlineStr">
         <is>
           <t>凯盛新能</t>
         </is>
       </c>
-      <c r="K65" s="5" t="inlineStr">
+      <c r="K65" s="9" t="inlineStr">
         <is>
           <t>大立科技</t>
         </is>
       </c>
-      <c r="N65" s="9" t="inlineStr">
+      <c r="N65" s="13" t="inlineStr">
         <is>
           <t>科伦药业</t>
         </is>
@@ -11521,29 +11527,29 @@
           <t>茂业商业5</t>
         </is>
       </c>
-      <c r="E66" s="12" t="inlineStr">
+      <c r="E66" s="5" t="inlineStr">
         <is>
           <t>格林达2</t>
         </is>
       </c>
-      <c r="G66" s="12" t="inlineStr">
+      <c r="G66" s="5" t="inlineStr">
         <is>
           <t>顺灏股份2</t>
         </is>
       </c>
-      <c r="H66" s="7" t="inlineStr">
+      <c r="H66" s="4" t="inlineStr">
         <is>
           <t>煌上煌</t>
         </is>
       </c>
-      <c r="N66" s="12" t="inlineStr">
+      <c r="N66" s="5" t="inlineStr">
         <is>
           <t>松炀资源2</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="B67" s="5" t="inlineStr">
+      <c r="B67" s="12" t="inlineStr">
         <is>
           <t>凤形股份</t>
         </is>
@@ -11558,12 +11564,12 @@
           <t>品渥食品</t>
         </is>
       </c>
-      <c r="H67" s="12" t="inlineStr">
+      <c r="H67" s="5" t="inlineStr">
         <is>
           <t>西陇科学3</t>
         </is>
       </c>
-      <c r="N67" s="12" t="inlineStr">
+      <c r="N67" s="5" t="inlineStr">
         <is>
           <t>威领股份2</t>
         </is>
@@ -11590,14 +11596,14 @@
           <t>三峡旅游2</t>
         </is>
       </c>
-      <c r="N68" s="19" t="inlineStr">
+      <c r="N68" s="9" t="inlineStr">
         <is>
           <t>信质集团</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="B69" s="19" t="inlineStr">
+      <c r="B69" s="20" t="inlineStr">
         <is>
           <t>华钰矿业</t>
         </is>
@@ -11607,7 +11613,7 @@
           <t>尤夫股份5</t>
         </is>
       </c>
-      <c r="G69" s="12" t="inlineStr">
+      <c r="G69" s="14" t="inlineStr">
         <is>
           <t>利欧股份2</t>
         </is>
@@ -11617,51 +11623,51 @@
           <t>卫信康</t>
         </is>
       </c>
-      <c r="N69" s="9" t="inlineStr">
+      <c r="N69" s="12" t="inlineStr">
         <is>
           <t>八方股份</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="B70" s="9" t="inlineStr">
+      <c r="B70" s="13" t="inlineStr">
         <is>
           <t>湖南黄金2</t>
         </is>
       </c>
-      <c r="E70" s="19" t="inlineStr">
+      <c r="E70" s="20" t="inlineStr">
         <is>
           <t>中天服务</t>
         </is>
       </c>
-      <c r="G70" s="19" t="inlineStr">
+      <c r="G70" s="20" t="inlineStr">
         <is>
           <t>金桥信息</t>
         </is>
       </c>
-      <c r="H70" s="9" t="inlineStr">
+      <c r="H70" s="8" t="inlineStr">
         <is>
           <t>富士莱</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="B71" s="19" t="inlineStr">
+      <c r="B71" s="20" t="inlineStr">
         <is>
           <t>汇成真空</t>
         </is>
       </c>
-      <c r="E71" s="19" t="inlineStr">
+      <c r="E71" s="20" t="inlineStr">
         <is>
           <t>亚振家居</t>
         </is>
       </c>
-      <c r="G71" s="19" t="inlineStr">
+      <c r="G71" s="20" t="inlineStr">
         <is>
           <t>艾布鲁</t>
         </is>
       </c>
-      <c r="H71" s="19" t="inlineStr">
+      <c r="H71" s="20" t="inlineStr">
         <is>
           <t>华森制药</t>
         </is>
@@ -11673,24 +11679,24 @@
           <t>华锡有色</t>
         </is>
       </c>
-      <c r="E72" s="19" t="inlineStr">
+      <c r="E72" s="14" t="inlineStr">
         <is>
           <t>德必集团</t>
         </is>
       </c>
-      <c r="G72" s="12" t="inlineStr">
+      <c r="G72" s="5" t="inlineStr">
         <is>
           <t>好想你2</t>
         </is>
       </c>
-      <c r="H72" s="19" t="inlineStr">
+      <c r="H72" s="20" t="inlineStr">
         <is>
           <t>众生药业</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="B73" s="19" t="inlineStr">
+      <c r="B73" s="9" t="inlineStr">
         <is>
           <t>天和磁材</t>
         </is>
@@ -11700,7 +11706,7 @@
           <t>丽人丽妆</t>
         </is>
       </c>
-      <c r="G73" s="9" t="inlineStr">
+      <c r="G73" s="13" t="inlineStr">
         <is>
           <t>先达股份5</t>
         </is>
@@ -11712,34 +11718,34 @@
       </c>
     </row>
     <row r="74">
-      <c r="B74" s="19" t="inlineStr">
+      <c r="B74" s="20" t="inlineStr">
         <is>
           <t>康惠制药</t>
         </is>
       </c>
-      <c r="E74" s="19" t="inlineStr">
+      <c r="E74" s="20" t="inlineStr">
         <is>
           <t>税友股份</t>
         </is>
       </c>
-      <c r="G74" s="9" t="inlineStr">
+      <c r="G74" s="13" t="inlineStr">
         <is>
           <t>金杯汽车</t>
         </is>
       </c>
-      <c r="H74" s="19" t="inlineStr">
+      <c r="H74" s="20" t="inlineStr">
         <is>
           <t>中储股份</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="B75" s="19" t="inlineStr">
+      <c r="B75" s="12" t="inlineStr">
         <is>
           <t>江苏新能</t>
         </is>
       </c>
-      <c r="E75" s="19" t="inlineStr">
+      <c r="E75" s="20" t="inlineStr">
         <is>
           <t>淮河能源</t>
         </is>
@@ -11749,7 +11755,7 @@
           <t>远大控股2</t>
         </is>
       </c>
-      <c r="H75" s="12" t="inlineStr">
+      <c r="H75" s="5" t="inlineStr">
         <is>
           <t>重庆建工3</t>
         </is>
@@ -11761,56 +11767,56 @@
           <t>海汽集团</t>
         </is>
       </c>
-      <c r="E76" s="19" t="inlineStr">
+      <c r="E76" s="14" t="inlineStr">
         <is>
           <t>电声股份</t>
         </is>
       </c>
-      <c r="G76" s="19" t="inlineStr">
+      <c r="G76" s="20" t="inlineStr">
         <is>
           <t>永和智控</t>
         </is>
       </c>
-      <c r="H76" s="7" t="inlineStr">
+      <c r="H76" s="6" t="inlineStr">
         <is>
           <t>丽尚国潮</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="B77" s="19" t="inlineStr">
+      <c r="B77" s="20" t="inlineStr">
         <is>
           <t>佳隆股份</t>
         </is>
       </c>
-      <c r="E77" s="7" t="inlineStr">
+      <c r="E77" s="6" t="inlineStr">
         <is>
           <t>华纺股份</t>
         </is>
       </c>
-      <c r="G77" s="19" t="inlineStr">
+      <c r="G77" s="20" t="inlineStr">
         <is>
           <t>康弘药业</t>
         </is>
       </c>
-      <c r="H77" s="5" t="inlineStr">
+      <c r="H77" s="20" t="inlineStr">
         <is>
           <t>航天晨光</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="B78" s="19" t="inlineStr">
+      <c r="B78" s="20" t="inlineStr">
         <is>
           <t>大有能源</t>
         </is>
       </c>
-      <c r="E78" s="12" t="inlineStr">
+      <c r="E78" s="5" t="inlineStr">
         <is>
           <t>中铝国际2</t>
         </is>
       </c>
-      <c r="G78" s="4" t="inlineStr">
+      <c r="G78" s="9" t="inlineStr">
         <is>
           <t>福莱新材</t>
         </is>
@@ -11822,17 +11828,17 @@
       </c>
     </row>
     <row r="79">
-      <c r="B79" s="19" t="inlineStr">
+      <c r="B79" s="20" t="inlineStr">
         <is>
           <t>海德股份</t>
         </is>
       </c>
-      <c r="E79" s="5" t="inlineStr">
+      <c r="E79" s="20" t="inlineStr">
         <is>
           <t>北摩高科</t>
         </is>
       </c>
-      <c r="G79" s="12" t="inlineStr">
+      <c r="G79" s="14" t="inlineStr">
         <is>
           <t>恒锋信息2</t>
         </is>
@@ -11854,12 +11860,12 @@
           <t>石基信息2</t>
         </is>
       </c>
-      <c r="G80" s="12" t="inlineStr">
+      <c r="G80" s="9" t="inlineStr">
         <is>
           <t>浙江荣泰3</t>
         </is>
       </c>
-      <c r="H80" s="19" t="inlineStr">
+      <c r="H80" s="20" t="inlineStr">
         <is>
           <t>润阳科技</t>
         </is>
@@ -11876,24 +11882,24 @@
           <t>保税科技4</t>
         </is>
       </c>
-      <c r="G81" s="19" t="inlineStr">
+      <c r="G81" s="20" t="inlineStr">
         <is>
           <t>澳洋健康</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="B82" s="5" t="inlineStr">
+      <c r="B82" s="12" t="inlineStr">
         <is>
           <t>泰豪科技2</t>
         </is>
       </c>
-      <c r="E82" s="19" t="inlineStr">
+      <c r="E82" s="20" t="inlineStr">
         <is>
           <t>一鸣食品</t>
         </is>
       </c>
-      <c r="G82" s="19" t="inlineStr">
+      <c r="G82" s="20" t="inlineStr">
         <is>
           <t>安妮股份</t>
         </is>
@@ -11910,19 +11916,19 @@
           <t>中锐股份</t>
         </is>
       </c>
-      <c r="G83" s="19" t="inlineStr">
+      <c r="G83" s="20" t="inlineStr">
         <is>
           <t>赤峰黄金</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="B84" s="19" t="inlineStr">
+      <c r="B84" s="20" t="inlineStr">
         <is>
           <t>海南椰岛</t>
         </is>
       </c>
-      <c r="E84" s="7" t="inlineStr">
+      <c r="E84" s="4" t="inlineStr">
         <is>
           <t>南极电商2</t>
         </is>
@@ -11934,12 +11940,12 @@
       </c>
     </row>
     <row r="85">
-      <c r="B85" s="19" t="inlineStr">
+      <c r="B85" s="20" t="inlineStr">
         <is>
           <t>海马汽车</t>
         </is>
       </c>
-      <c r="E85" s="19" t="inlineStr">
+      <c r="E85" s="9" t="inlineStr">
         <is>
           <t>南都物业</t>
         </is>
@@ -11956,7 +11962,7 @@
           <t>海南发展</t>
         </is>
       </c>
-      <c r="E86" s="19" t="inlineStr">
+      <c r="E86" s="20" t="inlineStr">
         <is>
           <t>益盛药业</t>
         </is>
@@ -11968,48 +11974,48 @@
       </c>
     </row>
     <row r="87">
-      <c r="B87" s="19" t="inlineStr">
+      <c r="B87" s="20" t="inlineStr">
         <is>
           <t>富岭股份</t>
         </is>
       </c>
-      <c r="E87" s="19" t="inlineStr">
+      <c r="E87" s="20" t="inlineStr">
         <is>
           <t>恒基达鑫</t>
         </is>
       </c>
-      <c r="G87" s="9" t="inlineStr">
+      <c r="G87" s="13" t="inlineStr">
         <is>
           <t>百亚股份</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="B88" s="19" t="inlineStr">
+      <c r="B88" s="20" t="inlineStr">
         <is>
           <t>葫芦娃</t>
         </is>
       </c>
-      <c r="G88" s="19" t="inlineStr">
+      <c r="G88" s="20" t="inlineStr">
         <is>
           <t>岳阳林纸</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="B89" s="12" t="inlineStr">
+      <c r="B89" s="5" t="inlineStr">
         <is>
           <t>格林达2</t>
         </is>
       </c>
-      <c r="G89" s="19" t="inlineStr">
+      <c r="G89" s="20" t="inlineStr">
         <is>
           <t>应流股份</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="B90" s="12" t="inlineStr">
+      <c r="B90" s="5" t="inlineStr">
         <is>
           <t>松炀资源2</t>
         </is>
@@ -12021,7 +12027,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="B91" s="9" t="inlineStr">
+      <c r="B91" s="13" t="inlineStr">
         <is>
           <t>隆鑫通用</t>
         </is>
@@ -12038,7 +12044,7 @@
           <t>川润股份2</t>
         </is>
       </c>
-      <c r="G92" s="19" t="inlineStr">
+      <c r="G92" s="14" t="inlineStr">
         <is>
           <t>润建股份</t>
         </is>
@@ -12057,55 +12063,55 @@
       </c>
     </row>
     <row r="94">
-      <c r="B94" s="19" t="inlineStr">
+      <c r="B94" s="20" t="inlineStr">
         <is>
           <t>远达环保</t>
         </is>
       </c>
-      <c r="G94" s="12" t="inlineStr">
+      <c r="G94" s="5" t="inlineStr">
         <is>
           <t>永安药业5</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="B95" s="11" t="inlineStr">
+      <c r="B95" s="13" t="inlineStr">
         <is>
           <t>汇通能源</t>
         </is>
       </c>
-      <c r="G95" s="12" t="inlineStr">
+      <c r="G95" s="5" t="inlineStr">
         <is>
           <t>三房巷2</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="B96" s="19" t="inlineStr">
+      <c r="B96" s="20" t="inlineStr">
         <is>
           <t>百隆东方</t>
         </is>
       </c>
-      <c r="G96" s="19" t="inlineStr">
+      <c r="G96" s="20" t="inlineStr">
         <is>
           <t>日出东方</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="B97" s="12" t="inlineStr">
+      <c r="B97" s="5" t="inlineStr">
         <is>
           <t>九鼎投资2</t>
         </is>
       </c>
-      <c r="G97" s="9" t="inlineStr">
+      <c r="G97" s="13" t="inlineStr">
         <is>
           <t>湖南黄金2</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="B98" s="19" t="inlineStr">
+      <c r="B98" s="20" t="inlineStr">
         <is>
           <t>天晟新材</t>
         </is>
@@ -12117,7 +12123,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="B99" s="9" t="inlineStr">
+      <c r="B99" s="13" t="inlineStr">
         <is>
           <t>联合化学2</t>
         </is>

</xml_diff>

<commit_message>
rerun datas and fix bug
</commit_message>
<xml_diff>
--- a/excel/fupan_analysis.xlsx
+++ b/excel/fupan_analysis.xlsx
@@ -239,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -247,7 +247,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -583,8 +583,8 @@
       <text>
         <t xml:space="preserve">11天7板 14:45:22 1
 AI文创+电影《731》+广播电视+卫星数据云服务
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -603,8 +603,8 @@
       <text>
         <t xml:space="preserve">13天7板 10:06:33 6
 华为概念+AI应用+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -704,7 +704,7 @@
 半年度增长+创新药+藏药龙头+西部大开发
 主:西部开发 次:创新药
 [西部开发] 西部大开发: 2.40
-[创新药] 创新药: 2.20
+[创新药] 创新药: 2.30
 </t>
       </text>
     </comment>
@@ -809,8 +809,8 @@
       <text>
         <t xml:space="preserve">8天6板 09:47:27 7
 电影《731》+AI智能体+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -952,7 +952,7 @@
         <t xml:space="preserve">5天3板 13:33:12 1
 中报预增+抗病毒药物
 主:创新药 次:预期改善
-[创新药] 化学制药: 1.60
+[创新药] 化学制药: 1.70
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -1038,8 +1038,8 @@
       <text>
         <t xml:space="preserve">6天4板 09:59:45 2
 华为概念+AI应用+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -1067,8 +1067,8 @@
       <text>
         <t xml:space="preserve">9天6板 10:17:04 2
 华为概念+中报预增+AI应用
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -1078,7 +1078,7 @@
         <t xml:space="preserve">5天5板 14:36:06 1
 医疗器械+细胞治疗+海南自贸港
 主:创新药 次:-
-[创新药] 医疗器械: 2.20
+[创新药] 医疗器械: 2.30
 </t>
       </text>
     </comment>
@@ -1121,8 +1121,8 @@
       <text>
         <t xml:space="preserve">8天7板 14:54:06 0
 AI智能体+出口数据上链+会展运营+上海国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 1.50
+主:AI应用 次:国企
+[AI应用] AI智能体: 1.60
 [国企] 上海国企: 1.10
 </t>
       </text>
@@ -1300,8 +1300,8 @@
       <text>
         <t xml:space="preserve">5天4板 10:11:24 13
 脑机接口（已澄清）+农批市场+特医食品+国企改革
-主:AI大模型 次:传统消费
-[AI大模型] 脑机接口（已澄清）: 2.30
+主:AI应用 次:传统消费
+[AI应用] 脑机接口（已澄清）: 2.40
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -1527,8 +1527,8 @@
       <text>
         <t xml:space="preserve">4天4板 09:57:57 1
 电影《731》+AI智能体+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -1577,7 +1577,7 @@
         <t xml:space="preserve">4天4板 09:25:02 1
 医疗器械+细胞治疗+海南自贸港
 主:创新药 次:-
-[创新药] 医疗器械: 2.20
+[创新药] 医疗器械: 2.30
 </t>
       </text>
     </comment>
@@ -1625,7 +1625,7 @@
         <t xml:space="preserve">3天3板 09:25:03 1
 医药流通+民营医院+黑龙江自贸区
 主:创新药 次:-
-[创新药] 医药流通: 1.80
+[创新药] 医药流通: 1.90
 </t>
       </text>
     </comment>
@@ -1682,9 +1682,9 @@
       <text>
         <t xml:space="preserve">7天5板 14:37:15 6
 水利+雅下水电概念+AI水科技+深圳国资
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -1712,7 +1712,7 @@
         <t xml:space="preserve">2天2板 09:25:00 1
 字节（营销）+医药包装+国企改革
 主:创新药 次:国企
-[创新药] 医药包装: 1.80
+[创新药] 医药包装: 1.90
 [国企] 国企改革: 1.30
 </t>
       </text>
@@ -1721,9 +1721,9 @@
       <text>
         <t xml:space="preserve">5天3板 10:42:21 1
 砺算科技+存储芯片+存算联一体化
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 存储芯片: 2.80
-[AI大模型] AI终端: 1.70
+[AI应用] AI终端: 1.80
 </t>
       </text>
     </comment>
@@ -1770,7 +1770,7 @@
         <t xml:space="preserve">3天3板 09:39:08 1
 FDA认证+神经介入+中报预增
 主:创新药 次:预期改善
-[创新药] FDA突破性医疗器械认证: 1.80
+[创新药] FDA突破性医疗器械认证: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -1789,8 +1789,8 @@
       <text>
         <t xml:space="preserve">5天5板 09:33:16 1
 电影《731》+AI智能体+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -1819,8 +1819,8 @@
       <text>
         <t xml:space="preserve">8天5板 09:34:56 2
 华为概念+AI应用+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -1867,8 +1867,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:25:00 0
 参股中昊芯英+AI教育
-主:AI大模型 次:-
-[AI大模型] AI教育: 1.70
+主:AI应用 次:-
+[AI应用] AI教育: 1.80
 </t>
       </text>
     </comment>
@@ -1941,7 +1941,7 @@
         <t xml:space="preserve">3天3板 09:25:00 6
 创新药+特医食品+医药百强
 主:创新药 次:传统消费
-[创新药] 创新药: 3.40
+[创新药] 创新药: 3.50
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -2009,7 +2009,7 @@
         <t xml:space="preserve">5天3板 13:17:19 4
 中报预增+氨糖+超级鱼油
 主:创新药 次:预期改善
-[创新药] 海洋医药: 1.80
+[创新药] 海洋医药: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -2018,8 +2018,8 @@
       <text>
         <t xml:space="preserve">3天3板 09:41:41 0
 电影《731》+AI智能体+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -2058,9 +2058,9 @@
       <text>
         <t xml:space="preserve">5天3板 09:31:33 0
 AI服务器电源+机器人概念+小米汽车+半年报增长
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.40
-[AI大模型] AI服务器电源: 1.90
+[AI应用] AI服务器电源: 2.00
 </t>
       </text>
     </comment>
@@ -2098,9 +2098,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:25:00 0
 创新药+脑机接口+AI眼镜+OTC药品
-主:创新药 次:AI大模型
-[创新药] OTC药品: 2.20
-[AI大模型] 脑机接口: 1.90
+主:创新药 次:AI应用
+[创新药] OTC药品: 2.30
+[AI应用] 脑机接口: 2.00
 </t>
       </text>
     </comment>
@@ -2118,8 +2118,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:25:00 0
 华为昇腾+AI交通+摩尔线程合作
-主:AI大模型 次:华为概念
-[AI大模型] AI交通: 1.70
+主:AI应用 次:华为概念
+[AI应用] AI交通: 1.80
 [华为概念] 华为昇腾: 1.20
 </t>
       </text>
@@ -2189,7 +2189,7 @@
         <t xml:space="preserve">2天2板 09:30:00 3
 中药+驱蚊液+国企
 主:创新药 次:国企
-[创新药] 中药: 2.00
+[创新药] 中药: 2.10
 [国企] 国企: 1.50
 </t>
       </text>
@@ -2199,7 +2199,7 @@
         <t xml:space="preserve">3天3板 14:18:18 0
 中药+三胎概念+国企
 主:创新药 次:国企
-[创新药] 中药: 2.00
+[创新药] 中药: 2.10
 [国企] 国企: 1.50
 </t>
       </text>
@@ -2210,7 +2210,7 @@
 藏药龙头+创新药+西部大开发
 主:西部开发 次:创新药
 [西部开发] 西部大开发: 2.40
-[创新药] 创新药: 2.20
+[创新药] 创新药: 2.30
 </t>
       </text>
     </comment>
@@ -2229,7 +2229,7 @@
         <t xml:space="preserve">2天2板 09:30:45 6
 创新药+小核酸药物+医药产品
 主:创新药 次:-
-[创新药] 创新药: 3.00
+[创新药] 创新药: 3.10
 </t>
       </text>
     </comment>
@@ -2267,7 +2267,7 @@
         <t xml:space="preserve">2天2板 09:25:00 0
 医疗器械+海外收入+子公司业绩
 主:创新药 次:预期改善
-[创新药] 医疗器械: 2.00
+[创新药] 医疗器械: 2.10
 [预期改善] 子公司业绩: 1.10
 </t>
       </text>
@@ -2306,9 +2306,9 @@
       <text>
         <t xml:space="preserve">3天3板 10:22:30 2
 脑机接口+AI医疗+综合医疗
-主:AI大模型 次:创新药
-[AI大模型] 脑机接口: 3.30
-[创新药] 综合医疗: 2.40
+主:AI应用 次:创新药
+[AI应用] 脑机接口: 3.40
+[创新药] 综合医疗: 2.50
 </t>
       </text>
     </comment>
@@ -2424,9 +2424,9 @@
       <text>
         <t xml:space="preserve">2天2板 10:14:03 2
 大洋千机大模型平台+机器人+机器视觉+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器视觉: 3.50
-[AI大模型] 大洋千机大模型平台: 1.90
+[AI应用] 大洋千机大模型平台: 2.00
 </t>
       </text>
     </comment>
@@ -2434,9 +2434,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:25:00 3
 华为昇腾+算力+AI智能体+OSS系统
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.60
-[AI大模型] AI智能体: 1.70
+[AI应用] AI智能体: 1.80
 </t>
       </text>
     </comment>
@@ -2445,7 +2445,7 @@
         <t xml:space="preserve">2天2板 09:30:30 5
 创新药+特医食品+医药百强
 主:创新药 次:传统消费
-[创新药] 创新药: 3.40
+[创新药] 创新药: 3.50
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -2475,7 +2475,7 @@
         <t xml:space="preserve">2天2板 09:36:33 2
 创新药+药品注册+化学制剂
 主:创新药 次:-
-[创新药] 创新药: 3.20
+[创新药] 创新药: 3.30
 </t>
       </text>
     </comment>
@@ -2524,7 +2524,7 @@
         <t xml:space="preserve">2天2板 09:25:03 0
 FDA突破性医疗器械认证+神经介入创新+中报预增
 主:创新药 次:预期改善
-[创新药] FDA突破性医疗器械认证: 1.80
+[创新药] FDA突破性医疗器械认证: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -2643,7 +2643,7 @@
         <t xml:space="preserve">4天3板 10:22:45 0
 中报预增+资产出售+化学制药
 主:创新药 次:预期改善
-[创新药] 化学制药: 1.60
+[创新药] 化学制药: 1.70
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -2720,9 +2720,9 @@
       <text>
         <t xml:space="preserve">3天2板 09:34:54 2
 砺算科技+AI终端+存储芯片
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 存储芯片: 2.80
-[AI大模型] AI终端: 1.70
+[AI应用] AI终端: 1.80
 </t>
       </text>
     </comment>
@@ -2731,7 +2731,7 @@
         <t xml:space="preserve">2天2板 09:37:43 0
 辅助生殖+创新药+医药制造
 主:创新药 次:-
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 </t>
       </text>
     </comment>
@@ -2963,7 +2963,7 @@
         <t xml:space="preserve">2天2板 09:34:57 2
 创新药+抗流感+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -2983,7 +2983,7 @@
         <t xml:space="preserve">2天2板 09:34:54 1
 高温合金+大飞机+微生态活菌+创新药
 主:创新药 次:军工
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [军工] 大飞机: 1.70
 </t>
       </text>
@@ -2993,7 +2993,7 @@
         <t xml:space="preserve">2天2板 09:30:59 23
 氨糖+海洋医药+中报预增
 主:创新药 次:预期改善
-[创新药] 海洋医药: 1.80
+[创新药] 海洋医药: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -3022,8 +3022,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:31:10 7
 脑机接口+军需品+核污染防治+国企
-主:AI大模型 次:国企
-[AI大模型] 脑机接口: 1.70
+主:AI应用 次:国企
+[AI应用] 脑机接口: 1.80
 [国企] 国企: 1.30
 </t>
       </text>
@@ -3093,7 +3093,7 @@
         <t xml:space="preserve">3天3板 09:25:03 1
 创新药+动物疫苗+多联多价疫苗+回购
 主:创新药 次:-
-[创新药] 动物疫苗: 3.60
+[创新药] 动物疫苗: 3.70
 </t>
       </text>
     </comment>
@@ -3121,8 +3121,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:30:00 0
 智算云+数字货币+信创+AI安全
-主:AI大模型 次:数字经济
-[AI大模型] AI安全: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI安全: 1.80
 [数字经济] 数字货币: 1.30
 </t>
       </text>
@@ -3200,7 +3200,7 @@
         <t xml:space="preserve">2天2板 09:45:57 1
 抗病毒药物+资产出售+中报预增
 主:创新药 次:预期改善
-[创新药] 化学制药: 1.60
+[创新药] 化学制药: 1.70
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -3292,8 +3292,8 @@
       <text>
         <t xml:space="preserve">4天3板 13:28:23 4
 华为概念+AI应用+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -3333,7 +3333,7 @@
         <t xml:space="preserve">3天3板 09:30:29 0
 医疗器械+细胞治疗+海南自贸港
 主:创新药 次:-
-[创新药] 医疗器械: 2.20
+[创新药] 医疗器械: 2.30
 </t>
       </text>
     </comment>
@@ -3430,9 +3430,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:30:03 0
 华为昇腾+算力+AI智能体+OSS系统
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.60
-[AI大模型] AI智能体: 1.70
+[AI应用] AI智能体: 1.80
 </t>
       </text>
     </comment>
@@ -3461,7 +3461,7 @@
         <t xml:space="preserve">3天2板 09:57:07 16
 原料药+创新药+仿制药
 主:创新药 次:-
-[创新药] 原料药: 2.60
+[创新药] 原料药: 2.70
 </t>
       </text>
     </comment>
@@ -3505,8 +3505,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:36:40 2
 AI智能体+数据要素+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -3604,9 +3604,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:40:03 4
 创新药+脑科学+SPD业务
-主:创新药 次:AI大模型
-[创新药] 创新药: 2.20
-[AI大模型] 脑机接口: 2.10
+主:创新药 次:AI应用
+[创新药] 创新药: 2.30
+[AI应用] 脑机接口: 2.20
 </t>
       </text>
     </comment>
@@ -3685,7 +3685,7 @@
         <t xml:space="preserve">2天2板 11:00:36 0
 创新药+降血脂药物+重组胶原蛋白+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 [国企] 国企改革: 1.30
 </t>
       </text>
@@ -3704,7 +3704,7 @@
         <t xml:space="preserve">首板涨停 09:25:00 0
 获新靶点研发项目+创新药+股份回购
 主:创新药 次:预期改善
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [预期改善] 股份回购: 0.70
 </t>
       </text>
@@ -3821,8 +3821,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:00 0
 智算云+数字货币+信创+AI安全
-主:AI大模型 次:数字经济
-[AI大模型] AI安全: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI安全: 1.80
 [数字经济] 数字货币: 1.30
 </t>
       </text>
@@ -3852,7 +3852,7 @@
         <t xml:space="preserve">2天2板 11:04:15 7
 创新药+化学制药+特色中间体
 主:创新药 次:-
-[创新药] 创新药: 3.20
+[创新药] 创新药: 3.30
 </t>
       </text>
     </comment>
@@ -3900,7 +3900,7 @@
         <t xml:space="preserve">首板涨停 09:31:00 0
 腹膜透析液+化学制药+年报增长
 主:创新药 次:预期改善
-[创新药] 化学制药: 1.60
+[创新药] 化学制药: 1.70
 [预期改善] 年报增长: 0.70
 </t>
       </text>
@@ -3916,8 +3916,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:30:01 0
 广播电视+AI智能体+数据要素+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -4082,9 +4082,9 @@
       <text>
         <t xml:space="preserve">4天4板 14:52:36 5
 水务建设+AI水科技+深圳国资
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -4137,8 +4137,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:00 0
 AI设计+订单增长+海外业务
-主:AI大模型 次:预期改善
-[AI大模型] AI设计: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI设计: 1.60
 [预期改善] 订单增长: 0.70
 </t>
       </text>
@@ -4148,7 +4148,7 @@
         <t xml:space="preserve">首板涨停 09:30:40 8
 中报预增+氨糖+海洋医药
 主:创新药 次:预期改善
-[创新药] 海洋医药: 1.80
+[创新药] 海洋医药: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -4176,9 +4176,9 @@
       <text>
         <t xml:space="preserve">2天2板 11:24:24 0
 军工+医疗AI+SIP芯片+华为昇腾
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] SIP芯片: 2.60
-[AI大模型] 医疗AI: 1.70
+[AI应用] 医疗AI: 1.80
 </t>
       </text>
     </comment>
@@ -4255,7 +4255,7 @@
         <t xml:space="preserve">3天3板 09:32:03 1
 参股投资+创新药+独家品种
 主:创新药 次:-
-[创新药] 中药: 2.40
+[创新药] 中药: 2.50
 </t>
       </text>
     </comment>
@@ -4263,9 +4263,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:50:24 7
 房地产+创新药+机器人
-主:机器人 次:大基建
+主:机器人 次:创新药
 [机器人] 机器人: 2.40
-[大基建] 房地产: 1.90
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -4284,7 +4284,7 @@
         <t xml:space="preserve">3天2板 13:33:12 0
 控制权拟变更+口腔医疗+永磁开关
 主:创新药 次:-
-[创新药] 牙科医疗: 2.00
+[创新药] 牙科医疗: 2.10
 </t>
       </text>
     </comment>
@@ -4367,9 +4367,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:00 5
 AI智能助手+云计算+机器人概念+板式家具
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.00
-[AI大模型] AI智能助手: 1.50
+[AI应用] AI智能助手: 1.60
 </t>
       </text>
     </comment>
@@ -4378,7 +4378,7 @@
         <t xml:space="preserve">首板涨停 09:30:19 0
 创新药+小核酸药物+医药产品
 主:创新药 次:-
-[创新药] 创新药: 3.00
+[创新药] 创新药: 3.10
 </t>
       </text>
     </comment>
@@ -4425,8 +4425,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:30:15 0
 社保卡服务+AI民生+数字人民币+数据要素
-主:AI大模型 次:数字经济
-[AI大模型] AI民生: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI民生: 1.80
 [数字经济] 数字人民币: 1.30
 </t>
       </text>
@@ -4484,7 +4484,7 @@
         <t xml:space="preserve">2天2板 09:30:55 1
 动物疫苗+多联多价疫苗+创新药+回购
 主:创新药 次:-
-[创新药] 动物疫苗: 3.60
+[创新药] 动物疫苗: 3.70
 </t>
       </text>
     </comment>
@@ -4492,9 +4492,9 @@
       <text>
         <t xml:space="preserve">3天3板 09:32:30 3
 数据中心+AI算力+液冷超充
-主:算力半导体 次:AI大模型
-[算力半导体] 液冷超充: 4.10
-[AI大模型] AI: 2.10
+主:算力半导体 次:AI应用
+[算力半导体] 液冷超充: 4.70
+[AI应用] AI: 1.60
 </t>
       </text>
     </comment>
@@ -4590,9 +4590,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:30:35 1
 AI服务器+高速铜缆+藕芯结构
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 高速铜缆: 2.80
-[AI大模型] AI服务器: 1.90
+[AI应用] AI服务器: 2.00
 </t>
       </text>
     </comment>
@@ -4610,7 +4610,7 @@
         <t xml:space="preserve">首板涨停 09:25:01 0
 辅助生殖+创新药+医药制造
 主:创新药 次:-
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 </t>
       </text>
     </comment>
@@ -4694,8 +4694,8 @@
       <text>
         <t xml:space="preserve">3天3板 10:44:12 5
 脑机接口（已澄清）+农批市场+特医食品+国企改革
-主:AI大模型 次:传统消费
-[AI大模型] 脑机接口（已澄清）: 2.30
+主:AI应用 次:传统消费
+[AI应用] 脑机接口（已澄清）: 2.40
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -4753,8 +4753,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:00 0
 参股中昊芯英+AI教育
-主:AI大模型 次:-
-[AI大模型] AI教育: 1.70
+主:AI应用 次:-
+[AI应用] AI教育: 1.80
 </t>
       </text>
     </comment>
@@ -4762,8 +4762,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:03 0
 拟收购存储资产+AI算力
-主:AI大模型 次:-
-[AI大模型] AI算力: 1.50
+主:算力半导体 次:-
+[算力半导体] AI算力: 2.40
 </t>
       </text>
     </comment>
@@ -4811,8 +4811,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:39:51 0
 AI智能体+电纸书+机器狗
-主:AI大模型 次:-
-[AI大模型] AI智能体: 1.50
+主:AI应用 次:-
+[AI应用] AI智能体: 1.60
 </t>
       </text>
     </comment>
@@ -4889,9 +4889,9 @@
       <text>
         <t xml:space="preserve">3天2板 14:55:24 0
 脑机接口+AI医疗+综合医疗
-主:AI大模型 次:创新药
-[AI大模型] 脑机接口: 3.30
-[创新药] 综合医疗: 2.40
+主:AI应用 次:创新药
+[AI应用] 脑机接口: 3.40
+[创新药] 综合医疗: 2.50
 </t>
       </text>
     </comment>
@@ -4919,8 +4919,8 @@
       <text>
         <t xml:space="preserve">2天2板 13:11:09 0
 脑机接口（已澄清）+农批市场+特医食品+国企改革
-主:AI大模型 次:传统消费
-[AI大模型] 脑机接口（已澄清）: 2.30
+主:AI应用 次:传统消费
+[AI应用] 脑机接口（已澄清）: 2.40
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -4948,9 +4948,9 @@
       <text>
         <t xml:space="preserve">3天2板 10:18:32 0
 AI服务器材料+光刻胶试产+英伟达概念
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 光刻胶试产: 2.80
-[AI大模型] AI服务器材料: 1.90
+[AI应用] AI服务器材料: 2.00
 </t>
       </text>
     </comment>
@@ -4958,9 +4958,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:32:03 0
 数据中心+AI算力+液冷超充
-主:算力半导体 次:AI大模型
-[算力半导体] 液冷超充: 4.10
-[AI大模型] AI: 2.10
+主:算力半导体 次:AI应用
+[算力半导体] 液冷超充: 4.70
+[AI应用] AI: 1.60
 </t>
       </text>
     </comment>
@@ -4968,8 +4968,8 @@
       <text>
         <t xml:space="preserve">4天3板 09:45:15 7
 稳定币+AI金融科技+限制性股票激励
-主:AI大模型 次:数字经济
-[AI大模型] AI大模型: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI大模型: 1.80
 [数字经济] 稳定币: 1.70
 </t>
       </text>
@@ -5047,7 +5047,7 @@
         <t xml:space="preserve">2天2板 09:31:15 5
 创新药+细胞免疫治疗+养老概念
 主:创新药 次:预期改善
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 [预期改善] 年报增长: 0.70
 </t>
       </text>
@@ -5086,7 +5086,7 @@
         <t xml:space="preserve">首板涨停 09:38:36 0
 核医药+创新药+阿尔兹海默症
 主:创新药 次:-
-[创新药] 核医药: 1.80
+[创新药] 核医药: 1.90
 </t>
       </text>
     </comment>
@@ -5240,8 +5240,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:03 0
 AI交通+华为昇腾+摩尔线程合作+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI交通: 1.70
+主:AI应用 次:华为概念
+[AI应用] AI交通: 1.80
 [华为概念] 华为昇腾: 1.20
 </t>
       </text>
@@ -5300,7 +5300,7 @@
         <t xml:space="preserve">首板涨停 09:45:33 0
 医疗器械+一季报增长+新产品获批
 主:创新药 次:预期改善
-[创新药] 医疗器械: 1.60
+[创新药] 医疗器械: 1.70
 [预期改善] 一季报增长: 0.70
 </t>
       </text>
@@ -5330,7 +5330,7 @@
 半导体洁净室+业绩预增+医疗器械
 主:算力半导体 次:创新药
 [算力半导体] 半导体洁净室: 2.40
-[创新药] 医疗器械: 1.60
+[创新药] 医疗器械: 1.70
 </t>
       </text>
     </comment>
@@ -5348,8 +5348,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:33:27 0
 AI应用+智算中心+一季报增长
-主:AI大模型 次:预期改善
-[AI大模型] AI应用: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI应用: 1.60
 [预期改善] 一季报增长: 0.70
 </t>
       </text>
@@ -5389,7 +5389,7 @@
         <t xml:space="preserve">首板涨停 09:25:02 0
 FDA突破性医疗器械认证+神经介入创新+中报预增
 主:创新药 次:预期改善
-[创新药] FDA突破性医疗器械认证: 1.80
+[创新药] FDA突破性医疗器械认证: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -5408,8 +5408,8 @@
       <text>
         <t xml:space="preserve">3天2板 09:53:16 12
 华为概念+AI应用+中报预增
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -5437,8 +5437,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:31:30 2
 稳定币+限制性股票激励+AI大模型
-主:AI大模型 次:数字经济
-[AI大模型] AI大模型: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI大模型: 1.80
 [数字经济] 稳定币: 1.70
 </t>
       </text>
@@ -5448,7 +5448,7 @@
         <t xml:space="preserve">2天2板 10:37:32 7
 医疗器械+细胞治疗+海南自贸港
 主:创新药 次:-
-[创新药] 医疗器械: 2.20
+[创新药] 医疗器械: 2.30
 </t>
       </text>
     </comment>
@@ -5466,9 +5466,9 @@
       <text>
         <t xml:space="preserve">3天2板 09:30:30 0
 数据中心电源+液冷技术+储能
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷技术: 3.50
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -5547,7 +5547,7 @@
         <t xml:space="preserve">首板涨停 09:46:48 0
 医美包装+医疗器械+香港子公司
 主:创新药 次:-
-[创新药] 医疗器械: 1.60
+[创新药] 医疗器械: 1.70
 </t>
       </text>
     </comment>
@@ -5591,7 +5591,7 @@
         <t xml:space="preserve">首板涨停 09:34:24 0
 中药+创新药+心脑血管
 主:创新药 次:-
-[创新药] 中药: 2.40
+[创新药] 中药: 2.50
 </t>
       </text>
     </comment>
@@ -5689,8 +5689,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:41:55 0
 全景无人机发布+全景相机+AI技术
-主:AI大模型 次:无人经济
-[AI大模型] AI技术: 1.70
+主:AI应用 次:无人经济
+[AI应用] AI技术: 1.80
 [无人经济] 全景无人机发布: 1.30
 </t>
       </text>
@@ -5700,7 +5700,7 @@
         <t xml:space="preserve">2天2板 09:34:15 0
 MASH药物合作+自有药品高增长
 主:创新药 次:-
-[创新药] 自有药品高增长: 1.80
+[创新药] 自有药品高增长: 1.90
 </t>
       </text>
     </comment>
@@ -5708,9 +5708,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:25:00 0
 脑机接口+OTC药品+创新药
-主:创新药 次:AI大模型
-[创新药] OTC药品: 2.20
-[AI大模型] 脑机接口: 1.90
+主:创新药 次:AI应用
+[创新药] OTC药品: 2.30
+[AI应用] 脑机接口: 2.00
 </t>
       </text>
     </comment>
@@ -5787,9 +5787,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:03:30 0
 AI医疗智能助手+机器人+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.00
-[AI大模型] AI医疗智能助手: 1.50
+[AI应用] AI医疗智能助手: 1.60
 </t>
       </text>
     </comment>
@@ -5864,9 +5864,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:36:57 0
 军工+医疗AI+SIP芯片+网络安全
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] SIP芯片: 2.60
-[AI大模型] 医疗AI: 1.70
+[AI应用] 医疗AI: 1.80
 </t>
       </text>
     </comment>
@@ -5941,8 +5941,8 @@
       <text>
         <t xml:space="preserve">2天2板 09:50:41 0
 细胞膜色谱+海洋经济+人工智能+中报增长
-主:AI大模型 次:预期改善
-[AI大模型] 人工智能: 1.70
+主:AI应用 次:预期改善
+[AI应用] 人工智能: 1.80
 [预期改善] 中报增长: 0.90
 </t>
       </text>
@@ -5962,7 +5962,7 @@
         <t xml:space="preserve">首板涨停 09:25:03 14
 购买专利+中药创新药+新药获批
 主:创新药 次:-
-[创新药] 中药创新药: 1.60
+[创新药] 中药创新药: 1.70
 </t>
       </text>
     </comment>
@@ -6040,9 +6040,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:39:11 1
 光学镜头+AI眼镜+外销+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器视觉: 2.50
-[AI大模型] AI眼镜: 1.50
+[AI应用] AI眼镜: 1.60
 </t>
       </text>
     </comment>
@@ -6051,7 +6051,7 @@
         <t xml:space="preserve">首板涨停 09:45:30 3
 中报预增+减肥药+中成药+创新药
 主:创新药 次:预期改善
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [预期改善] 中报预增: 0.70
 </t>
       </text>
@@ -6077,7 +6077,7 @@
         <t xml:space="preserve">首板涨停 09:48:24 0
 动物疫苗+多联多价疫苗+合作开发
 主:创新药 次:-
-[创新药] 动物疫苗: 3.60
+[创新药] 动物疫苗: 3.70
 </t>
       </text>
     </comment>
@@ -6094,8 +6094,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:38:28 0
 PET铜箔+环保+AI环保岛+海外布局
-主:AI大模型 次:-
-[AI大模型] AI环保岛: 1.50
+主:AI应用 次:-
+[AI应用] AI环保岛: 1.60
 </t>
       </text>
     </comment>
@@ -6131,8 +6131,8 @@
       <text>
         <t xml:space="preserve">2天2板 10:59:57 0
 社保卡服务+AI民生+数字人民币+数据要素
-主:AI大模型 次:数字经济
-[AI大模型] AI民生: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI民生: 1.80
 [数字经济] 数字人民币: 1.30
 </t>
       </text>
@@ -6259,9 +6259,9 @@
       <text>
         <t xml:space="preserve">3天3板 09:32:45 1
 水务建设+AI水科技+深圳国资
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -6278,9 +6278,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:10:33 0
 AI智能体+算力+有线电视+国企改革
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.40
-[AI大模型] AI智能体: 1.70
+[AI应用] AI智能体: 1.80
 </t>
       </text>
     </comment>
@@ -6299,7 +6299,7 @@
         <t xml:space="preserve">首板涨停 09:51:46 9
 达格列净获批+创新药CDMO+业绩改善
 主:创新药 次:预期改善
-[创新药] 创新药CDMO: 1.60
+[创新药] 创新药CDMO: 1.70
 [预期改善] 业绩改善: 0.70
 </t>
       </text>
@@ -6329,7 +6329,7 @@
         <t xml:space="preserve">首板涨停 09:56:21 0
 中药+创新药+国企
 主:创新药 次:国企
-[创新药] 中药: 1.80
+[创新药] 中药: 1.90
 [国企] 国企: 1.10
 </t>
       </text>
@@ -6369,7 +6369,7 @@
         <t xml:space="preserve">首板涨停 09:32:30 0
 原料药获批+创新药+化学制药
 主:创新药 次:-
-[创新药] 原料药获批: 2.00
+[创新药] 原料药获批: 2.10
 </t>
       </text>
     </comment>
@@ -6387,7 +6387,7 @@
         <t xml:space="preserve">2天2板 14:28:38 0
 特色原料药+JH389进展（减肥药）+中报预增
 主:创新药 次:预期改善
-[创新药] 特色原料药: 1.80
+[创新药] 特色原料药: 1.90
 [预期改善] 中报预增: 0.90
 </t>
       </text>
@@ -6426,8 +6426,8 @@
       <text>
         <t xml:space="preserve">2天2板 10:01:52 5
 AI服务器+PCB+国企改革
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 2.10
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 2.20
 [精密电子] PCB: 1.70
 </t>
       </text>
@@ -6464,9 +6464,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:38:01 0
 AI芯片+人形机器人+营收增长
-主:机器人 次:AI大模型
+主:算力半导体 次:机器人
+[算力半导体] AI芯片: 2.90
 [机器人] 人形机器人: 2.50
-[AI大模型] AI芯片: 1.50
 </t>
       </text>
     </comment>
@@ -6474,9 +6474,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:33:45 0
 业绩增长+AI算力需求+数据中心市场+电网设备
-主:算力半导体 次:AI大模型
-[算力半导体] 数据中心: 3.00
-[AI大模型] AI算力需求: 1.70
+主:算力半导体 次:电力
+[算力半导体] 数据中心: 3.40
+[电力] 电网设备: 1.30
 </t>
       </text>
     </comment>
@@ -6523,9 +6523,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:17:15 1
 机器人+智能驾培+AI应用
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.20
-[AI大模型] AI应用: 1.70
+[AI应用] AI应用: 1.80
 </t>
       </text>
     </comment>
@@ -6534,7 +6534,7 @@
         <t xml:space="preserve">首板涨停 09:41:30 0
 创新药上市+销售增长+股票发行受理
 主:创新药 次:大金融
-[创新药] 创新药上市: 1.60
+[创新药] 创新药上市: 1.70
 [大金融] 股票发行受理: 1.10
 </t>
       </text>
@@ -6554,7 +6554,7 @@
         <t xml:space="preserve">首板涨停 09:49:55 1
 汽车电子+上海国企+医疗器械
 主:创新药 次:消费电子
-[创新药] 医疗器械: 2.40
+[创新药] 医疗器械: 2.50
 [消费电子] 汽车电子: 1.90
 </t>
       </text>
@@ -6573,7 +6573,7 @@
         <t xml:space="preserve">首板涨停 09:56:24 0
 黄甲软肝+创新药+中药
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -6611,8 +6611,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:33:24 7
 AI智能体+数据要素+广播电视+国企
-主:AI大模型 次:国企
-[AI大模型] AI智能体: 2.90
+主:AI应用 次:国企
+[AI应用] AI智能体: 3.00
 [国企] 国企: 2.30
 </t>
       </text>
@@ -6670,7 +6670,7 @@
         <t xml:space="preserve">2天2板 10:02:57 2
 创新药+独家品种+心脑血管在研项目
 主:创新药 次:-
-[创新药] 中药: 2.40
+[创新药] 中药: 2.50
 </t>
       </text>
     </comment>
@@ -6678,9 +6678,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:50:00 0
 液冷用泵+AI营销+华为概念+中报预增
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷用泵: 3.10
-[AI大模型] AI营销: 1.70
+[AI应用] AI营销: 1.80
 </t>
       </text>
     </comment>
@@ -6756,8 +6756,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:34:01 2
 期权激励+中报预增+AI产品
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -6766,8 +6766,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:21:12 1
 AI智能体+拟购买智者品牌股权+营销传播
-主:AI大模型 次:-
-[AI大模型] AI智能体: 1.50
+主:AI应用 次:-
+[AI应用] AI智能体: 1.60
 </t>
       </text>
     </comment>
@@ -6826,7 +6826,7 @@
         <t xml:space="preserve">首板涨停 10:05:04 4
 创新药+中成药+西藏
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -6834,9 +6834,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:40:45 17
 低压电器+数据中心+股份回购
-主:算力半导体 次:AI大模型
-[算力半导体] 数据中心: 3.00
-[AI大模型] AI算力需求: 1.70
+主:算力半导体 次:电力
+[算力半导体] 数据中心: 3.40
+[电力] 电网设备: 1.30
 </t>
       </text>
     </comment>
@@ -6844,8 +6844,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:55:39 4
 智慧交通+无人驾驶+AI智能助手
-主:AI大模型 次:无人经济
-[AI大模型] AI智能助手: 1.50
+主:AI应用 次:无人经济
+[AI应用] AI智能助手: 1.60
 [无人经济] 无人驾驶: 1.10
 </t>
       </text>
@@ -6855,7 +6855,7 @@
         <t xml:space="preserve">首板涨停 09:40:00 0
 医疗器械+海外收入+子公司业绩
 主:创新药 次:预期改善
-[创新药] 医疗器械: 2.00
+[创新药] 医疗器械: 2.10
 [预期改善] 子公司业绩: 1.10
 </t>
       </text>
@@ -6884,7 +6884,7 @@
         <t xml:space="preserve">首板涨停 09:34:02 7
 创新药+中成药+新活素+藏药
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -6932,9 +6932,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:54:18 0
 养老机器人+男装+AI新零售+回购
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.20
-[AI大模型] AI新零售: 1.70
+[AI应用] AI新零售: 1.80
 </t>
       </text>
     </comment>
@@ -6971,7 +6971,7 @@
         <t xml:space="preserve">首板涨停 09:38:45 0
 业绩减亏+创新药+医药制剂
 主:创新药 次:预期改善
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 [预期改善] 业绩减亏: 0.70
 </t>
       </text>
@@ -7001,7 +7001,7 @@
         <t xml:space="preserve">5天3板 10:20:27 0
 创新药+医药制造+辅助生殖
 主:创新药 次:-
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 </t>
       </text>
     </comment>
@@ -7018,8 +7018,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:22:05 2
 DeepSeek概念+华为昇腾+时空信息
-主:AI大模型 次:华为概念
-[AI大模型] DeepSeek概念: 1.50
+主:AI应用 次:华为概念
+[AI应用] DeepSeek概念: 1.60
 [华为概念] 华为昇腾: 1.00
 </t>
       </text>
@@ -7038,9 +7038,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:01:37 0
 砺算科技+AI终端+存储芯片+车规产品
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 存储芯片: 2.80
-[AI大模型] AI终端: 1.70
+[AI应用] AI终端: 1.80
 </t>
       </text>
     </comment>
@@ -7106,8 +7106,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:43:56 2
 华为概念+中报预增+AI应用
-主:AI大模型 次:华为概念
-[AI大模型] AI产品: 2.90
+主:AI应用 次:华为概念
+[AI应用] AI产品: 3.00
 [华为概念] 华为概念: 2.20
 </t>
       </text>
@@ -7164,7 +7164,7 @@
         <t xml:space="preserve">首板涨停 09:30:54 0
 医疗器械+海外收入+子公司业绩
 主:创新药 次:预期改善
-[创新药] 医疗器械: 2.00
+[创新药] 医疗器械: 2.10
 [预期改善] 子公司业绩: 1.10
 </t>
       </text>
@@ -7213,7 +7213,7 @@
         <t xml:space="preserve">首板涨停 09:43:19 0
 半年报增长+日化龙头+合成生物
 主:创新药 次:预期改善
-[创新药] 合成生物: 1.60
+[创新药] 合成生物: 1.70
 [预期改善] 半年报增长: 0.70
 </t>
       </text>
@@ -7261,8 +7261,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:38:54 0
 无人车+AI物流+快递
-主:无人经济 次:-
-[无人经济] 无人车: 1.50
+主:AI应用 次:无人经济
+[AI应用] AI物流: 1.60
+[无人经济] 无人车: 1.30
 </t>
       </text>
     </comment>
@@ -7299,7 +7300,7 @@
         <t xml:space="preserve">首板涨停 10:11:42 0
 字节（营销）+医药包装+国企改革
 主:创新药 次:国企
-[创新药] 医药包装: 1.80
+[创新药] 医药包装: 1.90
 [国企] 国企改革: 1.30
 </t>
       </text>
@@ -7318,9 +7319,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:09:26 0
 AI智能体+人形机器人+工业软件
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 人形机器人: 2.50
-[AI大模型] AI智能体: 1.50
+[AI应用] AI智能体: 1.60
 </t>
       </text>
     </comment>
@@ -7386,9 +7387,9 @@
       <text>
         <t xml:space="preserve">2天2板 13:11:54 2
 脑机接口+AI医疗+综合医疗
-主:AI大模型 次:创新药
-[AI大模型] 脑机接口: 3.30
-[创新药] 综合医疗: 2.40
+主:AI应用 次:创新药
+[AI应用] 脑机接口: 3.40
+[创新药] 综合医疗: 2.50
 </t>
       </text>
     </comment>
@@ -7543,7 +7544,7 @@
 藏药龙头+创新药+西部大开发
 主:西部开发 次:创新药
 [西部开发] 西部大开发: 2.40
-[创新药] 创新药: 2.20
+[创新药] 创新药: 2.30
 </t>
       </text>
     </comment>
@@ -7571,8 +7572,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:16:25 0
 军工电子+无人机+AI应用
-主:AI大模型 次:军工
-[AI大模型] AI应用: 1.50
+主:AI应用 次:军工
+[AI应用] AI应用: 1.60
 [军工] 军工电子: 1.50
 </t>
       </text>
@@ -7641,8 +7642,8 @@
       <text>
         <t xml:space="preserve">3天2板 13:39:56 3
 脑机接口+AI按摩椅+AI大模型
-主:AI大模型 次:机器人
-[AI大模型] 脑机接口: 2.30
+主:AI应用 次:机器人
+[AI应用] 脑机接口: 2.40
 [机器人] 机器人概念: 2.00
 </t>
       </text>
@@ -7679,8 +7680,8 @@
       <text>
         <t xml:space="preserve">2天2板 10:36:03 0
 新剧上线+短剧出海+Rokid合作(AI眼镜)+国企
-主:AI大模型 次:全球布局
-[AI大模型] Rokid合作(AI眼镜): 1.50
+主:AI应用 次:全球布局
+[AI应用] Rokid合作(AI眼镜): 1.60
 [全球布局] 短剧出海: 1.30
 </t>
       </text>
@@ -7690,7 +7691,7 @@
         <t xml:space="preserve">首板涨停 09:35:53 0
 中药+大健康+中报增长+国企改革
 主:创新药 次:国企
-[创新药] 中药: 2.20
+[创新药] 中药: 2.30
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -7763,8 +7764,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:41:33 0
 AI教育+订单增长+政策支持
-主:AI大模型 次:预期改善
-[AI大模型] AI教育: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI教育: 1.60
 [预期改善] 订单增长: 0.70
 </t>
       </text>
@@ -7774,7 +7775,7 @@
         <t xml:space="preserve">首板涨停 10:01:45 0
 中报预增+资产出售+抗病毒药物
 主:创新药 次:预期改善
-[创新药] 化学制药: 1.60
+[创新药] 化学制药: 1.70
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -7784,7 +7785,7 @@
         <t xml:space="preserve">首板涨停 10:27:39 0
 创新药+医保纳入+业绩扭亏
 主:创新药 次:预期改善
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [预期改善] 业绩扭亏: 0.70
 </t>
       </text>
@@ -7794,7 +7795,7 @@
         <t xml:space="preserve">首板涨停 10:07:10 5
 创新药+抗流感+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -7861,9 +7862,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:06:00 0
 机器人+军工+商业航天+AI应用
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.00
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -7920,8 +7921,8 @@
       <text>
         <t xml:space="preserve">2天2板 11:08:42 7
 树图+数据要素+数字政府+AI
-主:AI大模型 次:-
-[AI大模型] AI: 1.70
+主:AI应用 次:-
+[AI应用] AI: 1.80
 </t>
       </text>
     </comment>
@@ -7955,8 +7956,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:47:54 2
 AI服务器+PCB+国企改革
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 2.10
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 2.20
 [精密电子] PCB: 1.70
 </t>
       </text>
@@ -7995,7 +7996,7 @@
         <t xml:space="preserve">首板涨停 09:33:26 0
 创新药+细胞免疫治疗+养老概念+年报增长
 主:创新药 次:预期改善
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 [预期改善] 年报增长: 0.70
 </t>
       </text>
@@ -8023,8 +8024,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:04:00 1
 AI服务器+光模块+HDI能力+子公司股权
-主:AI大模型 次:-
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:-
+[AI应用] AI服务器: 1.60
 </t>
       </text>
     </comment>
@@ -8033,7 +8034,7 @@
         <t xml:space="preserve">首板涨停 10:31:29 3
 原料药+创新药+仿制药
 主:创新药 次:-
-[创新药] 原料药: 2.60
+[创新药] 原料药: 2.70
 </t>
       </text>
     </comment>
@@ -8042,7 +8043,7 @@
         <t xml:space="preserve">首板涨停 10:13:15 0
 医药中间体+CDMO+投资创业基金+一季报扭亏
 主:创新药 次:大金融
-[创新药] 医药中间体: 1.60
+[创新药] 医药中间体: 1.70
 [大金融] 投资创业基金: 1.10
 </t>
       </text>
@@ -8051,9 +8052,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:32:36 13
 低压电器+数据中心+股份回购
-主:算力半导体 次:AI大模型
-[算力半导体] 数据中心: 3.00
-[AI大模型] AI算力需求: 1.70
+主:算力半导体 次:电力
+[算力半导体] 数据中心: 3.40
+[电力] 电网设备: 1.30
 </t>
       </text>
     </comment>
@@ -8068,8 +8069,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:25:03 0
 AI智能体+仪器仪表+核污染防治+电网设备
-主:AI大模型 次:新型能源
-[AI大模型] AI智能体: 1.70
+主:AI应用 次:新型能源
+[AI应用] AI智能体: 1.80
 [新型能源] 光伏概念: 1.20
 </t>
       </text>
@@ -8098,7 +8099,7 @@
         <t xml:space="preserve">首板涨停 09:56:21 0
 智能医疗+医疗器械+海外并购
 主:创新药 次:-
-[创新药] 智能医疗: 1.80
+[创新药] 智能医疗: 1.90
 </t>
       </text>
     </comment>
@@ -8116,8 +8117,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:37:20 0
 中报预增+固态电池+覆铜板
-主:AI大模型 次:新型能源
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:新型能源
+[AI应用] AI服务器: 1.60
 [新型能源] 固态电池: 1.20
 </t>
       </text>
@@ -8136,9 +8137,9 @@
       <text>
         <t xml:space="preserve">3天2板 14:15:09 0
 AI服务器电源+机器人概念+小米汽车+半年报增长
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.40
-[AI大模型] AI服务器电源: 1.90
+[AI应用] AI服务器电源: 2.00
 </t>
       </text>
     </comment>
@@ -8165,8 +8166,8 @@
       <text>
         <t xml:space="preserve">3天2板 11:22:45 7
 稳定币+短剧游戏+限制性股票激励+AI大模型
-主:AI大模型 次:数字经济
-[AI大模型] AI大模型: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI大模型: 1.80
 [数字经济] 稳定币: 1.70
 </t>
       </text>
@@ -8262,7 +8263,7 @@
         <t xml:space="preserve">首板涨停 11:11:54 1
 汽车电子+上海国企+医疗器械
 主:创新药 次:消费电子
-[创新药] 医疗器械: 2.40
+[创新药] 医疗器械: 2.50
 [消费电子] 汽车电子: 1.90
 </t>
       </text>
@@ -8271,9 +8272,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:05:39 12
 算力+AI游戏+全球化卡牌+中报预增
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.60
-[AI大模型] AI游戏: 1.70
+[AI应用] AI游戏: 1.80
 </t>
       </text>
     </comment>
@@ -8301,8 +8302,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:35:03 8
 AI营销+AI智能体+业绩增长
-主:AI大模型 次:预期改善
-[AI大模型] AI营销: 1.70
+主:AI应用 次:预期改善
+[AI应用] AI营销: 1.80
 [预期改善] 业绩增长: 0.70
 </t>
       </text>
@@ -8321,7 +8322,7 @@
         <t xml:space="preserve">首板涨停 10:25:04 1
 阶跃星辰相关+汽车电子+医疗器械+上海国企
 主:创新药 次:消费电子
-[创新药] 医疗器械: 2.40
+[创新药] 医疗器械: 2.50
 [消费电子] 汽车电子: 1.90
 </t>
       </text>
@@ -8350,8 +8351,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:59:58 0
 洗护产品+医美概念+AI合作
-主:AI大模型 次:-
-[AI大模型] AI合作: 1.50
+主:AI应用 次:-
+[AI应用] AI合作: 1.60
 </t>
       </text>
     </comment>
@@ -8360,7 +8361,7 @@
         <t xml:space="preserve">首板涨停 10:30:21 2
 创新药+一致性评价+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -8397,8 +8398,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:34:16 2
 全景无人机发布+全景相机+AI技术
-主:AI大模型 次:无人经济
-[AI大模型] AI技术: 1.70
+主:AI应用 次:无人经济
+[AI应用] AI技术: 1.80
 [无人经济] 全景无人机发布: 1.30
 </t>
       </text>
@@ -8524,7 +8525,7 @@
         <t xml:space="preserve">首板涨停 10:45:13 0
 医药流通+民营医院+黑龙江自贸区
 主:创新药 次:-
-[创新药] 医药流通: 1.80
+[创新药] 医药流通: 1.90
 </t>
       </text>
     </comment>
@@ -8532,8 +8533,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:37:00 0
 影视IP+短剧+Rokid合作
-主:AI大模型 次:全球布局
-[AI大模型] Rokid合作(AI眼镜): 1.50
+主:AI应用 次:全球布局
+[AI应用] Rokid合作(AI眼镜): 1.60
 [全球布局] 短剧出海: 1.30
 </t>
       </text>
@@ -8618,8 +8619,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:48:39 6
 脑机接口+智能电动床+鸿蒙系统
-主:AI大模型 次:华为概念
-[AI大模型] 脑机接口: 1.50
+主:AI应用 次:华为概念
+[AI应用] 脑机接口: 1.60
 [华为概念] 鸿蒙系统: 1.00
 </t>
       </text>
@@ -8687,9 +8688,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:07:12 0
 智算算力+AI解决方案+武汉国资
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 智算算力: 2.40
-[AI大模型] AI解决方案: 1.50
+[AI应用] AI解决方案: 1.60
 </t>
       </text>
     </comment>
@@ -8761,7 +8762,7 @@
         <t xml:space="preserve">首板涨停 11:12:22 0
 创新药+小核酸药物+医药产品
 主:创新药 次:-
-[创新药] 创新药: 3.00
+[创新药] 创新药: 3.10
 </t>
       </text>
     </comment>
@@ -8797,9 +8798,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:42:44 0
 无人机+光学镜头+机器视觉+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器视觉: 2.50
-[AI大模型] AI眼镜: 1.50
+[AI应用] AI眼镜: 1.60
 </t>
       </text>
     </comment>
@@ -8835,9 +8836,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:07:07 1
 机器人+房地产+城市更新
-主:机器人 次:大基建
+主:机器人 次:创新药
 [机器人] 机器人: 2.40
-[大基建] 房地产: 1.90
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -8856,7 +8857,7 @@
         <t xml:space="preserve">首板涨停 09:50:27 0
 牙科医疗+高低压开关设备
 主:创新药 次:-
-[创新药] 牙科医疗: 2.00
+[创新药] 牙科医疗: 2.10
 </t>
       </text>
     </comment>
@@ -8874,7 +8875,7 @@
         <t xml:space="preserve">首板涨停 10:54:15 0
 创新药+中药+摘帽+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 [国企] 国企改革: 1.10
 </t>
       </text>
@@ -8904,7 +8905,7 @@
         <t xml:space="preserve">首板涨停 09:39:33 0
 牙科医疗+永磁开关业务
 主:创新药 次:-
-[创新药] 牙科医疗: 2.00
+[创新药] 牙科医疗: 2.10
 </t>
       </text>
     </comment>
@@ -8922,9 +8923,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:12:20 0
 算力租赁+AI算力出海+DeepSeek概念+云计算
-主:算力半导体 次:AI大模型
-[算力半导体] 算力租赁: 2.40
-[AI大模型] DeepSeek概念: 1.50
+主:算力半导体 次:AI应用
+[算力半导体] 算力租赁: 2.60
+[AI应用] DeepSeek概念: 1.60
 </t>
       </text>
     </comment>
@@ -8989,7 +8990,7 @@
         <t xml:space="preserve">首板涨停 10:20:34 0
 创新药+LH-1801+科技创新债+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -9018,7 +9019,7 @@
         <t xml:space="preserve">首板涨停 11:26:57 2
 创新药+药品注册+化学制剂
 主:创新药 次:-
-[创新药] 创新药: 3.20
+[创新药] 创新药: 3.30
 </t>
       </text>
     </comment>
@@ -9027,7 +9028,7 @@
         <t xml:space="preserve">首板涨停 13:02:06 0
 创新药+中成药出口
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -9055,9 +9056,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:42:32 5
 机器人+大洋千机大模型平台+机器视觉+控制权或变更
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器视觉: 3.50
-[AI大模型] 大洋千机大模型平台: 1.90
+[AI应用] 大洋千机大模型平台: 2.00
 </t>
       </text>
     </comment>
@@ -9081,9 +9082,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:41:51 0
 数据中心+AI+HVDC产品+电源设备
-主:算力半导体 次:AI大模型
-[算力半导体] 液冷超充: 4.10
-[AI大模型] AI: 2.10
+主:算力半导体 次:AI应用
+[算力半导体] 液冷超充: 4.70
+[AI应用] AI: 1.60
 </t>
       </text>
     </comment>
@@ -9110,8 +9111,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:01:36 0
 脑机接口+POCT+微流控荧光
-主:AI大模型 次:-
-[AI大模型] 脑机接口: 1.50
+主:AI应用 次:-
+[AI应用] 脑机接口: 1.60
 </t>
       </text>
     </comment>
@@ -9159,8 +9160,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:00:54 3
 消费电子+AIoT+华为概念
-主:AI大模型 次:消费电子
-[AI大模型] AIoT: 1.50
+主:AI应用 次:消费电子
+[AI应用] AIoT: 1.60
 [消费电子] 消费电子: 1.10
 </t>
       </text>
@@ -9209,9 +9210,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:45:16 9
 创新药+数字疗法+SPD业务
-主:创新药 次:AI大模型
-[创新药] 创新药: 2.20
-[AI大模型] 脑机接口: 2.10
+主:创新药 次:AI应用
+[创新药] 创新药: 2.30
+[AI应用] 脑机接口: 2.20
 </t>
       </text>
     </comment>
@@ -9266,7 +9267,7 @@
         <t xml:space="preserve">首板涨停 13:00:12 10
 辅助生殖+独家代理+创新药
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -9284,9 +9285,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:21:12 1
 手游《超自然行动组》+AI智能体+游戏出海
-主:AI大模型 次:全球布局
-[AI大模型] AI智能体: 1.50
-[全球布局] 游戏出海: 1.10
+主:AI应用 次:新消费
+[AI应用] AI智能体: 1.60
+[新消费] 游戏出海: 1.10
 </t>
       </text>
     </comment>
@@ -9363,7 +9364,7 @@
         <t xml:space="preserve">首板涨停 13:02:45 8
 细胞治疗+民营医院 + 幽门螺杆菌
 主:创新药 次:-
-[创新药] 医疗器械: 2.20
+[创新药] 医疗器械: 2.30
 </t>
       </text>
     </comment>
@@ -9402,7 +9403,7 @@
         <t xml:space="preserve">首板涨停 09:40:57 0
 中报增长+皮肤健康+创新药
 主:创新药 次:预期改善
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [预期改善] 中报增长: 0.70
 </t>
       </text>
@@ -9490,7 +9491,7 @@
         <t xml:space="preserve">首板涨停 10:30:09 0
 中药+驱蚊液+国企
 主:创新药 次:国企
-[创新药] 中药: 2.00
+[创新药] 中药: 2.10
 [国企] 国企: 1.50
 </t>
       </text>
@@ -9509,8 +9510,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:02:27 0
 中报预增+渔业+AI应用+央企
-主:AI大模型 次:国企
-[AI大模型] AI应用: 1.50
+主:AI应用 次:国企
+[AI应用] AI应用: 1.60
 [国企] 央企: 1.10
 </t>
       </text>
@@ -9530,7 +9531,7 @@
         <t xml:space="preserve">首板涨停 13:13:48 1
 创新药+高温合金
 主:创新药 次:军工
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [军工] 大飞机: 1.70
 </t>
       </text>
@@ -9577,9 +9578,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:21:51 0
 AI算力需求+数据中心市场+电网设备
-主:算力半导体 次:AI大模型
-[算力半导体] 数据中心: 3.00
-[AI大模型] AI算力需求: 1.70
+主:算力半导体 次:电力
+[算力半导体] 数据中心: 3.40
+[电力] 电网设备: 1.30
 </t>
       </text>
     </comment>
@@ -9648,7 +9649,7 @@
         <t xml:space="preserve">首板涨停 09:30:24 7
 创新药+新药获批+减肥药
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -9746,7 +9747,7 @@
         <t xml:space="preserve">首板涨停 10:32:25 0
 创新药+特医食品+医药百强
 主:创新药 次:传统消费
-[创新药] 创新药: 3.40
+[创新药] 创新药: 3.50
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -9784,7 +9785,7 @@
         <t xml:space="preserve">首板涨停 13:36:33 0
 中药+药品再注册+国企改革+中报增长
 主:创新药 次:国企
-[创新药] 中药: 2.20
+[创新药] 中药: 2.30
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -9851,9 +9852,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:09:00 4
 脑机接口+AI医疗+综合医疗
-主:AI大模型 次:创新药
-[AI大模型] 脑机接口: 3.30
-[创新药] 综合医疗: 2.40
+主:AI应用 次:创新药
+[AI应用] 脑机接口: 3.40
+[创新药] 综合医疗: 2.50
 </t>
       </text>
     </comment>
@@ -9890,8 +9891,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:31:12 4
 新剧上线+短剧出海+Rokid合作+国企
-主:AI大模型 次:全球布局
-[AI大模型] Rokid合作(AI眼镜): 1.50
+主:AI应用 次:全球布局
+[AI应用] Rokid合作(AI眼镜): 1.60
 [全球布局] 短剧出海: 1.30
 </t>
       </text>
@@ -9936,8 +9937,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:46:49 0
 脑机接口（已澄清）+农批市场+特医食品+国企改革
-主:AI大模型 次:传统消费
-[AI大模型] 脑机接口（已澄清）: 2.30
+主:AI应用 次:传统消费
+[AI应用] 脑机接口（已澄清）: 2.40
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -9985,8 +9986,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:32:42 0
 智能终端+AI布局+一季报增长
-主:AI大模型 次:预期改善
-[AI大模型] AI布局: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI布局: 1.60
 [预期改善] 一季报增长: 0.70
 </t>
       </text>
@@ -10044,7 +10045,7 @@
         <t xml:space="preserve">首板涨停 13:14:24 0
 创新药+回购+降脂新药进展
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -10053,7 +10054,7 @@
         <t xml:space="preserve">首板涨停 13:03:54 0
 肿瘤医疗+水暖阀门+亏损收窄
 主:创新药 次:-
-[创新药] 肿瘤医疗: 1.60
+[创新药] 肿瘤医疗: 1.70
 </t>
       </text>
     </comment>
@@ -10082,7 +10083,7 @@
         <t xml:space="preserve">首板涨停 11:26:57 0
 基因修饰动物模型+辅助生殖+股东增持
 主:创新药 次:预期改善
-[创新药] 医疗服务: 1.60
+[创新药] 医疗服务: 1.70
 [预期改善] 股东增持: 0.70
 </t>
       </text>
@@ -10190,8 +10191,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:49:15 3
 AI芯片+控制权变更+人造石英石
-主:AI大模型 次:-
-[AI大模型] AI芯片: 1.50
+主:算力半导体 次:-
+[算力半导体] AI芯片: 2.90
 </t>
       </text>
     </comment>
@@ -10209,9 +10210,9 @@
       <text>
         <t xml:space="preserve">2天2板 09:31:27 2
 水务建设+AI水科技+深圳国资
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -10219,8 +10220,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:25:48 4
 区块链+航运数字化+AI大模型+央企
-主:AI大模型 次:数字经济
-[AI大模型] AI大模型: 1.50
+主:AI应用 次:数字经济
+[AI应用] AI大模型: 1.60
 [数字经济] 区块链: 1.10
 </t>
       </text>
@@ -10239,8 +10240,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:38:52 0
 股东回馈+按摩器具+机器人概念
-主:AI大模型 次:机器人
-[AI大模型] 脑机接口: 2.30
+主:AI应用 次:机器人
+[AI应用] 脑机接口: 2.40
 [机器人] 机器人概念: 2.00
 </t>
       </text>
@@ -10249,8 +10250,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:46:24 5
 中报预增+AI产品+PCB
-主:AI大模型 次:精密电子
-[AI大模型] AI产品: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI产品: 1.60
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -10285,8 +10286,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:16:06 0
 数据要素+AI+央国企
-主:AI大模型 次:国企
-[AI大模型] AI: 1.50
+主:AI应用 次:国企
+[AI应用] AI: 1.60
 [国企] 央国企: 1.10
 </t>
       </text>
@@ -10295,8 +10296,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:16:46 0
 军工+低空经济+AI技术
-主:AI大模型 次:军工
-[AI大模型] AI技术: 1.50
+主:AI应用 次:军工
+[AI应用] AI技术: 1.60
 [军工] 军工: 1.50
 </t>
       </text>
@@ -10394,7 +10395,7 @@
         <t xml:space="preserve">首板涨停 09:32:42 0
 创新药+国际拓展+原料药制剂一体化
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -10402,8 +10403,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:33:27 0
 华为概念+AIPC+背光模组
-主:AI大模型 次:华为概念
-[AI大模型] AIPC: 1.50
+主:AI应用 次:华为概念
+[AI应用] AIPC: 1.60
 [华为概念] 华为概念: 1.00
 </t>
       </text>
@@ -10441,8 +10442,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:49:45 4
 公布半年报+AI多模态+IP优势
-主:AI大模型 次:新消费
-[AI大模型] AI多模态: 1.50
+主:AI应用 次:新消费
+[AI应用] AI多模态: 1.60
 [新消费] IP优势: 1.10
 </t>
       </text>
@@ -10490,8 +10491,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:41:45 0
 RWA+RFID+中报增长
-主:AI大模型 次:数字经济
-[AI大模型] AI赋能: 1.50
+主:AI应用 次:数字经济
+[AI应用] AI赋能: 1.60
 [数字经济] RWA: 1.30
 </t>
       </text>
@@ -10615,8 +10616,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:50:45 12
 石化物流+投资基金（人工智能）+武汉二期
-主:AI大模型 次:无人经济
-[AI大模型] 投资基金（人工智能）: 1.50
+主:AI应用 次:无人经济
+[AI应用] 投资基金（人工智能）: 1.60
 [无人经济] 石化物流: 1.10
 </t>
       </text>
@@ -10625,8 +10626,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:49:42 0
 PCB+光模块+AI应用
-主:AI大模型 次:精密电子
-[AI大模型] AI应用: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI应用: 1.60
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -10645,8 +10646,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:34:23 0
 覆铜板+AI服务器+中报预增
-主:AI大模型 次:新型能源
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:新型能源
+[AI应用] AI服务器: 1.60
 [新型能源] 固态电池: 1.20
 </t>
       </text>
@@ -10714,9 +10715,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:00:51 0
 数据中心+算力+AI应用+视频会议
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 数据中心: 2.60
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -10926,9 +10927,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:55:00 0
 股份注销+建筑陶瓷+AI
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 数据中心: 2.40
-[AI大模型] AI: 1.70
+[AI应用] AI: 1.80
 </t>
       </text>
     </comment>
@@ -10957,7 +10958,7 @@
         <t xml:space="preserve">首板涨停 13:10:42 5
 农药+合成生物+湖南国资
 主:创新药 次:农业
-[创新药] 合成生物: 1.60
+[创新药] 合成生物: 1.70
 [农业] 农药: 1.10
 </t>
       </text>
@@ -11031,9 +11032,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:12:12 0
 AI智能体+文化大数据+电视广播+国企改革
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.40
-[AI大模型] AI智能体: 1.70
+[AI应用] AI智能体: 1.80
 </t>
       </text>
     </comment>
@@ -11051,9 +11052,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:15:24 0
 半导体+AI+智慧供热+磁悬浮离心式压缩机
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 半导体: 2.40
-[AI大模型] AI: 1.50
+[AI应用] AI: 1.60
 </t>
       </text>
     </comment>
@@ -11062,7 +11063,7 @@
         <t xml:space="preserve">首板涨停 13:01:15 0
 创新药+小核酸药物+心血管系统类
 主:创新药 次:-
-[创新药] 创新药: 3.00
+[创新药] 创新药: 3.10
 </t>
       </text>
     </comment>
@@ -11100,8 +11101,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:26:38 0
 脑机接口+智能制造+央企
-主:AI大模型 次:国企
-[AI大模型] 脑机接口: 1.50
+主:AI应用 次:国企
+[AI应用] 脑机接口: 1.60
 [国企] 央企: 1.10
 </t>
       </text>
@@ -11110,8 +11111,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:59:09 2
 树图+数据要素+数字政府+AI
-主:AI大模型 次:-
-[AI大模型] AI: 1.70
+主:AI应用 次:-
+[AI应用] AI: 1.80
 </t>
       </text>
     </comment>
@@ -11120,7 +11121,7 @@
         <t xml:space="preserve">首板涨停 09:33:30 6
 MASH药物合作+无创检测权威认可+自有药品高增长
 主:创新药 次:-
-[创新药] 自有药品高增长: 1.80
+[创新药] 自有药品高增长: 1.90
 </t>
       </text>
     </comment>
@@ -11253,7 +11254,7 @@
         <t xml:space="preserve">首板涨停 13:12:33 0
 西瓜霜+主营优势+创新药进展
 主:创新药 次:-
-[创新药] 创新药进展: 1.60
+[创新药] 创新药进展: 1.70
 </t>
       </text>
     </comment>
@@ -11308,9 +11309,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:44:57 0
 机器人+AI应用+智能交通
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.20
-[AI大模型] AI应用: 1.70
+[AI应用] AI应用: 1.80
 </t>
       </text>
     </comment>
@@ -11328,8 +11329,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:01:06 2
 细胞膜色谱+海洋经济+人工智能+中报增长
-主:AI大模型 次:预期改善
-[AI大模型] 人工智能: 1.70
+主:AI应用 次:预期改善
+[AI应用] 人工智能: 1.80
 [预期改善] 中报增长: 0.90
 </t>
       </text>
@@ -11348,7 +11349,7 @@
         <t xml:space="preserve">首板涨停 09:37:32 0
 创新药+细胞免疫治疗+养老概念
 主:创新药 次:预期改善
-[创新药] 创新药: 2.60
+[创新药] 创新药: 2.70
 [预期改善] 年报增长: 0.70
 </t>
       </text>
@@ -11367,9 +11368,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:55:46 2
 半导体设备+AI需求+业绩增长
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 半导体设备: 2.40
-[AI大模型] AI需求: 1.50
+[AI应用] AI需求: 1.60
 </t>
       </text>
     </comment>
@@ -11434,8 +11435,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:07:37 1
 AI服务器+PCB+光模块+国企改革
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 2.10
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 2.20
 [精密电子] PCB: 1.70
 </t>
       </text>
@@ -11539,8 +11540,8 @@
       <text>
         <t xml:space="preserve">首板涨停 09:35:06 2
 影视制作+AI应用+国企改革
-主:AI大模型 次:国企
-[AI大模型] AI应用: 1.50
+主:AI应用 次:国企
+[AI应用] AI应用: 1.60
 [国企] 国企改革: 1.10
 </t>
       </text>
@@ -11643,7 +11644,7 @@
         <t xml:space="preserve">首板涨停 14:48:15 0
 创新药+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 [国企] 国企改革: 1.30
 </t>
       </text>
@@ -11701,8 +11702,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:06:41 0
 脑机接口+AI大模型+股权投资基金
-主:AI大模型 次:机器人
-[AI大模型] 脑机接口: 2.30
+主:AI应用 次:机器人
+[AI应用] 脑机接口: 2.40
 [机器人] 机器人概念: 2.00
 </t>
       </text>
@@ -11711,9 +11712,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:15:00 27
 收入传言+国产算力芯片+大模型合作+一季报增长
-主:算力半导体 次:AI大模型
-[算力半导体] 国产算力芯片: 2.40
-[AI大模型] 大模型合作: 1.70
+主:算力半导体 次:AI应用
+[算力半导体] AI芯片: 3.10
+[AI应用] 大模型合作: 1.60
 </t>
       </text>
     </comment>
@@ -11731,9 +11732,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:08:22 0
 人形机器人+新能源汽车+脑机接口
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 人形机器人: 2.50
-[AI大模型] 脑机接口: 1.50
+[AI应用] 脑机接口: 1.60
 </t>
       </text>
     </comment>
@@ -11751,9 +11752,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:38:35 1
 房地产+创新药+机器人
-主:机器人 次:大基建
+主:机器人 次:创新药
 [机器人] 机器人: 2.40
-[大基建] 房地产: 1.90
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -11825,7 +11826,7 @@
         <t xml:space="preserve">首板涨停 13:03:24 29
 GSK合作+创新药+国际化+研发管线
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -11844,7 +11845,7 @@
         <t xml:space="preserve">首板涨停 13:46:09 0
 创新药+LH-1801+科技创新债+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -11883,7 +11884,7 @@
         <t xml:space="preserve">首板涨停 13:11:00 0
 大飞机+高温合金+创新药+股权激励
 主:创新药 次:军工
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [军工] 大飞机: 1.70
 </t>
       </text>
@@ -11892,8 +11893,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:06:57 2
 AI服务器电源+英伟达概念+海外拓展
-主:AI大模型 次:预期改善
-[AI大模型] AI服务器电源: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI服务器电源: 1.60
 [预期改善] 海外拓展: 0.70
 </t>
       </text>
@@ -11967,8 +11968,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:03:39 1
 影视制作+AIGC+腾讯概念
-主:AI大模型 次:大金融
-[AI大模型] AIGC: 1.50
+主:AI应用 次:大金融
+[AI应用] AIGC: 1.60
 [大金融] 腾讯概念: 1.10
 </t>
       </text>
@@ -12062,9 +12063,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:27:32 0
 砺算科技+GPU+存算联一体化
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 存储芯片: 2.80
-[AI大模型] AI终端: 1.70
+[AI应用] AI终端: 1.80
 </t>
       </text>
     </comment>
@@ -12073,7 +12074,7 @@
         <t xml:space="preserve">首板涨停 13:15:31 5
 中报预增+JH389进展+特色原料药
 主:创新药 次:预期改善
-[创新药] 特色原料药: 1.80
+[创新药] 特色原料药: 1.90
 [预期改善] 中报预增: 0.90
 </t>
       </text>
@@ -12082,9 +12083,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:10:33 0
 工业级四足机器人+AI教育+智能控制部件
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 工业级四足机器人: 2.00
-[AI大模型] AI教育: 1.50
+[AI应用] AI教育: 1.60
 </t>
       </text>
     </comment>
@@ -12092,8 +12093,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:34:00 5
 收购+AI计算
-主:AI大模型 次:-
-[AI大模型] AI计算: 1.50
+主:AI应用 次:-
+[AI应用] AI计算: 1.60
 </t>
       </text>
     </comment>
@@ -12141,8 +12142,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:08:27 0
 参股灵伴智能（AI应用）+纺织梳理器材+国企改革
-主:AI大模型 次:化工
-[AI大模型] 参股灵伴智能（AI应用）: 1.50
+主:AI应用 次:化工
+[AI应用] 参股灵伴智能（AI应用）: 1.60
 [化工] 纺织梳理器材: 1.10
 </t>
       </text>
@@ -12221,7 +12222,7 @@
         <t xml:space="preserve">首板涨停 14:08:45 3
 基因修饰动物模型+医疗服务
 主:创新药 次:预期改善
-[创新药] 医疗服务: 1.60
+[创新药] 医疗服务: 1.70
 [预期改善] 股东增持: 0.70
 </t>
       </text>
@@ -12230,9 +12231,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:00:06 0
 脑机接口+AI医疗+综合医疗
-主:AI大模型 次:创新药
-[AI大模型] 脑机接口: 3.30
-[创新药] 综合医疗: 2.40
+主:AI应用 次:创新药
+[AI应用] 脑机接口: 3.40
+[创新药] 综合医疗: 2.50
 </t>
       </text>
     </comment>
@@ -12318,7 +12319,7 @@
         <t xml:space="preserve">首板涨停 09:44:51 0
 中报亏损收窄+创新药+中药
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -12326,9 +12327,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:10:06 0
 机器人+AI专网+专用通信
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.00
-[AI大模型] AI专网: 1.50
+[AI应用] AI专网: 1.60
 </t>
       </text>
     </comment>
@@ -12347,7 +12348,7 @@
         <t xml:space="preserve">首板涨停 10:06:00 0
 创新药+化学制药+药品获批
 主:创新药 次:-
-[创新药] 创新药: 3.20
+[创新药] 创新药: 3.30
 </t>
       </text>
     </comment>
@@ -12376,7 +12377,7 @@
         <t xml:space="preserve">首板涨停 14:50:06 0
 创新药+仲裁解决+新品推广
 主:创新药 次:-
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 </t>
       </text>
     </comment>
@@ -12393,8 +12394,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:24:57 3
 AI服务器+PCB+一季报增长
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 1.60
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -12492,9 +12493,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:40:15 0
 男装+AI新零售+回购+机器人概念
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.20
-[AI大模型] AI新零售: 1.70
+[AI应用] AI新零售: 1.80
 </t>
       </text>
     </comment>
@@ -12503,7 +12504,7 @@
         <t xml:space="preserve">首板涨停 09:45:03 0
 减肥药服务+创新药CRO+订单增长
 主:创新药 次:预期改善
-[创新药] 创新药CRO: 1.60
+[创新药] 创新药CRO: 1.70
 [预期改善] 订单增长: 0.70
 </t>
       </text>
@@ -12532,8 +12533,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:09:51 0
 华润入主+PCB+AI眼镜+亏损收窄
-主:AI大模型 次:精密电子
-[AI大模型] AI眼镜: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI眼镜: 1.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -12582,8 +12583,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:20:36 0
 低代码平台+实验室管理系统+国家电网+AI应用
-主:AI大模型 次:传统消费
-[AI大模型] AI应用: 1.50
+主:AI应用 次:传统消费
+[AI应用] AI应用: 1.60
 [传统消费] 国家电网: 1.10
 </t>
       </text>
@@ -12602,9 +12603,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:43:13 0
 安保运营服务+智能安防+AI应用
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.40
-[AI大模型] AI应用: 1.70
+[AI应用] AI应用: 1.80
 </t>
       </text>
     </comment>
@@ -12612,9 +12613,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:07:46 0
 数据中心+蚂蚁金服概念+AI应用+IT运维
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 数据中心: 2.40
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -12681,7 +12682,7 @@
         <t xml:space="preserve">首板涨停 09:45:43 0
 中报预增+氨糖+超级鱼油
 主:创新药 次:预期改善
-[创新药] 海洋医药: 1.80
+[创新药] 海洋医药: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -12700,8 +12701,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:22:24 0
 半年报增长+PCB钻针+AI需求+产能扩张
-主:AI大模型 次:精密电子
-[AI大模型] AI需求: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI需求: 1.60
 [精密电子] PCB钻针: 1.10
 </t>
       </text>
@@ -12719,9 +12720,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:32:12 0
 水务建设+AI水科技+国企改革
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -12749,8 +12750,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:29:21 35
 PCB+AI算力+封装基板+央企
-主:AI大模型 次:精密电子
-[AI大模型] AI算力: 1.70
+主:算力半导体 次:精密电子
+[算力半导体] AI算力: 2.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -12760,7 +12761,7 @@
         <t xml:space="preserve">首板涨停 14:23:21 0
 固态电池+创新药+一季报增长
 主:创新药 次:新型能源
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [新型能源] 固态电池: 1.20
 </t>
       </text>
@@ -12825,9 +12826,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:35:30 0
 数据中心+AI算力+液冷超充
-主:算力半导体 次:AI大模型
-[算力半导体] 液冷超充: 4.10
-[AI大模型] AI: 2.10
+主:算力半导体 次:AI应用
+[算力半导体] 液冷超充: 4.70
+[AI应用] AI: 1.60
 </t>
       </text>
     </comment>
@@ -12845,9 +12846,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:49:03 2
 液冷服务器+AIoT+数据中心节能
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷服务器: 3.10
-[AI大模型] AIoT: 1.50
+[AI应用] AIoT: 1.60
 </t>
       </text>
     </comment>
@@ -12981,9 +12982,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:09:37 3
 AI服务器材料+光刻胶试产+英伟达概念
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 光刻胶试产: 2.80
-[AI大模型] AI服务器材料: 1.90
+[AI应用] AI服务器材料: 2.00
 </t>
       </text>
     </comment>
@@ -13028,8 +13029,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:02:12 1
 AI智能体+新生儿基因检测+生育健康+DeepSeek概念
-主:AI大模型 次:-
-[AI大模型] AI智能体: 1.70
+主:AI应用 次:-
+[AI应用] AI智能体: 1.80
 </t>
       </text>
     </comment>
@@ -13121,7 +13122,7 @@
         <t xml:space="preserve">首板涨停 10:27:33 0
 控制权变更+中药+智能医疗
 主:创新药 次:-
-[创新药] 中药: 1.80
+[创新药] 中药: 1.90
 </t>
       </text>
     </comment>
@@ -13169,7 +13170,7 @@
         <t xml:space="preserve">首板涨停 10:33:45 11
 阶跃星辰相关+汽车电子+医疗器械+上海国企
 主:创新药 次:消费电子
-[创新药] 医疗器械: 2.40
+[创新药] 医疗器械: 2.50
 [消费电子] 汽车电子: 1.90
 </t>
       </text>
@@ -13247,9 +13248,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:58:25 0
 机器人系统首发+AI视频技术+华为昇腾
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人系统首发: 2.00
-[AI大模型] AI视频技术: 1.50
+[AI应用] AI视频技术: 1.60
 </t>
       </text>
     </comment>
@@ -13317,7 +13318,7 @@
         <t xml:space="preserve">首板涨停 09:56:10 0
 中药+医药商业+控制权变更
 主:创新药 次:-
-[创新药] 中药: 1.80
+[创新药] 中药: 1.90
 </t>
       </text>
     </comment>
@@ -13432,9 +13433,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:56:30 0
 AI应用+数据中心+储能+液冷技术
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷技术: 3.50
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -13472,8 +13473,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:05:05 1
 中报增长+吸收合并+AI算力
-主:AI大模型 次:预期改善
-[AI大模型] AI算力: 1.50
+主:算力半导体 次:预期改善
+[算力半导体] AI算力: 2.40
 [预期改善] 中报增长: 0.70
 </t>
       </text>
@@ -13512,8 +13513,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:09:37 0
 洗护产品+日化板块上涨
-主:AI大模型 次:-
-[AI大模型] AI合作: 1.50
+主:AI应用 次:-
+[AI应用] AI合作: 1.60
 </t>
       </text>
     </comment>
@@ -13531,7 +13532,7 @@
         <t xml:space="preserve">首板涨停 14:09:58 1
 阶跃星辰相关+汽车电子+医疗器械+上海国企
 主:创新药 次:消费电子
-[创新药] 医疗器械: 2.40
+[创新药] 医疗器械: 2.50
 [消费电子] 汽车电子: 1.90
 </t>
       </text>
@@ -13540,9 +13541,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:59:48 5
 水利+雅下水电概念+深海科技+深圳国资
-主:西部开发 次:AI大模型
+主:西部开发 次:AI应用
 [西部开发] 水利: 2.40
-[AI大模型] AI水科技: 2.30
+[AI应用] AI水科技: 2.40
 </t>
       </text>
     </comment>
@@ -13560,8 +13561,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:56:24 0
 职业教育+AI教育+信创
-主:AI大模型 次:-
-[AI大模型] AI教育: 1.50
+主:AI应用 次:-
+[AI应用] AI教育: 1.60
 </t>
       </text>
     </comment>
@@ -13608,9 +13609,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:12:54 0
 AI服务器材料+光刻胶试产+英伟达概念
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 光刻胶试产: 2.80
-[AI大模型] AI服务器材料: 1.90
+[AI应用] AI服务器材料: 2.00
 </t>
       </text>
     </comment>
@@ -13665,8 +13666,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:42:13 0
 军需品+脑机接口+核污染防治+国企
-主:AI大模型 次:国企
-[AI大模型] 脑机接口: 1.70
+主:AI应用 次:国企
+[AI应用] 脑机接口: 1.80
 [国企] 国企: 1.30
 </t>
       </text>
@@ -13675,8 +13676,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:05:42 0
 社保卡+数字人民币+跨境支付+AI Agent
-主:AI大模型 次:数字经济
-[AI大模型] AI Agent: 1.50
+主:AI应用 次:数字经济
+[AI应用] AI Agent: 1.60
 [数字经济] 数字人民币: 1.10
 </t>
       </text>
@@ -13713,7 +13714,7 @@
         <t xml:space="preserve">首板涨停 09:55:35 0
 创新药+CRO+年报增长
 主:创新药 次:预期改善
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [预期改善] 年报增长: 0.70
 </t>
       </text>
@@ -13769,7 +13770,7 @@
         <t xml:space="preserve">2天2板 13:27:42 3
 创新药+特医食品+医药百强
 主:创新药 次:传统消费
-[创新药] 创新药: 3.40
+[创新药] 创新药: 3.50
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -13779,7 +13780,7 @@
         <t xml:space="preserve">首板涨停 11:10:45 0
 海南自贸区+创新药+央企+亏损收窄
 主:创新药 次:国企
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [国企] 央企: 1.10
 </t>
       </text>
@@ -13798,8 +13799,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:45:24 0
 物理AI+具身智能+空间计算+参股芯明智能
-主:AI大模型 次:-
-[AI大模型] 物理AI: 1.50
+主:AI应用 次:-
+[AI应用] 物理AI: 1.60
 </t>
       </text>
     </comment>
@@ -13856,8 +13857,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:11:33 0
 鸿蒙概念+华为海思概念股+信创+AI智能体
-主:AI大模型 次:华为概念
-[AI大模型] AI智能体: 1.50
+主:AI应用 次:华为概念
+[AI应用] AI智能体: 1.60
 [华为概念] 鸿蒙概念: 1.20
 </t>
       </text>
@@ -13876,9 +13877,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:28:03 0
 AI应用+短剧+芯片突破
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 芯片突破: 2.40
-[AI大模型] AI应用: 1.50
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -13953,7 +13954,7 @@
         <t xml:space="preserve">首板涨停 11:07:40 1
 创新药+临床进展+商业化推进
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -13980,8 +13981,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:19:42 0
 RFID+AI赋能+无人机+RWA
-主:AI大模型 次:数字经济
-[AI大模型] AI赋能: 1.50
+主:AI应用 次:数字经济
+[AI应用] AI赋能: 1.60
 [数字经济] RWA: 1.30
 </t>
       </text>
@@ -14069,8 +14070,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:03:24 0
 华为战略合作+智行云枢平台+智慧高速网络+并购重组预期
-主:AI大模型 次:无人经济
-[AI大模型] AI智能助手: 1.50
+主:AI应用 次:无人经济
+[AI应用] AI智能助手: 1.60
 [无人经济] 无人驾驶: 1.10
 </t>
       </text>
@@ -14099,8 +14100,8 @@
       <text>
         <t xml:space="preserve">首板涨停 10:00:24 5
 一季报增长+短剧+IP经济+AIGC
-主:AI大模型 次:新消费
-[AI大模型] AIGC: 1.50
+主:AI应用 次:新消费
+[AI应用] AIGC: 1.60
 [新消费] IP经济: 1.10
 </t>
       </text>
@@ -14184,8 +14185,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:05:09 10
 华润入主+PCB+亏损收窄
-主:AI大模型 次:精密电子
-[AI大模型] AI眼镜: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI眼镜: 1.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -14287,9 +14288,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:10:39 1
 半年报增长+AI服务器电源+机器人概念+小米汽车
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.40
-[AI大模型] AI服务器电源: 1.90
+[AI应用] AI服务器电源: 2.00
 </t>
       </text>
     </comment>
@@ -14297,9 +14298,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:18:45 0
 智慧医疗+云计算+华为+AI应用
-主:创新药 次:AI大模型
-[创新药] 智慧医疗: 1.60
-[AI大模型] AI应用: 1.50
+主:创新药 次:AI应用
+[创新药] 智慧医疗: 1.70
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -14354,7 +14355,7 @@
         <t xml:space="preserve">首板涨停 13:03:12 0
 中药+大健康+中报增长+国企改革
 主:创新药 次:国企
-[创新药] 中药: 2.20
+[创新药] 中药: 2.30
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -14390,8 +14391,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:19:12 0
 AI电源+泰国工厂产能扩张+供货台达电子
-主:AI大模型 次:-
-[AI大模型] AI电源: 1.50
+主:AI应用 次:-
+[AI应用] AI电源: 1.60
 </t>
       </text>
     </comment>
@@ -14399,9 +14400,9 @@
       <text>
         <t xml:space="preserve">首板涨停 11:19:49 16
 人形机器人+AI缝纫机+外销
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 人形机器人: 2.50
-[AI大模型] AI缝纫机: 1.50
+[AI应用] AI缝纫机: 1.60
 </t>
       </text>
     </comment>
@@ -14446,8 +14447,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:04:25 0
 AI财税+DeepSeek概念+区块链+中报营收增
-主:AI大模型 次:数字经济
-[AI大模型] AI财税: 1.70
+主:AI应用 次:数字经济
+[AI应用] AI财税: 1.80
 [数字经济] 区块链: 1.10
 </t>
       </text>
@@ -14456,9 +14457,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:03:21 0
 数字货币+跨境支付+AI金融
-主:数字经济 次:全球布局
+主:AI应用 次:数字经济
+[AI应用] AI金融: 1.60
 [数字经济] 数字货币: 1.10
-[全球布局] 跨境支付: 1.10
 </t>
       </text>
     </comment>
@@ -14487,7 +14488,7 @@
         <t xml:space="preserve">首板涨停 13:21:09 4
 疫苗研发+自研管线进展+经营风险改善
 主:创新药 次:-
-[创新药] 疫苗研发: 1.60
+[创新药] 疫苗研发: 1.70
 </t>
       </text>
     </comment>
@@ -14515,8 +14516,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:23:20 1
 AI服务器+PCB+国企改革
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 2.10
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 2.20
 [精密电子] PCB: 1.70
 </t>
       </text>
@@ -14555,9 +14556,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:17:04 4
 创新药+脑科学+SPD业务
-主:创新药 次:AI大模型
-[创新药] 创新药: 2.20
-[AI大模型] 脑机接口: 2.10
+主:创新药 次:AI应用
+[创新药] 创新药: 2.30
+[AI应用] 脑机接口: 2.20
 </t>
       </text>
     </comment>
@@ -14566,7 +14567,7 @@
         <t xml:space="preserve">首板涨停 13:06:39 17
 创新药+CAR-T研究+医保销售
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -14766,9 +14767,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:35:52 0
 AI芯片+定增获批+一季报增长
-主:算力半导体 次:AI大模型
-[算力半导体] 国产算力芯片: 2.40
-[AI大模型] 大模型合作: 1.70
+主:算力半导体 次:AI应用
+[算力半导体] AI芯片: 3.10
+[AI应用] 大模型合作: 1.60
 </t>
       </text>
     </comment>
@@ -14805,9 +14806,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:30:23 1
 口腔医疗+AI应用+一季报增长
-主:创新药 次:AI大模型
-[创新药] 口腔医疗: 1.60
-[AI大模型] AI应用: 1.50
+主:创新药 次:AI应用
+[创新药] 口腔医疗: 1.70
+[AI应用] AI应用: 1.60
 </t>
       </text>
     </comment>
@@ -14815,9 +14816,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:09:33 0
 创新药+脑机接口+AI医疗+SPD业务
-主:创新药 次:AI大模型
-[创新药] 创新药: 2.20
-[AI大模型] 脑机接口: 2.10
+主:创新药 次:AI应用
+[创新药] 创新药: 2.30
+[AI应用] 脑机接口: 2.20
 </t>
       </text>
     </comment>
@@ -14844,9 +14845,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:04:36 1
 AI营销+液冷用泵+华为概念
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷用泵: 3.10
-[AI大模型] AI营销: 1.70
+[AI应用] AI营销: 1.80
 </t>
       </text>
     </comment>
@@ -14873,9 +14874,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:52:59 0
 AI芯片+脑机接口+机器人概念+国企改革
-主:机器人 次:AI大模型
+主:算力半导体 次:机器人
+[算力半导体] AI芯片: 2.90
 [机器人] 机器人概念: 2.00
-[AI大模型] AI芯片: 1.70
 </t>
       </text>
     </comment>
@@ -14903,9 +14904,9 @@
       <text>
         <t xml:space="preserve">首板涨停 09:36:20 0
 高速铜缆+AI服务器+藕芯结构
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 高速铜缆: 2.80
-[AI大模型] AI服务器: 1.90
+[AI应用] AI服务器: 2.00
 </t>
       </text>
     </comment>
@@ -14924,7 +14925,7 @@
 机器人概念+无框电机研发+医疗器械+小米概念
 主:机器人 次:创新药
 [机器人] 机器人概念: 2.00
-[创新药] 医疗器械: 1.60
+[创新药] 医疗器械: 1.70
 </t>
       </text>
     </comment>
@@ -14932,9 +14933,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:09:06 0
 建筑陶瓷+AI+数据中心
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 数据中心: 2.40
-[AI大模型] AI: 1.70
+[AI应用] AI: 1.80
 </t>
       </text>
     </comment>
@@ -14969,9 +14970,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:25:51 1
 优先审评+原料药制剂一体化+创新药+AI制药
-主:创新药 次:AI大模型
-[创新药] 原料药制剂一体化: 1.80
-[AI大模型] AI制药: 1.50
+主:创新药 次:AI应用
+[创新药] 原料药制剂一体化: 1.90
+[AI应用] AI制药: 1.60
 </t>
       </text>
     </comment>
@@ -14979,8 +14980,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:54:33 0
 亏损收窄+AI算力+智算服务
-主:AI大模型 次:-
-[AI大模型] AI算力: 1.50
+主:算力半导体 次:-
+[算力半导体] AI算力: 2.40
 </t>
       </text>
     </comment>
@@ -15018,9 +15019,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:57:01 2
 机器视觉+机器人+大洋千机大模型平台+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器视觉: 3.50
-[AI大模型] 大洋千机大模型平台: 1.90
+[AI应用] 大洋千机大模型平台: 2.00
 </t>
       </text>
     </comment>
@@ -15028,9 +15029,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:28:51 18
 算力+AI游戏+全球化卡牌+中报预增
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.60
-[AI大模型] AI游戏: 1.70
+[AI应用] AI游戏: 1.80
 </t>
       </text>
     </comment>
@@ -15058,7 +15059,7 @@
         <t xml:space="preserve">首板涨停 10:07:40 0
 创新药+中报预增+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 [国企] 国企改革: 1.10
 </t>
       </text>
@@ -15160,8 +15161,8 @@
       <text>
         <t xml:space="preserve">首板涨停 11:28:02 0
 电极箔+可应用AI服务器
-主:AI大模型 次:-
-[AI大模型] 可应用AI服务器: 1.50
+主:AI应用 次:-
+[AI应用] 可应用AI服务器: 1.60
 </t>
       </text>
     </comment>
@@ -15316,7 +15317,7 @@
         <t xml:space="preserve">首板涨停 14:02:57 0
 创新药+临床进展+中药主业
 主:创新药 次:-
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 </t>
       </text>
     </comment>
@@ -15335,7 +15336,7 @@
         <t xml:space="preserve">首板涨停 13:10:44 25
 动物疫苗+多联多价疫苗+创新药+回购
 主:创新药 次:-
-[创新药] 动物疫苗: 3.60
+[创新药] 动物疫苗: 3.70
 </t>
       </text>
     </comment>
@@ -15370,8 +15371,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:08:44 1
 PCB+AI服务器+扩产
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 1.60
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -15429,9 +15430,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:17:43 0
 安保运营服务+智能安防+算力+AI应用
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 算力: 2.40
-[AI大模型] AI应用: 1.70
+[AI应用] AI应用: 1.80
 </t>
       </text>
     </comment>
@@ -15469,7 +15470,7 @@
         <t xml:space="preserve">首板涨停 09:53:46 3
 创新药+特医食品+医药百强
 主:创新药 次:传统消费
-[创新药] 创新药: 3.40
+[创新药] 创新药: 3.50
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -15507,8 +15508,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:45:29 0
 PCB+先进封装+AI复苏
-主:AI大模型 次:精密电子
-[AI大模型] AI复苏: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI复苏: 1.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -15535,9 +15536,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:51:09 0
 AI服务器+国产算力+一季报增长
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 国产算力: 2.40
-[AI大模型] AI服务器: 1.50
+[AI应用] AI服务器: 1.60
 </t>
       </text>
     </comment>
@@ -15574,8 +15575,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:37:02 0
 脑机接口（已澄清）+农批市场+特医食品+国企改革
-主:AI大模型 次:传统消费
-[AI大模型] 脑机接口（已澄清）: 2.30
+主:AI应用 次:传统消费
+[AI应用] 脑机接口（已澄清）: 2.40
 [传统消费] 特医食品: 1.90
 </t>
       </text>
@@ -15593,8 +15594,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:46:12 1
 覆铜板+中报预增+AI材料
-主:AI大模型 次:预期改善
-[AI大模型] AI材料: 1.50
+主:AI应用 次:预期改善
+[AI应用] AI材料: 1.60
 [预期改善] 中报预增: 0.70
 </t>
       </text>
@@ -15623,8 +15624,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:54:24 0
 AI智能体+仪器仪表+核污染防治+光伏概念
-主:AI大模型 次:新型能源
-[AI大模型] AI智能体: 1.70
+主:AI应用 次:新型能源
+[AI应用] AI智能体: 1.80
 [新型能源] 光伏概念: 1.20
 </t>
       </text>
@@ -15799,7 +15800,7 @@
         <t xml:space="preserve">首板涨停 13:58:18 0
 中报预增+PCB+动物疫苗
 主:创新药 次:精密电子
-[创新药] 动物疫苗: 1.60
+[创新药] 动物疫苗: 1.70
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -15839,7 +15840,7 @@
         <t xml:space="preserve">首板涨停 14:01:51 0
 创新药+独家品种+心脑血管在研项目
 主:创新药 次:-
-[创新药] 中药: 2.40
+[创新药] 中药: 2.50
 </t>
       </text>
     </comment>
@@ -15887,9 +15888,9 @@
       <text>
         <t xml:space="preserve">首板涨停 10:20:57 36
 固态电池+机器人概念+AI端侧+中报预增
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人概念: 2.00
-[AI大模型] AI端侧: 1.50
+[AI应用] AI端侧: 1.60
 </t>
       </text>
     </comment>
@@ -16033,8 +16034,8 @@
       <text>
         <t xml:space="preserve">首板涨停 13:56:12 0
 PCB+AI算力+封装基板+央企
-主:AI大模型 次:精密电子
-[AI大模型] AI算力: 1.70
+主:算力半导体 次:精密电子
+[算力半导体] AI算力: 2.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -16143,8 +16144,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:18:06 0
 智能物流+业务量增长+收购
-主:无人经济 次:-
-[无人经济] 无人车: 1.50
+主:AI应用 次:无人经济
+[AI应用] AI物流: 1.60
+[无人经济] 无人车: 1.30
 </t>
       </text>
     </comment>
@@ -16236,9 +16238,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:12:06 4
 中报预增+AI服务器+液冷服务器+央国企
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 液冷服务器: 2.90
-[AI大模型] AI服务器: 1.50
+[AI应用] AI服务器: 1.60
 </t>
       </text>
     </comment>
@@ -16266,9 +16268,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:44:09 9
 半年度增长+AI服务器+GB200出货+机器人
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.00
-[AI大模型] AI服务器: 1.70
+[AI应用] AI服务器: 1.80
 </t>
       </text>
     </comment>
@@ -16276,8 +16278,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:38:17 1
 PCB+先进封装
-主:AI大模型 次:精密电子
-[AI大模型] AI复苏: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI复苏: 1.60
 [精密电子] PCB: 1.30
 </t>
       </text>
@@ -16287,7 +16289,7 @@
         <t xml:space="preserve">首板涨停 10:24:21 1
 创新药+临床进展+儿童药
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -16374,7 +16376,7 @@
         <t xml:space="preserve">首板涨停 11:08:03 0
 资产收购筹划+创新药+国企改革
 主:创新药 次:国企
-[创新药] 创新药: 2.00
+[创新药] 创新药: 2.10
 [国企] 国企改革: 1.50
 </t>
       </text>
@@ -16515,9 +16517,9 @@
       <text>
         <t xml:space="preserve">首板涨停 14:40:33 0
 半年度增长+AI服务器+GB200受益
-主:机器人 次:AI大模型
+主:机器人 次:AI应用
 [机器人] 机器人: 2.00
-[AI大模型] AI服务器: 1.70
+[AI应用] AI服务器: 1.80
 </t>
       </text>
     </comment>
@@ -16552,8 +16554,8 @@
       <text>
         <t xml:space="preserve">首板涨停 14:44:33 0
 PCB+AI服务器+中报预增
-主:AI大模型 次:精密电子
-[AI大模型] AI服务器: 1.50
+主:AI应用 次:精密电子
+[AI应用] AI服务器: 1.60
 [精密电子] PCB: 1.10
 </t>
       </text>
@@ -16689,7 +16691,7 @@
         <t xml:space="preserve">首板涨停 11:26:15 0
 创新药H1710+肝素业务+国际化产能
 主:创新药 次:-
-[创新药] 创新药H1710: 1.60
+[创新药] 创新药H1710: 1.70
 </t>
       </text>
     </comment>
@@ -16735,7 +16737,7 @@
         <t xml:space="preserve">首板涨停 13:30:14 1
 FDA认证+神经介入+中报预增
 主:创新药 次:预期改善
-[创新药] FDA突破性医疗器械认证: 1.80
+[创新药] FDA突破性医疗器械认证: 1.90
 [预期改善] 中报预增: 1.30
 </t>
       </text>
@@ -16763,9 +16765,9 @@
       <text>
         <t xml:space="preserve">首板涨停 13:33:55 0
 高速铜缆+藕芯结构+AI服务器
-主:算力半导体 次:AI大模型
+主:算力半导体 次:AI应用
 [算力半导体] 高速铜缆: 2.80
-[AI大模型] AI服务器: 1.90
+[AI应用] AI服务器: 2.00
 </t>
       </text>
     </comment>
@@ -17019,7 +17021,7 @@
 西部大开发+藏药龙头+创新药
 主:西部开发 次:创新药
 [西部开发] 西部大开发: 2.40
-[创新药] 创新药: 2.20
+[创新药] 创新药: 2.30
 </t>
       </text>
     </comment>
@@ -17038,7 +17040,7 @@
         <t xml:space="preserve">首板涨停 14:09:24 1
 创新药+CAR-T研究+医保销售
 主:创新药 次:-
-[创新药] 创新药: 1.80
+[创新药] 创新药: 1.90
 </t>
       </text>
     </comment>
@@ -17114,7 +17116,7 @@
         <t xml:space="preserve">首板涨停 14:48:55 0
 医美器械+创新药+海外增长
 主:创新药 次:-
-[创新药] 创新药: 1.60
+[创新药] 创新药: 1.70
 </t>
       </text>
     </comment>
@@ -17123,7 +17125,7 @@
         <t xml:space="preserve">首板涨停 14:51:31 0
 创新药+新药获批+小核酸战略
 主:创新药 次:-
-[创新药] 创新药: 3.00
+[创新药] 创新药: 3.10
 </t>
       </text>
     </comment>
@@ -18038,7 +18040,7 @@
     <row r="5">
       <c r="A5" s="22" t="inlineStr">
         <is>
-          <t>算力半导体(301)</t>
+          <t>算力半导体(316)</t>
         </is>
       </c>
       <c r="B5" s="23" t="inlineStr">
@@ -18312,7 +18314,7 @@
     <row r="7">
       <c r="A7" s="26" t="inlineStr">
         <is>
-          <t>AI大模型(205)</t>
+          <t>创新药(194)</t>
         </is>
       </c>
       <c r="B7" s="15" t="inlineStr">
@@ -18449,7 +18451,7 @@
     <row r="8">
       <c r="A8" s="27" t="inlineStr">
         <is>
-          <t>创新药(194)</t>
+          <t>AI应用(193)</t>
         </is>
       </c>
       <c r="B8" s="16" t="inlineStr">
@@ -19134,7 +19136,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>全球布局(95)</t>
+          <t>全球布局(93)</t>
         </is>
       </c>
       <c r="B13" s="25" t="inlineStr">
@@ -19404,7 +19406,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>无人经济(67)</t>
+          <t>电力(67)</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
@@ -19541,7 +19543,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>电力(67)</t>
+          <t>商业航天(67)</t>
         </is>
       </c>
       <c r="B16" s="14" t="inlineStr">
@@ -19657,7 +19659,7 @@
           <t>合力泰2</t>
         </is>
       </c>
-      <c r="AA16" s="21" t="inlineStr">
+      <c r="AA16" s="25" t="inlineStr">
         <is>
           <t>塞力医疗2</t>
         </is>
@@ -19666,7 +19668,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>商业航天(67)</t>
+          <t>无人经济(66)</t>
         </is>
       </c>
       <c r="B17" s="16" t="inlineStr">
@@ -20302,7 +20304,7 @@
           <t>科德教育</t>
         </is>
       </c>
-      <c r="AA21" s="21" t="inlineStr">
+      <c r="AA21" s="18" t="inlineStr">
         <is>
           <t>开普云</t>
         </is>
@@ -20577,7 +20579,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>大金融(37)</t>
+          <t>大金融(36)</t>
         </is>
       </c>
       <c r="B24" s="16" t="inlineStr">
@@ -20980,7 +20982,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>新消费(19)</t>
+          <t>新消费(20)</t>
         </is>
       </c>
       <c r="B27" s="16" t="inlineStr">
@@ -21672,7 +21674,7 @@
           <t>金钼股份</t>
         </is>
       </c>
-      <c r="F32" s="15" t="inlineStr">
+      <c r="F32" s="21" t="inlineStr">
         <is>
           <t>申通快递</t>
         </is>
@@ -22727,7 +22729,7 @@
           <t>东信和平2</t>
         </is>
       </c>
-      <c r="D40" s="21" t="inlineStr">
+      <c r="D40" s="25" t="inlineStr">
         <is>
           <t>塞力医疗</t>
         </is>
@@ -23238,7 +23240,7 @@
           <t>好上好</t>
         </is>
       </c>
-      <c r="AA43" s="21" t="inlineStr">
+      <c r="AA43" s="18" t="inlineStr">
         <is>
           <t>中旗新材</t>
         </is>
@@ -24042,7 +24044,7 @@
           <t>荣泰健康</t>
         </is>
       </c>
-      <c r="R50" s="21" t="inlineStr">
+      <c r="R50" s="18" t="inlineStr">
         <is>
           <t>寒武纪</t>
         </is>
@@ -24589,7 +24591,7 @@
           <t>京粮控股</t>
         </is>
       </c>
-      <c r="G56" s="21" t="inlineStr">
+      <c r="G56" s="18" t="inlineStr">
         <is>
           <t>深南电路</t>
         </is>
@@ -24972,7 +24974,7 @@
           <t>日出东方</t>
         </is>
       </c>
-      <c r="Z60" s="21" t="inlineStr">
+      <c r="Z60" s="18" t="inlineStr">
         <is>
           <t>海光信息</t>
         </is>
@@ -25417,7 +25419,7 @@
           <t>可立克</t>
         </is>
       </c>
-      <c r="S67" s="21" t="inlineStr">
+      <c r="S67" s="25" t="inlineStr">
         <is>
           <t>荣科科技</t>
         </is>
@@ -25504,7 +25506,7 @@
           <t>税友股份</t>
         </is>
       </c>
-      <c r="AA68" s="32" t="inlineStr">
+      <c r="AA68" s="21" t="inlineStr">
         <is>
           <t>神州信息</t>
         </is>
@@ -25556,7 +25558,7 @@
           <t>宏昌科技</t>
         </is>
       </c>
-      <c r="Z69" s="21" t="inlineStr">
+      <c r="Z69" s="25" t="inlineStr">
         <is>
           <t>塞力医疗</t>
         </is>
@@ -25670,7 +25672,7 @@
           <t>国光连锁</t>
         </is>
       </c>
-      <c r="Z71" s="21" t="inlineStr">
+      <c r="Z71" s="18" t="inlineStr">
         <is>
           <t>寒武纪</t>
         </is>
@@ -25692,12 +25694,12 @@
           <t>华伍股份</t>
         </is>
       </c>
-      <c r="E72" s="21" t="inlineStr">
+      <c r="E72" s="25" t="inlineStr">
         <is>
           <t>通策医疗</t>
         </is>
       </c>
-      <c r="Q72" s="21" t="inlineStr">
+      <c r="Q72" s="25" t="inlineStr">
         <is>
           <t>塞力医疗</t>
         </is>
@@ -25727,7 +25729,7 @@
           <t>苏州龙杰</t>
         </is>
       </c>
-      <c r="Z72" s="21" t="inlineStr">
+      <c r="Z72" s="14" t="inlineStr">
         <is>
           <t>成都华微</t>
         </is>
@@ -25784,7 +25786,7 @@
           <t>华海药业</t>
         </is>
       </c>
-      <c r="Z73" s="21" t="inlineStr">
+      <c r="Z73" s="18" t="inlineStr">
         <is>
           <t>浙大网新</t>
         </is>
@@ -26355,7 +26357,7 @@
           <t>银龙股份</t>
         </is>
       </c>
-      <c r="S86" s="21" t="inlineStr">
+      <c r="S86" s="18" t="inlineStr">
         <is>
           <t>深南电路</t>
         </is>
@@ -26412,7 +26414,7 @@
           <t>云南锗业</t>
         </is>
       </c>
-      <c r="X87" s="15" t="inlineStr">
+      <c r="X87" s="21" t="inlineStr">
         <is>
           <t>申通快递</t>
         </is>
@@ -35714,7 +35716,7 @@
         </is>
       </c>
       <c r="B4" s="39" t="n">
-        <v>301</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5">
@@ -35730,21 +35732,21 @@
     <row r="6">
       <c r="A6" s="44" t="inlineStr">
         <is>
-          <t>AI大模型</t>
+          <t>创新药</t>
         </is>
       </c>
       <c r="B6" s="39" t="n">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="45" t="inlineStr">
         <is>
-          <t>创新药</t>
+          <t>AI应用</t>
         </is>
       </c>
       <c r="B7" s="39" t="n">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8">
@@ -35802,7 +35804,7 @@
         </is>
       </c>
       <c r="B13" s="39" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14">
@@ -35818,7 +35820,7 @@
     <row r="15">
       <c r="A15" s="39" t="inlineStr">
         <is>
-          <t>无人经济</t>
+          <t>电力</t>
         </is>
       </c>
       <c r="B15" s="39" t="n">
@@ -35828,7 +35830,7 @@
     <row r="16">
       <c r="A16" s="39" t="inlineStr">
         <is>
-          <t>电力</t>
+          <t>商业航天</t>
         </is>
       </c>
       <c r="B16" s="39" t="n">
@@ -35838,11 +35840,11 @@
     <row r="17">
       <c r="A17" s="39" t="inlineStr">
         <is>
-          <t>商业航天</t>
+          <t>无人经济</t>
         </is>
       </c>
       <c r="B17" s="39" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -35912,7 +35914,7 @@
         </is>
       </c>
       <c r="B24" s="39" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
@@ -35942,7 +35944,7 @@
         </is>
       </c>
       <c r="B27" s="39" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">

</xml_diff>